<commit_message>
NMI, Interrupt, VIA fixes
</commit_message>
<xml_diff>
--- a/BitMagic.X16Emulator/state_object.xlsx
+++ b/BitMagic.X16Emulator/state_object.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Source\BitMagic\BitMagic.X16Emulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13265863-A441-4700-8A6F-F2E2AC0B513D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE2C78F-4B6A-422D-9346-BF9B1BA40333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30855" windowHeight="21600" xr2:uid="{E785A1AE-7179-42D9-8B33-8945211A7A0B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{E785A1AE-7179-42D9-8B33-8945211A7A0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="141">
   <si>
     <t>memory_ptr</t>
   </si>
@@ -340,27 +340,6 @@
     <t>via_t2counter_value</t>
   </si>
   <si>
-    <t>via_interrupt_timer1</t>
-  </si>
-  <si>
-    <t>via_interrupt_timer2</t>
-  </si>
-  <si>
-    <t>via_interrupt_cb1</t>
-  </si>
-  <si>
-    <t>via_interrupt_cb2</t>
-  </si>
-  <si>
-    <t>via_interrupt_shiftregister</t>
-  </si>
-  <si>
-    <t>via_interrupt_ca1</t>
-  </si>
-  <si>
-    <t>via_interrupt_ca2</t>
-  </si>
-  <si>
     <t>via_timer1_continuous</t>
   </si>
   <si>
@@ -473,6 +452,12 @@
   </si>
   <si>
     <t>Rendering</t>
+  </si>
+  <si>
+    <t>register_a_indata</t>
+  </si>
+  <si>
+    <t>register_a_outdata</t>
   </si>
 </sst>
 </file>
@@ -836,8 +821,8 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A134" sqref="A134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,32 +839,32 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -887,7 +872,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -901,16 +886,16 @@
         <v>8</v>
       </c>
       <c r="F2">
-        <f>LEN(A2)</f>
+        <f t="shared" ref="F2:F49" si="0">LEN(A2)</f>
         <v>10</v>
       </c>
       <c r="G2" t="str">
-        <f>IF(B2="", "", IF(E2/D2&lt;&gt;FLOOR(E2/D2,1),"ERROR",""))</f>
+        <f t="shared" ref="G2:G49" si="1">IF(B2="", "", IF(E2/D2&lt;&gt;FLOOR(E2/D2,1),"ERROR",""))</f>
         <v/>
       </c>
       <c r="I2" t="str">
-        <f>IF(B2="",IF(A2="","","; " &amp;A2),A2&amp;REPT(" ",MAX(F:F)-F2+1)&amp;B2&amp;" ? "&amp;IF(H2&lt;&gt;"","; "&amp;H2,""))</f>
-        <v xml:space="preserve">memory_ptr                  qword ? </v>
+        <f t="shared" ref="I2:I33" si="2">IF(B2="",IF(A2="","","; " &amp;A2),A2&amp;REPT(" ",MAX(F:F)-F2+1)&amp;B2&amp;" ? "&amp;IF(H2&lt;&gt;"","; "&amp;H2,""))</f>
+        <v xml:space="preserve">memory_ptr             qword ? </v>
       </c>
       <c r="J2" t="str">
         <f>IF(B2&lt;&gt;"", "        public "&amp;VLOOKUP(B2,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A2)&amp;" = "&amp;C2&amp;";"&amp;IF(H2="",""," // "&amp;H2), IF(A2&lt;&gt;"","        // "&amp;A2,""))</f>
@@ -922,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -936,16 +921,16 @@
         <v>16</v>
       </c>
       <c r="F3">
-        <f>LEN(A3)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G3" t="str">
-        <f>IF(B3="", "", IF(E3/D3&lt;&gt;FLOOR(E3/D3,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I3" t="str">
-        <f>IF(B3="",IF(A3="","","; " &amp;A3),A3&amp;REPT(" ",MAX(F:F)-F3+1)&amp;B3&amp;" ? "&amp;IF(H3&lt;&gt;"","; "&amp;H3,""))</f>
-        <v xml:space="preserve">rom_ptr                     qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">rom_ptr                qword ? </v>
       </c>
       <c r="J3" t="str">
         <f>IF(B3&lt;&gt;"", "        public "&amp;VLOOKUP(B3,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A3)&amp;" = "&amp;C3&amp;";"&amp;IF(H3="",""," // "&amp;H3), IF(A3&lt;&gt;"","        // "&amp;A3,""))</f>
@@ -957,7 +942,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -971,16 +956,16 @@
         <v>24</v>
       </c>
       <c r="F4">
-        <f>LEN(A4)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G4" t="str">
-        <f>IF(B4="", "", IF(E4/D4&lt;&gt;FLOOR(E4/D4,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I4" t="str">
-        <f>IF(B4="",IF(A4="","","; " &amp;A4),A4&amp;REPT(" ",MAX(F:F)-F4+1)&amp;B4&amp;" ? "&amp;IF(H4&lt;&gt;"","; "&amp;H4,""))</f>
-        <v xml:space="preserve">rambank_ptr                 qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">rambank_ptr            qword ? </v>
       </c>
       <c r="J4" t="str">
         <f>IF(B4&lt;&gt;"", "        public "&amp;VLOOKUP(B4,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A4)&amp;" = "&amp;C4&amp;";"&amp;IF(H4="",""," // "&amp;H4), IF(A4&lt;&gt;"","        // "&amp;A4,""))</f>
@@ -992,7 +977,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1006,16 +991,16 @@
         <v>32</v>
       </c>
       <c r="F5">
-        <f>LEN(A5)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G5" t="str">
-        <f>IF(B5="", "", IF(E5/D5&lt;&gt;FLOOR(E5/D5,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I5" t="str">
-        <f>IF(B5="",IF(A5="","","; " &amp;A5),A5&amp;REPT(" ",MAX(F:F)-F5+1)&amp;B5&amp;" ? "&amp;IF(H5&lt;&gt;"","; "&amp;H5,""))</f>
-        <v xml:space="preserve">display_ptr                 qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">display_ptr            qword ? </v>
       </c>
       <c r="J5" t="str">
         <f>IF(B5&lt;&gt;"", "        public "&amp;VLOOKUP(B5,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A5)&amp;" = "&amp;C5&amp;";"&amp;IF(H5="",""," // "&amp;H5), IF(A5&lt;&gt;"","        // "&amp;A5,""))</f>
@@ -1027,7 +1012,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1041,16 +1026,16 @@
         <v>40</v>
       </c>
       <c r="F6">
-        <f>LEN(A6)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="G6" t="str">
-        <f>IF(B6="", "", IF(E6/D6&lt;&gt;FLOOR(E6/D6,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I6" t="str">
-        <f>IF(B6="",IF(A6="","","; " &amp;A6),A6&amp;REPT(" ",MAX(F:F)-F6+1)&amp;B6&amp;" ? "&amp;IF(H6&lt;&gt;"","; "&amp;H6,""))</f>
-        <v xml:space="preserve">display_buffer_ptr          qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">display_buffer_ptr     qword ? </v>
       </c>
       <c r="J6" t="str">
         <f>IF(B6&lt;&gt;"", "        public "&amp;VLOOKUP(B6,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A6)&amp;" = "&amp;C6&amp;";"&amp;IF(H6="",""," // "&amp;H6), IF(A6&lt;&gt;"","        // "&amp;A6,""))</f>
@@ -1062,7 +1047,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1076,16 +1061,16 @@
         <v>48</v>
       </c>
       <c r="F7">
-        <f>LEN(A7)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G7" t="str">
-        <f>IF(B7="", "", IF(E7/D7&lt;&gt;FLOOR(E7/D7,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I7" t="str">
-        <f>IF(B7="",IF(A7="","","; " &amp;A7),A7&amp;REPT(" ",MAX(F:F)-F7+1)&amp;B7&amp;" ? "&amp;IF(H7&lt;&gt;"","; "&amp;H7,""))</f>
-        <v xml:space="preserve">history_ptr                 qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">history_ptr            qword ? </v>
       </c>
       <c r="J7" t="str">
         <f>IF(B7&lt;&gt;"", "        public "&amp;VLOOKUP(B7,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A7)&amp;" = "&amp;C7&amp;";"&amp;IF(H7="",""," // "&amp;H7), IF(A7&lt;&gt;"","        // "&amp;A7,""))</f>
@@ -1102,15 +1087,15 @@
         <v>48</v>
       </c>
       <c r="F8">
-        <f>LEN(A8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G8" t="str">
-        <f>IF(B8="", "", IF(E8/D8&lt;&gt;FLOOR(E8/D8,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I8" t="str">
-        <f>IF(B8="",IF(A8="","","; " &amp;A8),A8&amp;REPT(" ",MAX(F:F)-F8+1)&amp;B8&amp;" ? "&amp;IF(H8&lt;&gt;"","; "&amp;H8,""))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J8" t="str">
@@ -1120,7 +1105,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D9" t="str">
         <f>IF(B9="", "", VLOOKUP(B9,Sheet2!A:B,2,FALSE))</f>
@@ -1131,15 +1116,15 @@
         <v>48</v>
       </c>
       <c r="F9">
-        <f>LEN(A9)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G9" t="str">
-        <f>IF(B9="", "", IF(E9/D9&lt;&gt;FLOOR(E9/D9,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I9" t="str">
-        <f>IF(B9="",IF(A9="","","; " &amp;A9),A9&amp;REPT(" ",MAX(F:F)-F9+1)&amp;B9&amp;" ? "&amp;IF(H9&lt;&gt;"","; "&amp;H9,""))</f>
+        <f t="shared" si="2"/>
         <v>; Vera</v>
       </c>
       <c r="J9" t="str">
@@ -1152,7 +1137,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1166,16 +1151,16 @@
         <v>56</v>
       </c>
       <c r="F10">
-        <f>LEN(A10)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G10" t="str">
-        <f>IF(B10="", "", IF(E10/D10&lt;&gt;FLOOR(E10/D10,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I10" t="str">
-        <f>IF(B10="",IF(A10="","","; " &amp;A10),A10&amp;REPT(" ",MAX(F:F)-F10+1)&amp;B10&amp;" ? "&amp;IF(H10&lt;&gt;"","; "&amp;H10,""))</f>
-        <v xml:space="preserve">vram_ptr                    qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">vram_ptr               qword ? </v>
       </c>
       <c r="J10" t="str">
         <f>IF(B10&lt;&gt;"", "        public "&amp;VLOOKUP(B10,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A10)&amp;" = "&amp;C10&amp;";"&amp;IF(H10="",""," // "&amp;H10), IF(A10&lt;&gt;"","        // "&amp;A10,""))</f>
@@ -1187,7 +1172,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1201,16 +1186,16 @@
         <v>64</v>
       </c>
       <c r="F11">
-        <f>LEN(A11)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G11" t="str">
-        <f>IF(B11="", "", IF(E11/D11&lt;&gt;FLOOR(E11/D11,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I11" t="str">
-        <f>IF(B11="",IF(A11="","","; " &amp;A11),A11&amp;REPT(" ",MAX(F:F)-F11+1)&amp;B11&amp;" ? "&amp;IF(H11&lt;&gt;"","; "&amp;H11,""))</f>
-        <v xml:space="preserve">palette_ptr                 qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">palette_ptr            qword ? </v>
       </c>
       <c r="J11" t="str">
         <f>IF(B11&lt;&gt;"", "        public "&amp;VLOOKUP(B11,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A11)&amp;" = "&amp;C11&amp;";"&amp;IF(H11="",""," // "&amp;H11), IF(A11&lt;&gt;"","        // "&amp;A11,""))</f>
@@ -1227,15 +1212,15 @@
         <v>64</v>
       </c>
       <c r="F12">
-        <f>LEN(A12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G12" t="str">
-        <f>IF(B12="", "", IF(E12/D12&lt;&gt;FLOOR(E12/D12,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I12" t="str">
-        <f>IF(B12="",IF(A12="","","; " &amp;A12),A12&amp;REPT(" ",MAX(F:F)-F12+1)&amp;B12&amp;" ? "&amp;IF(H12&lt;&gt;"","; "&amp;H12,""))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J12" t="str">
@@ -1248,7 +1233,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1262,16 +1247,16 @@
         <v>72</v>
       </c>
       <c r="F13">
-        <f>LEN(A13)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="G13" t="str">
-        <f>IF(B13="", "", IF(E13/D13&lt;&gt;FLOOR(E13/D13,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I13" t="str">
-        <f>IF(B13="",IF(A13="","","; " &amp;A13),A13&amp;REPT(" ",MAX(F:F)-F13+1)&amp;B13&amp;" ? "&amp;IF(H13&lt;&gt;"","; "&amp;H13,""))</f>
-        <v xml:space="preserve">data0_address               qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">data0_address          qword ? </v>
       </c>
       <c r="J13" t="str">
         <f>IF(B13&lt;&gt;"", "        public "&amp;VLOOKUP(B13,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A13)&amp;" = "&amp;C13&amp;";"&amp;IF(H13="",""," // "&amp;H13), IF(A13&lt;&gt;"","        // "&amp;A13,""))</f>
@@ -1283,7 +1268,7 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1297,16 +1282,16 @@
         <v>80</v>
       </c>
       <c r="F14">
-        <f>LEN(A14)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="G14" t="str">
-        <f>IF(B14="", "", IF(E14/D14&lt;&gt;FLOOR(E14/D14,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I14" t="str">
-        <f>IF(B14="",IF(A14="","","; " &amp;A14),A14&amp;REPT(" ",MAX(F:F)-F14+1)&amp;B14&amp;" ? "&amp;IF(H14&lt;&gt;"","; "&amp;H14,""))</f>
-        <v xml:space="preserve">data1_address               qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">data1_address          qword ? </v>
       </c>
       <c r="J14" t="str">
         <f>IF(B14&lt;&gt;"", "        public "&amp;VLOOKUP(B14,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A14)&amp;" = "&amp;C14&amp;";"&amp;IF(H14="",""," // "&amp;H14), IF(A14&lt;&gt;"","        // "&amp;A14,""))</f>
@@ -1318,7 +1303,7 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1332,16 +1317,16 @@
         <v>88</v>
       </c>
       <c r="F15">
-        <f>LEN(A15)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G15" t="str">
-        <f>IF(B15="", "", IF(E15/D15&lt;&gt;FLOOR(E15/D15,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I15" t="str">
-        <f>IF(B15="",IF(A15="","","; " &amp;A15),A15&amp;REPT(" ",MAX(F:F)-F15+1)&amp;B15&amp;" ? "&amp;IF(H15&lt;&gt;"","; "&amp;H15,""))</f>
-        <v xml:space="preserve">data0_step                  qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">data0_step             qword ? </v>
       </c>
       <c r="J15" t="str">
         <f>IF(B15&lt;&gt;"", "        public "&amp;VLOOKUP(B15,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A15)&amp;" = "&amp;C15&amp;";"&amp;IF(H15="",""," // "&amp;H15), IF(A15&lt;&gt;"","        // "&amp;A15,""))</f>
@@ -1353,7 +1338,7 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1367,16 +1352,16 @@
         <v>96</v>
       </c>
       <c r="F16">
-        <f>LEN(A16)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G16" t="str">
-        <f>IF(B16="", "", IF(E16/D16&lt;&gt;FLOOR(E16/D16,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I16" t="str">
-        <f>IF(B16="",IF(A16="","","; " &amp;A16),A16&amp;REPT(" ",MAX(F:F)-F16+1)&amp;B16&amp;" ? "&amp;IF(H16&lt;&gt;"","; "&amp;H16,""))</f>
-        <v xml:space="preserve">data1_step                  qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">data1_step             qword ? </v>
       </c>
       <c r="J16" t="str">
         <f>IF(B16&lt;&gt;"", "        public "&amp;VLOOKUP(B16,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A16)&amp;" = "&amp;C16&amp;";"&amp;IF(H16="",""," // "&amp;H16), IF(A16&lt;&gt;"","        // "&amp;A16,""))</f>
@@ -1393,15 +1378,15 @@
         <v>96</v>
       </c>
       <c r="F17">
-        <f>LEN(A17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G17" t="str">
-        <f>IF(B17="", "", IF(E17/D17&lt;&gt;FLOOR(E17/D17,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I17" t="str">
-        <f>IF(B17="",IF(A17="","","; " &amp;A17),A17&amp;REPT(" ",MAX(F:F)-F17+1)&amp;B17&amp;" ? "&amp;IF(H17&lt;&gt;"","; "&amp;H17,""))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J17" t="str">
@@ -1414,7 +1399,7 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1428,16 +1413,16 @@
         <v>104</v>
       </c>
       <c r="F18">
-        <f>LEN(A18)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="G18" t="str">
-        <f>IF(B18="", "", IF(E18/D18&lt;&gt;FLOOR(E18/D18,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I18" t="str">
-        <f>IF(B18="",IF(A18="","","; " &amp;A18),A18&amp;REPT(" ",MAX(F:F)-F18+1)&amp;B18&amp;" ? "&amp;IF(H18&lt;&gt;"","; "&amp;H18,""))</f>
-        <v xml:space="preserve">clock_previous              qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">clock_previous         qword ? </v>
       </c>
       <c r="J18" t="str">
         <f>IF(B18&lt;&gt;"", "        public "&amp;VLOOKUP(B18,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A18)&amp;" = "&amp;C18&amp;";"&amp;IF(H18="",""," // "&amp;H18), IF(A18&lt;&gt;"","        // "&amp;A18,""))</f>
@@ -1449,7 +1434,7 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1463,16 +1448,16 @@
         <v>112</v>
       </c>
       <c r="F19">
-        <f>LEN(A19)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G19" t="str">
-        <f>IF(B19="", "", IF(E19/D19&lt;&gt;FLOOR(E19/D19,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I19" t="str">
-        <f>IF(B19="",IF(A19="","","; " &amp;A19),A19&amp;REPT(" ",MAX(F:F)-F19+1)&amp;B19&amp;" ? "&amp;IF(H19&lt;&gt;"","; "&amp;H19,""))</f>
-        <v xml:space="preserve">clock                       qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">clock                  qword ? </v>
       </c>
       <c r="J19" t="str">
         <f>IF(B19&lt;&gt;"", "        public "&amp;VLOOKUP(B19,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A19)&amp;" = "&amp;C19&amp;";"&amp;IF(H19="",""," // "&amp;H19), IF(A19&lt;&gt;"","        // "&amp;A19,""))</f>
@@ -1484,7 +1469,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1498,16 +1483,16 @@
         <v>120</v>
       </c>
       <c r="F20">
-        <f>LEN(A20)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G20" t="str">
-        <f>IF(B20="", "", IF(E20/D20&lt;&gt;FLOOR(E20/D20,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I20" t="str">
-        <f>IF(B20="",IF(A20="","","; " &amp;A20),A20&amp;REPT(" ",MAX(F:F)-F20+1)&amp;B20&amp;" ? "&amp;IF(H20&lt;&gt;"","; "&amp;H20,""))</f>
-        <v xml:space="preserve">vera_clock                  qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">vera_clock             qword ? </v>
       </c>
       <c r="J20" t="str">
         <f>IF(B20&lt;&gt;"", "        public "&amp;VLOOKUP(B20,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A20)&amp;" = "&amp;C20&amp;";"&amp;IF(H20="",""," // "&amp;H20), IF(A20&lt;&gt;"","        // "&amp;A20,""))</f>
@@ -1524,15 +1509,15 @@
         <v>120</v>
       </c>
       <c r="F21">
-        <f>LEN(A21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G21" t="str">
-        <f>IF(B21="", "", IF(E21/D21&lt;&gt;FLOOR(E21/D21,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I21" t="str">
-        <f>IF(B21="",IF(A21="","","; " &amp;A21),A21&amp;REPT(" ",MAX(F:F)-F21+1)&amp;B21&amp;" ? "&amp;IF(H21&lt;&gt;"","; "&amp;H21,""))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J21" t="str">
@@ -1545,7 +1530,7 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1559,16 +1544,16 @@
         <v>128</v>
       </c>
       <c r="F22">
-        <f>LEN(A22)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G22" t="str">
-        <f>IF(B22="", "", IF(E22/D22&lt;&gt;FLOOR(E22/D22,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I22" t="str">
-        <f>IF(B22="",IF(A22="","","; " &amp;A22),A22&amp;REPT(" ",MAX(F:F)-F22+1)&amp;B22&amp;" ? "&amp;IF(H22&lt;&gt;"","; "&amp;H22,""))</f>
-        <v xml:space="preserve">history_pos                 qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">history_pos            qword ? </v>
       </c>
       <c r="J22" t="str">
         <f>IF(B22&lt;&gt;"", "        public "&amp;VLOOKUP(B22,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A22)&amp;" = "&amp;C22&amp;";"&amp;IF(H22="",""," // "&amp;H22), IF(A22&lt;&gt;"","        // "&amp;A22,""))</f>
@@ -1585,15 +1570,15 @@
         <v>128</v>
       </c>
       <c r="F23">
-        <f>LEN(A23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G23" t="str">
-        <f>IF(B23="", "", IF(E23/D23&lt;&gt;FLOOR(E23/D23,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I23" t="str">
-        <f>IF(B23="",IF(A23="","","; " &amp;A23),A23&amp;REPT(" ",MAX(F:F)-F23+1)&amp;B23&amp;" ? "&amp;IF(H23&lt;&gt;"","; "&amp;H23,""))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J23" t="str">
@@ -1606,7 +1591,7 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1620,16 +1605,16 @@
         <v>136</v>
       </c>
       <c r="F24">
-        <f>LEN(A24)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G24" t="str">
-        <f>IF(B24="", "", IF(E24/D24&lt;&gt;FLOOR(E24/D24,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I24" t="str">
-        <f>IF(B24="",IF(A24="","","; " &amp;A24),A24&amp;REPT(" ",MAX(F:F)-F24+1)&amp;B24&amp;" ? "&amp;IF(H24&lt;&gt;"","; "&amp;H24,""))</f>
-        <v xml:space="preserve">layer0_jmp                  qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">layer0_jmp             qword ? </v>
       </c>
       <c r="J24" t="str">
         <f>IF(B24&lt;&gt;"", "        public "&amp;VLOOKUP(B24,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A24)&amp;" = "&amp;C24&amp;";"&amp;IF(H24="",""," // "&amp;H24), IF(A24&lt;&gt;"","        // "&amp;A24,""))</f>
@@ -1641,7 +1626,7 @@
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1655,16 +1640,16 @@
         <v>144</v>
       </c>
       <c r="F25">
-        <f>LEN(A25)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G25" t="str">
-        <f>IF(B25="", "", IF(E25/D25&lt;&gt;FLOOR(E25/D25,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I25" t="str">
-        <f>IF(B25="",IF(A25="","","; " &amp;A25),A25&amp;REPT(" ",MAX(F:F)-F25+1)&amp;B25&amp;" ? "&amp;IF(H25&lt;&gt;"","; "&amp;H25,""))</f>
-        <v xml:space="preserve">layer0_rtn                  qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">layer0_rtn             qword ? </v>
       </c>
       <c r="J25" t="str">
         <f>IF(B25&lt;&gt;"", "        public "&amp;VLOOKUP(B25,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A25)&amp;" = "&amp;C25&amp;";"&amp;IF(H25="",""," // "&amp;H25), IF(A25&lt;&gt;"","        // "&amp;A25,""))</f>
@@ -1676,7 +1661,7 @@
         <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1690,16 +1675,16 @@
         <v>152</v>
       </c>
       <c r="F26">
-        <f>LEN(A26)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G26" t="str">
-        <f>IF(B26="", "", IF(E26/D26&lt;&gt;FLOOR(E26/D26,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I26" t="str">
-        <f>IF(B26="",IF(A26="","","; " &amp;A26),A26&amp;REPT(" ",MAX(F:F)-F26+1)&amp;B26&amp;" ? "&amp;IF(H26&lt;&gt;"","; "&amp;H26,""))</f>
-        <v xml:space="preserve">layer1_jmp                  qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">layer1_jmp             qword ? </v>
       </c>
       <c r="J26" t="str">
         <f>IF(B26&lt;&gt;"", "        public "&amp;VLOOKUP(B26,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A26)&amp;" = "&amp;C26&amp;";"&amp;IF(H26="",""," // "&amp;H26), IF(A26&lt;&gt;"","        // "&amp;A26,""))</f>
@@ -1711,7 +1696,7 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1725,16 +1710,16 @@
         <v>160</v>
       </c>
       <c r="F27">
-        <f>LEN(A27)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G27" t="str">
-        <f>IF(B27="", "", IF(E27/D27&lt;&gt;FLOOR(E27/D27,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I27" t="str">
-        <f>IF(B27="",IF(A27="","","; " &amp;A27),A27&amp;REPT(" ",MAX(F:F)-F27+1)&amp;B27&amp;" ? "&amp;IF(H27&lt;&gt;"","; "&amp;H27,""))</f>
-        <v xml:space="preserve">layer1_rtn                  qword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">layer1_rtn             qword ? </v>
       </c>
       <c r="J27" t="str">
         <f>IF(B27&lt;&gt;"", "        public "&amp;VLOOKUP(B27,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A27)&amp;" = "&amp;C27&amp;";"&amp;IF(H27="",""," // "&amp;H27), IF(A27&lt;&gt;"","        // "&amp;A27,""))</f>
@@ -1751,15 +1736,15 @@
         <v>160</v>
       </c>
       <c r="F28">
-        <f>LEN(A28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G28" t="str">
-        <f>IF(B28="", "", IF(E28/D28&lt;&gt;FLOOR(E28/D28,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I28" t="str">
-        <f>IF(B28="",IF(A28="","","; " &amp;A28),A28&amp;REPT(" ",MAX(F:F)-F28+1)&amp;B28&amp;" ? "&amp;IF(H28&lt;&gt;"","; "&amp;H28,""))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J28" t="str">
@@ -1772,10 +1757,10 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C29" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D29">
         <f>IF(B29="", "", VLOOKUP(B29,Sheet2!A:B,2,FALSE))</f>
@@ -1786,16 +1771,16 @@
         <v>164</v>
       </c>
       <c r="F29">
-        <f>LEN(A29)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G29" t="str">
-        <f>IF(B29="", "", IF(E29/D29&lt;&gt;FLOOR(E29/D29,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I29" t="str">
-        <f>IF(B29="",IF(A29="","","; " &amp;A29),A29&amp;REPT(" ",MAX(F:F)-F29+1)&amp;B29&amp;" ? "&amp;IF(H29&lt;&gt;"","; "&amp;H29,""))</f>
-        <v xml:space="preserve">dc_hscale                   dword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">dc_hscale              dword ? </v>
       </c>
       <c r="J29" t="str">
         <f>IF(B29&lt;&gt;"", "        public "&amp;VLOOKUP(B29,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A29)&amp;" = "&amp;C29&amp;";"&amp;IF(H29="",""," // "&amp;H29), IF(A29&lt;&gt;"","        // "&amp;A29,""))</f>
@@ -1807,10 +1792,10 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C30" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D30">
         <f>IF(B30="", "", VLOOKUP(B30,Sheet2!A:B,2,FALSE))</f>
@@ -1821,16 +1806,16 @@
         <v>168</v>
       </c>
       <c r="F30">
-        <f>LEN(A30)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G30" t="str">
-        <f>IF(B30="", "", IF(E30/D30&lt;&gt;FLOOR(E30/D30,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I30" t="str">
-        <f>IF(B30="",IF(A30="","","; " &amp;A30),A30&amp;REPT(" ",MAX(F:F)-F30+1)&amp;B30&amp;" ? "&amp;IF(H30&lt;&gt;"","; "&amp;H30,""))</f>
-        <v xml:space="preserve">dc_vscale                   dword ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">dc_vscale              dword ? </v>
       </c>
       <c r="J30" t="str">
         <f>IF(B30&lt;&gt;"", "        public "&amp;VLOOKUP(B30,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A30)&amp;" = "&amp;C30&amp;";"&amp;IF(H30="",""," // "&amp;H30), IF(A30&lt;&gt;"","        // "&amp;A30,""))</f>
@@ -1847,15 +1832,15 @@
         <v>168</v>
       </c>
       <c r="F31">
-        <f>LEN(A31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G31" t="str">
-        <f>IF(B31="", "", IF(E31/D31&lt;&gt;FLOOR(E31/D31,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I31" t="str">
-        <f>IF(B31="",IF(A31="","","; " &amp;A31),A31&amp;REPT(" ",MAX(F:F)-F31+1)&amp;B31&amp;" ? "&amp;IF(H31&lt;&gt;"","; "&amp;H31,""))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J31" t="str">
@@ -1868,7 +1853,7 @@
         <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1882,16 +1867,16 @@
         <v>170</v>
       </c>
       <c r="F32">
-        <f>LEN(A32)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G32" t="str">
-        <f>IF(B32="", "", IF(E32/D32&lt;&gt;FLOOR(E32/D32,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I32" t="str">
-        <f>IF(B32="",IF(A32="","","; " &amp;A32),A32&amp;REPT(" ",MAX(F:F)-F32+1)&amp;B32&amp;" ? "&amp;IF(H32&lt;&gt;"","; "&amp;H32,""))</f>
-        <v xml:space="preserve">register_pc                 word ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">register_pc            word ? </v>
       </c>
       <c r="J32" t="str">
         <f>IF(B32&lt;&gt;"", "        public "&amp;VLOOKUP(B32,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A32)&amp;" = "&amp;C32&amp;";"&amp;IF(H32="",""," // "&amp;H32), IF(A32&lt;&gt;"","        // "&amp;A32,""))</f>
@@ -1903,10 +1888,10 @@
         <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C33" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D33">
         <f>IF(B33="", "", VLOOKUP(B33,Sheet2!A:B,2,FALSE))</f>
@@ -1917,16 +1902,16 @@
         <v>172</v>
       </c>
       <c r="F33">
-        <f>LEN(A33)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="G33" t="str">
-        <f>IF(B33="", "", IF(E33/D33&lt;&gt;FLOOR(E33/D33,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I33" t="str">
-        <f>IF(B33="",IF(A33="","","; " &amp;A33),A33&amp;REPT(" ",MAX(F:F)-F33+1)&amp;B33&amp;" ? "&amp;IF(H33&lt;&gt;"","; "&amp;H33,""))</f>
-        <v xml:space="preserve">stackpointer                word ? </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">stackpointer           word ? </v>
       </c>
       <c r="J33" t="str">
         <f>IF(B33&lt;&gt;"", "        public "&amp;VLOOKUP(B33,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A33)&amp;" = "&amp;C33&amp;";"&amp;IF(H33="",""," // "&amp;H33), IF(A33&lt;&gt;"","        // "&amp;A33,""))</f>
@@ -1943,15 +1928,15 @@
         <v>172</v>
       </c>
       <c r="F34">
-        <f>LEN(A34)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G34" t="str">
-        <f>IF(B34="", "", IF(E34/D34&lt;&gt;FLOOR(E34/D34,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I34" t="str">
-        <f>IF(B34="",IF(A34="","","; " &amp;A34),A34&amp;REPT(" ",MAX(F:F)-F34+1)&amp;B34&amp;" ? "&amp;IF(H34&lt;&gt;"","; "&amp;H34,""))</f>
+        <f t="shared" ref="I34:I65" si="3">IF(B34="",IF(A34="","","; " &amp;A34),A34&amp;REPT(" ",MAX(F:F)-F34+1)&amp;B34&amp;" ? "&amp;IF(H34&lt;&gt;"","; "&amp;H34,""))</f>
         <v/>
       </c>
       <c r="J34" t="str">
@@ -1964,7 +1949,7 @@
         <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1978,16 +1963,16 @@
         <v>173</v>
       </c>
       <c r="F35">
-        <f>LEN(A35)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G35" t="str">
-        <f>IF(B35="", "", IF(E35/D35&lt;&gt;FLOOR(E35/D35,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I35" t="str">
-        <f>IF(B35="",IF(A35="","","; " &amp;A35),A35&amp;REPT(" ",MAX(F:F)-F35+1)&amp;B35&amp;" ? "&amp;IF(H35&lt;&gt;"","; "&amp;H35,""))</f>
-        <v xml:space="preserve">register_a                  byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">register_a             byte ? </v>
       </c>
       <c r="J35" t="str">
         <f>IF(B35&lt;&gt;"", "        public "&amp;VLOOKUP(B35,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A35)&amp;" = "&amp;C35&amp;";"&amp;IF(H35="",""," // "&amp;H35), IF(A35&lt;&gt;"","        // "&amp;A35,""))</f>
@@ -1999,7 +1984,7 @@
         <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -2013,16 +1998,16 @@
         <v>174</v>
       </c>
       <c r="F36">
-        <f>LEN(A36)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G36" t="str">
-        <f>IF(B36="", "", IF(E36/D36&lt;&gt;FLOOR(E36/D36,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I36" t="str">
-        <f>IF(B36="",IF(A36="","","; " &amp;A36),A36&amp;REPT(" ",MAX(F:F)-F36+1)&amp;B36&amp;" ? "&amp;IF(H36&lt;&gt;"","; "&amp;H36,""))</f>
-        <v xml:space="preserve">register_x                  byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">register_x             byte ? </v>
       </c>
       <c r="J36" t="str">
         <f>IF(B36&lt;&gt;"", "        public "&amp;VLOOKUP(B36,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A36)&amp;" = "&amp;C36&amp;";"&amp;IF(H36="",""," // "&amp;H36), IF(A36&lt;&gt;"","        // "&amp;A36,""))</f>
@@ -2034,7 +2019,7 @@
         <v>26</v>
       </c>
       <c r="B37" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2048,16 +2033,16 @@
         <v>175</v>
       </c>
       <c r="F37">
-        <f>LEN(A37)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G37" t="str">
-        <f>IF(B37="", "", IF(E37/D37&lt;&gt;FLOOR(E37/D37,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I37" t="str">
-        <f>IF(B37="",IF(A37="","","; " &amp;A37),A37&amp;REPT(" ",MAX(F:F)-F37+1)&amp;B37&amp;" ? "&amp;IF(H37&lt;&gt;"","; "&amp;H37,""))</f>
-        <v xml:space="preserve">register_y                  byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">register_y             byte ? </v>
       </c>
       <c r="J37" t="str">
         <f>IF(B37&lt;&gt;"", "        public "&amp;VLOOKUP(B37,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A37)&amp;" = "&amp;C37&amp;";"&amp;IF(H37="",""," // "&amp;H37), IF(A37&lt;&gt;"","        // "&amp;A37,""))</f>
@@ -2074,15 +2059,15 @@
         <v>175</v>
       </c>
       <c r="F38">
-        <f>LEN(A38)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G38" t="str">
-        <f>IF(B38="", "", IF(E38/D38&lt;&gt;FLOOR(E38/D38,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I38" t="str">
-        <f>IF(B38="",IF(A38="","","; " &amp;A38),A38&amp;REPT(" ",MAX(F:F)-F38+1)&amp;B38&amp;" ? "&amp;IF(H38&lt;&gt;"","; "&amp;H38,""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J38" t="str">
@@ -2095,7 +2080,7 @@
         <v>27</v>
       </c>
       <c r="B39" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2109,16 +2094,16 @@
         <v>176</v>
       </c>
       <c r="F39">
-        <f>LEN(A39)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="G39" t="str">
-        <f>IF(B39="", "", IF(E39/D39&lt;&gt;FLOOR(E39/D39,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I39" t="str">
-        <f>IF(B39="",IF(A39="","","; " &amp;A39),A39&amp;REPT(" ",MAX(F:F)-F39+1)&amp;B39&amp;" ? "&amp;IF(H39&lt;&gt;"","; "&amp;H39,""))</f>
-        <v xml:space="preserve">flags_decimal               byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">flags_decimal          byte ? </v>
       </c>
       <c r="J39" t="str">
         <f>IF(B39&lt;&gt;"", "        public "&amp;VLOOKUP(B39,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A39)&amp;" = "&amp;C39&amp;";"&amp;IF(H39="",""," // "&amp;H39), IF(A39&lt;&gt;"","        // "&amp;A39,""))</f>
@@ -2130,7 +2115,7 @@
         <v>28</v>
       </c>
       <c r="B40" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2144,16 +2129,16 @@
         <v>177</v>
       </c>
       <c r="F40">
-        <f>LEN(A40)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G40" t="str">
-        <f>IF(B40="", "", IF(E40/D40&lt;&gt;FLOOR(E40/D40,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I40" t="str">
-        <f>IF(B40="",IF(A40="","","; " &amp;A40),A40&amp;REPT(" ",MAX(F:F)-F40+1)&amp;B40&amp;" ? "&amp;IF(H40&lt;&gt;"","; "&amp;H40,""))</f>
-        <v xml:space="preserve">flags_break                 byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">flags_break            byte ? </v>
       </c>
       <c r="J40" t="str">
         <f>IF(B40&lt;&gt;"", "        public "&amp;VLOOKUP(B40,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A40)&amp;" = "&amp;C40&amp;";"&amp;IF(H40="",""," // "&amp;H40), IF(A40&lt;&gt;"","        // "&amp;A40,""))</f>
@@ -2165,7 +2150,7 @@
         <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -2179,16 +2164,16 @@
         <v>178</v>
       </c>
       <c r="F41">
-        <f>LEN(A41)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="G41" t="str">
-        <f>IF(B41="", "", IF(E41/D41&lt;&gt;FLOOR(E41/D41,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I41" t="str">
-        <f>IF(B41="",IF(A41="","","; " &amp;A41),A41&amp;REPT(" ",MAX(F:F)-F41+1)&amp;B41&amp;" ? "&amp;IF(H41&lt;&gt;"","; "&amp;H41,""))</f>
-        <v xml:space="preserve">flags_overflow              byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">flags_overflow         byte ? </v>
       </c>
       <c r="J41" t="str">
         <f>IF(B41&lt;&gt;"", "        public "&amp;VLOOKUP(B41,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A41)&amp;" = "&amp;C41&amp;";"&amp;IF(H41="",""," // "&amp;H41), IF(A41&lt;&gt;"","        // "&amp;A41,""))</f>
@@ -2200,7 +2185,7 @@
         <v>30</v>
       </c>
       <c r="B42" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -2214,16 +2199,16 @@
         <v>179</v>
       </c>
       <c r="F42">
-        <f>LEN(A42)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="G42" t="str">
-        <f>IF(B42="", "", IF(E42/D42&lt;&gt;FLOOR(E42/D42,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I42" t="str">
-        <f>IF(B42="",IF(A42="","","; " &amp;A42),A42&amp;REPT(" ",MAX(F:F)-F42+1)&amp;B42&amp;" ? "&amp;IF(H42&lt;&gt;"","; "&amp;H42,""))</f>
-        <v xml:space="preserve">flags_negative              byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">flags_negative         byte ? </v>
       </c>
       <c r="J42" t="str">
         <f>IF(B42&lt;&gt;"", "        public "&amp;VLOOKUP(B42,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A42)&amp;" = "&amp;C42&amp;";"&amp;IF(H42="",""," // "&amp;H42), IF(A42&lt;&gt;"","        // "&amp;A42,""))</f>
@@ -2235,7 +2220,7 @@
         <v>31</v>
       </c>
       <c r="B43" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -2249,16 +2234,16 @@
         <v>180</v>
       </c>
       <c r="F43">
-        <f>LEN(A43)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G43" t="str">
-        <f>IF(B43="", "", IF(E43/D43&lt;&gt;FLOOR(E43/D43,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I43" t="str">
-        <f>IF(B43="",IF(A43="","","; " &amp;A43),A43&amp;REPT(" ",MAX(F:F)-F43+1)&amp;B43&amp;" ? "&amp;IF(H43&lt;&gt;"","; "&amp;H43,""))</f>
-        <v xml:space="preserve">flags_carry                 byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">flags_carry            byte ? </v>
       </c>
       <c r="J43" t="str">
         <f>IF(B43&lt;&gt;"", "        public "&amp;VLOOKUP(B43,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A43)&amp;" = "&amp;C43&amp;";"&amp;IF(H43="",""," // "&amp;H43), IF(A43&lt;&gt;"","        // "&amp;A43,""))</f>
@@ -2270,7 +2255,7 @@
         <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -2284,16 +2269,16 @@
         <v>181</v>
       </c>
       <c r="F44">
-        <f>LEN(A44)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G44" t="str">
-        <f>IF(B44="", "", IF(E44/D44&lt;&gt;FLOOR(E44/D44,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I44" t="str">
-        <f>IF(B44="",IF(A44="","","; " &amp;A44),A44&amp;REPT(" ",MAX(F:F)-F44+1)&amp;B44&amp;" ? "&amp;IF(H44&lt;&gt;"","; "&amp;H44,""))</f>
-        <v xml:space="preserve">flags_zero                  byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">flags_zero             byte ? </v>
       </c>
       <c r="J44" t="str">
         <f>IF(B44&lt;&gt;"", "        public "&amp;VLOOKUP(B44,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A44)&amp;" = "&amp;C44&amp;";"&amp;IF(H44="",""," // "&amp;H44), IF(A44&lt;&gt;"","        // "&amp;A44,""))</f>
@@ -2305,7 +2290,7 @@
         <v>33</v>
       </c>
       <c r="B45" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -2319,16 +2304,16 @@
         <v>182</v>
       </c>
       <c r="F45">
-        <f>LEN(A45)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="G45" t="str">
-        <f>IF(B45="", "", IF(E45/D45&lt;&gt;FLOOR(E45/D45,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I45" t="str">
-        <f>IF(B45="",IF(A45="","","; " &amp;A45),A45&amp;REPT(" ",MAX(F:F)-F45+1)&amp;B45&amp;" ? "&amp;IF(H45&lt;&gt;"","; "&amp;H45,""))</f>
-        <v xml:space="preserve">flags_interruptDisable      byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">flags_interruptDisable byte ? </v>
       </c>
       <c r="J45" t="str">
         <f>IF(B45&lt;&gt;"", "        public "&amp;VLOOKUP(B45,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A45)&amp;" = "&amp;C45&amp;";"&amp;IF(H45="",""," // "&amp;H45), IF(A45&lt;&gt;"","        // "&amp;A45,""))</f>
@@ -2345,15 +2330,15 @@
         <v>182</v>
       </c>
       <c r="F46">
-        <f>LEN(A46)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G46" t="str">
-        <f>IF(B46="", "", IF(E46/D46&lt;&gt;FLOOR(E46/D46,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I46" t="str">
-        <f>IF(B46="",IF(A46="","","; " &amp;A46),A46&amp;REPT(" ",MAX(F:F)-F46+1)&amp;B46&amp;" ? "&amp;IF(H46&lt;&gt;"","; "&amp;H46,""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J46" t="str">
@@ -2366,7 +2351,7 @@
         <v>34</v>
       </c>
       <c r="B47" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -2380,16 +2365,16 @@
         <v>183</v>
       </c>
       <c r="F47">
-        <f>LEN(A47)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G47" t="str">
-        <f>IF(B47="", "", IF(E47/D47&lt;&gt;FLOOR(E47/D47,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I47" t="str">
-        <f>IF(B47="",IF(A47="","","; " &amp;A47),A47&amp;REPT(" ",MAX(F:F)-F47+1)&amp;B47&amp;" ? "&amp;IF(H47&lt;&gt;"","; "&amp;H47,""))</f>
-        <v xml:space="preserve">interrupt                   byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">interrupt              byte ? </v>
       </c>
       <c r="J47" t="str">
         <f>IF(B47&lt;&gt;"", "        public "&amp;VLOOKUP(B47,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A47)&amp;" = "&amp;C47&amp;";"&amp;IF(H47="",""," // "&amp;H47), IF(A47&lt;&gt;"","        // "&amp;A47,""))</f>
@@ -2401,7 +2386,7 @@
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -2415,16 +2400,16 @@
         <v>184</v>
       </c>
       <c r="F48">
-        <f>LEN(A48)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G48" t="str">
-        <f>IF(B48="", "", IF(E48/D48&lt;&gt;FLOOR(E48/D48,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I48" t="str">
-        <f>IF(B48="",IF(A48="","","; " &amp;A48),A48&amp;REPT(" ",MAX(F:F)-F48+1)&amp;B48&amp;" ? "&amp;IF(H48&lt;&gt;"","; "&amp;H48,""))</f>
-        <v xml:space="preserve">nmi                         byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">nmi                    byte ? </v>
       </c>
       <c r="J48" t="str">
         <f>IF(B48&lt;&gt;"", "        public "&amp;VLOOKUP(B48,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A48)&amp;" = "&amp;C48&amp;";"&amp;IF(H48="",""," // "&amp;H48), IF(A48&lt;&gt;"","        // "&amp;A48,""))</f>
@@ -2436,7 +2421,7 @@
         <v>36</v>
       </c>
       <c r="B49" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -2450,16 +2435,16 @@
         <v>185</v>
       </c>
       <c r="F49">
-        <f>LEN(A49)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="G49" t="str">
-        <f>IF(B49="", "", IF(E49/D49&lt;&gt;FLOOR(E49/D49,1),"ERROR",""))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I49" t="str">
-        <f>IF(B49="",IF(A49="","","; " &amp;A49),A49&amp;REPT(" ",MAX(F:F)-F49+1)&amp;B49&amp;" ? "&amp;IF(H49&lt;&gt;"","; "&amp;H49,""))</f>
-        <v xml:space="preserve">nmi_previous                byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">nmi_previous           byte ? </v>
       </c>
       <c r="J49" t="str">
         <f>IF(B49&lt;&gt;"", "        public "&amp;VLOOKUP(B49,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A49)&amp;" = "&amp;C49&amp;";"&amp;IF(H49="",""," // "&amp;H49), IF(A49&lt;&gt;"","        // "&amp;A49,""))</f>
@@ -2476,15 +2461,15 @@
         <v>185</v>
       </c>
       <c r="F50">
-        <f t="shared" ref="F50:F113" si="0">LEN(A50)</f>
+        <f t="shared" ref="F50:F113" si="4">LEN(A50)</f>
         <v>0</v>
       </c>
       <c r="G50" t="str">
-        <f t="shared" ref="G50:G113" si="1">IF(B50="", "", IF(E50/D50&lt;&gt;FLOOR(E50/D50,1),"ERROR",""))</f>
+        <f t="shared" ref="G50:G113" si="5">IF(B50="", "", IF(E50/D50&lt;&gt;FLOOR(E50/D50,1),"ERROR",""))</f>
         <v/>
       </c>
       <c r="I50" t="str">
-        <f>IF(B50="",IF(A50="","","; " &amp;A50),A50&amp;REPT(" ",MAX(F:F)-F50+1)&amp;B50&amp;" ? "&amp;IF(H50&lt;&gt;"","; "&amp;H50,""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J50" t="str">
@@ -2497,7 +2482,7 @@
         <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -2511,16 +2496,16 @@
         <v>186</v>
       </c>
       <c r="F51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="G51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I51" t="str">
-        <f>IF(B51="",IF(A51="","","; " &amp;A51),A51&amp;REPT(" ",MAX(F:F)-F51+1)&amp;B51&amp;" ? "&amp;IF(H51&lt;&gt;"","; "&amp;H51,""))</f>
-        <v xml:space="preserve">addrsel                     byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">addrsel                byte ? </v>
       </c>
       <c r="J51" t="str">
         <f>IF(B51&lt;&gt;"", "        public "&amp;VLOOKUP(B51,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A51)&amp;" = "&amp;C51&amp;";"&amp;IF(H51="",""," // "&amp;H51), IF(A51&lt;&gt;"","        // "&amp;A51,""))</f>
@@ -2532,7 +2517,7 @@
         <v>38</v>
       </c>
       <c r="B52" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2546,16 +2531,16 @@
         <v>187</v>
       </c>
       <c r="F52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="G52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I52" t="str">
-        <f>IF(B52="",IF(A52="","","; " &amp;A52),A52&amp;REPT(" ",MAX(F:F)-F52+1)&amp;B52&amp;" ? "&amp;IF(H52&lt;&gt;"","; "&amp;H52,""))</f>
-        <v xml:space="preserve">dcsel                       byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">dcsel                  byte ? </v>
       </c>
       <c r="J52" t="str">
         <f>IF(B52&lt;&gt;"", "        public "&amp;VLOOKUP(B52,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A52)&amp;" = "&amp;C52&amp;";"&amp;IF(H52="",""," // "&amp;H52), IF(A52&lt;&gt;"","        // "&amp;A52,""))</f>
@@ -2567,7 +2552,7 @@
         <v>39</v>
       </c>
       <c r="B53" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -2581,16 +2566,16 @@
         <v>188</v>
       </c>
       <c r="F53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="G53" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I53" t="str">
-        <f>IF(B53="",IF(A53="","","; " &amp;A53),A53&amp;REPT(" ",MAX(F:F)-F53+1)&amp;B53&amp;" ? "&amp;IF(H53&lt;&gt;"","; "&amp;H53,""))</f>
-        <v xml:space="preserve">dc_border                   byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">dc_border              byte ? </v>
       </c>
       <c r="J53" t="str">
         <f>IF(B53&lt;&gt;"", "        public "&amp;VLOOKUP(B53,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A53)&amp;" = "&amp;C53&amp;";"&amp;IF(H53="",""," // "&amp;H53), IF(A53&lt;&gt;"","        // "&amp;A53,""))</f>
@@ -2607,15 +2592,15 @@
         <v>188</v>
       </c>
       <c r="F54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G54" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I54" t="str">
-        <f>IF(B54="",IF(A54="","","; " &amp;A54),A54&amp;REPT(" ",MAX(F:F)-F54+1)&amp;B54&amp;" ? "&amp;IF(H54&lt;&gt;"","; "&amp;H54,""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J54" t="str">
@@ -2628,7 +2613,7 @@
         <v>40</v>
       </c>
       <c r="B55" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C55">
         <v>640</v>
@@ -2642,16 +2627,16 @@
         <v>190</v>
       </c>
       <c r="F55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="G55" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I55" t="str">
-        <f>IF(B55="",IF(A55="","","; " &amp;A55),A55&amp;REPT(" ",MAX(F:F)-F55+1)&amp;B55&amp;" ? "&amp;IF(H55&lt;&gt;"","; "&amp;H55,""))</f>
-        <v xml:space="preserve">dc_hstart                   word ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">dc_hstart              word ? </v>
       </c>
       <c r="J55" t="str">
         <f>IF(B55&lt;&gt;"", "        public "&amp;VLOOKUP(B55,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A55)&amp;" = "&amp;C55&amp;";"&amp;IF(H55="",""," // "&amp;H55), IF(A55&lt;&gt;"","        // "&amp;A55,""))</f>
@@ -2663,7 +2648,7 @@
         <v>41</v>
       </c>
       <c r="B56" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -2677,16 +2662,16 @@
         <v>192</v>
       </c>
       <c r="F56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="G56" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I56" t="str">
-        <f>IF(B56="",IF(A56="","","; " &amp;A56),A56&amp;REPT(" ",MAX(F:F)-F56+1)&amp;B56&amp;" ? "&amp;IF(H56&lt;&gt;"","; "&amp;H56,""))</f>
-        <v xml:space="preserve">dc_hstop                    word ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">dc_hstop               word ? </v>
       </c>
       <c r="J56" t="str">
         <f>IF(B56&lt;&gt;"", "        public "&amp;VLOOKUP(B56,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A56)&amp;" = "&amp;C56&amp;";"&amp;IF(H56="",""," // "&amp;H56), IF(A56&lt;&gt;"","        // "&amp;A56,""))</f>
@@ -2698,7 +2683,7 @@
         <v>42</v>
       </c>
       <c r="B57" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C57">
         <v>480</v>
@@ -2712,16 +2697,16 @@
         <v>194</v>
       </c>
       <c r="F57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="G57" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I57" t="str">
-        <f>IF(B57="",IF(A57="","","; " &amp;A57),A57&amp;REPT(" ",MAX(F:F)-F57+1)&amp;B57&amp;" ? "&amp;IF(H57&lt;&gt;"","; "&amp;H57,""))</f>
-        <v xml:space="preserve">dc_vstart                   word ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">dc_vstart              word ? </v>
       </c>
       <c r="J57" t="str">
         <f>IF(B57&lt;&gt;"", "        public "&amp;VLOOKUP(B57,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A57)&amp;" = "&amp;C57&amp;";"&amp;IF(H57="",""," // "&amp;H57), IF(A57&lt;&gt;"","        // "&amp;A57,""))</f>
@@ -2733,7 +2718,7 @@
         <v>43</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -2747,16 +2732,16 @@
         <v>196</v>
       </c>
       <c r="F58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="G58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I58" t="str">
-        <f>IF(B58="",IF(A58="","","; " &amp;A58),A58&amp;REPT(" ",MAX(F:F)-F58+1)&amp;B58&amp;" ? "&amp;IF(H58&lt;&gt;"","; "&amp;H58,""))</f>
-        <v xml:space="preserve">dc_vstop                    word ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">dc_vstop               word ? </v>
       </c>
       <c r="J58" t="str">
         <f>IF(B58&lt;&gt;"", "        public "&amp;VLOOKUP(B58,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A58)&amp;" = "&amp;C58&amp;";"&amp;IF(H58="",""," // "&amp;H58), IF(A58&lt;&gt;"","        // "&amp;A58,""))</f>
@@ -2773,15 +2758,15 @@
         <v>196</v>
       </c>
       <c r="F59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G59" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I59" t="str">
-        <f>IF(B59="",IF(A59="","","; " &amp;A59),A59&amp;REPT(" ",MAX(F:F)-F59+1)&amp;B59&amp;" ? "&amp;IF(H59&lt;&gt;"","; "&amp;H59,""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J59" t="str">
@@ -2794,7 +2779,7 @@
         <v>44</v>
       </c>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -2808,16 +2793,16 @@
         <v>197</v>
       </c>
       <c r="F60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="G60" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I60" t="str">
-        <f>IF(B60="",IF(A60="","","; " &amp;A60),A60&amp;REPT(" ",MAX(F:F)-F60+1)&amp;B60&amp;" ? "&amp;IF(H60&lt;&gt;"","; "&amp;H60,""))</f>
-        <v xml:space="preserve">sprite_enable               byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">sprite_enable          byte ? </v>
       </c>
       <c r="J60" t="str">
         <f>IF(B60&lt;&gt;"", "        public "&amp;VLOOKUP(B60,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A60)&amp;" = "&amp;C60&amp;";"&amp;IF(H60="",""," // "&amp;H60), IF(A60&lt;&gt;"","        // "&amp;A60,""))</f>
@@ -2829,7 +2814,7 @@
         <v>45</v>
       </c>
       <c r="B61" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -2843,16 +2828,16 @@
         <v>198</v>
       </c>
       <c r="F61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="G61" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I61" t="str">
-        <f>IF(B61="",IF(A61="","","; " &amp;A61),A61&amp;REPT(" ",MAX(F:F)-F61+1)&amp;B61&amp;" ? "&amp;IF(H61&lt;&gt;"","; "&amp;H61,""))</f>
-        <v xml:space="preserve">layer0_enable               byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">layer0_enable          byte ? </v>
       </c>
       <c r="J61" t="str">
         <f>IF(B61&lt;&gt;"", "        public "&amp;VLOOKUP(B61,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A61)&amp;" = "&amp;C61&amp;";"&amp;IF(H61="",""," // "&amp;H61), IF(A61&lt;&gt;"","        // "&amp;A61,""))</f>
@@ -2864,7 +2849,7 @@
         <v>46</v>
       </c>
       <c r="B62" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -2878,16 +2863,16 @@
         <v>199</v>
       </c>
       <c r="F62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="G62" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I62" t="str">
-        <f>IF(B62="",IF(A62="","","; " &amp;A62),A62&amp;REPT(" ",MAX(F:F)-F62+1)&amp;B62&amp;" ? "&amp;IF(H62&lt;&gt;"","; "&amp;H62,""))</f>
-        <v xml:space="preserve">layer1_enable               byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">layer1_enable          byte ? </v>
       </c>
       <c r="J62" t="str">
         <f>IF(B62&lt;&gt;"", "        public "&amp;VLOOKUP(B62,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A62)&amp;" = "&amp;C62&amp;";"&amp;IF(H62="",""," // "&amp;H62), IF(A62&lt;&gt;"","        // "&amp;A62,""))</f>
@@ -2904,15 +2889,15 @@
         <v>199</v>
       </c>
       <c r="F63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G63" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I63" t="str">
-        <f>IF(B63="",IF(A63="","","; " &amp;A63),A63&amp;REPT(" ",MAX(F:F)-F63+1)&amp;B63&amp;" ? "&amp;IF(H63&lt;&gt;"","; "&amp;H63,""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J63" t="str">
@@ -2925,7 +2910,7 @@
         <v>47</v>
       </c>
       <c r="B64" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -2939,16 +2924,16 @@
         <v>200</v>
       </c>
       <c r="F64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="G64" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I64" t="str">
-        <f>IF(B64="",IF(A64="","","; " &amp;A64),A64&amp;REPT(" ",MAX(F:F)-F64+1)&amp;B64&amp;" ? "&amp;IF(H64&lt;&gt;"","; "&amp;H64,""))</f>
-        <v xml:space="preserve">display_carry               byte ? </v>
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">display_carry          byte ? </v>
       </c>
       <c r="J64" t="str">
         <f>IF(B64&lt;&gt;"", "        public "&amp;VLOOKUP(B64,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A64)&amp;" = "&amp;C64&amp;";"&amp;IF(H64="",""," // "&amp;H64), IF(A64&lt;&gt;"","        // "&amp;A64,""))</f>
@@ -2965,15 +2950,15 @@
         <v>200</v>
       </c>
       <c r="F65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G65" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I65" t="str">
-        <f>IF(B65="",IF(A65="","","; " &amp;A65),A65&amp;REPT(" ",MAX(F:F)-F65+1)&amp;B65&amp;" ? "&amp;IF(H65&lt;&gt;"","; "&amp;H65,""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J65" t="str">
@@ -2986,7 +2971,7 @@
         <v>48</v>
       </c>
       <c r="B66" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -3000,16 +2985,16 @@
         <v>204</v>
       </c>
       <c r="F66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I66" t="str">
-        <f>IF(B66="",IF(A66="","","; " &amp;A66),A66&amp;REPT(" ",MAX(F:F)-F66+1)&amp;B66&amp;" ? "&amp;IF(H66&lt;&gt;"","; "&amp;H66,""))</f>
-        <v xml:space="preserve">layer0_mapAddress           dword ? </v>
+        <f t="shared" ref="I66:I97" si="6">IF(B66="",IF(A66="","","; " &amp;A66),A66&amp;REPT(" ",MAX(F:F)-F66+1)&amp;B66&amp;" ? "&amp;IF(H66&lt;&gt;"","; "&amp;H66,""))</f>
+        <v xml:space="preserve">layer0_mapAddress      dword ? </v>
       </c>
       <c r="J66" t="str">
         <f>IF(B66&lt;&gt;"", "        public "&amp;VLOOKUP(B66,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A66)&amp;" = "&amp;C66&amp;";"&amp;IF(H66="",""," // "&amp;H66), IF(A66&lt;&gt;"","        // "&amp;A66,""))</f>
@@ -3021,7 +3006,7 @@
         <v>49</v>
       </c>
       <c r="B67" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -3035,16 +3020,16 @@
         <v>208</v>
       </c>
       <c r="F67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I67" t="str">
-        <f>IF(B67="",IF(A67="","","; " &amp;A67),A67&amp;REPT(" ",MAX(F:F)-F67+1)&amp;B67&amp;" ? "&amp;IF(H67&lt;&gt;"","; "&amp;H67,""))</f>
-        <v xml:space="preserve">layer0_tileAddress          dword ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer0_tileAddress     dword ? </v>
       </c>
       <c r="J67" t="str">
         <f>IF(B67&lt;&gt;"", "        public "&amp;VLOOKUP(B67,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A67)&amp;" = "&amp;C67&amp;";"&amp;IF(H67="",""," // "&amp;H67), IF(A67&lt;&gt;"","        // "&amp;A67,""))</f>
@@ -3056,7 +3041,7 @@
         <v>50</v>
       </c>
       <c r="B68" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -3070,16 +3055,16 @@
         <v>210</v>
       </c>
       <c r="F68">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="G68" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I68" t="str">
-        <f>IF(B68="",IF(A68="","","; " &amp;A68),A68&amp;REPT(" ",MAX(F:F)-F68+1)&amp;B68&amp;" ? "&amp;IF(H68&lt;&gt;"","; "&amp;H68,""))</f>
-        <v xml:space="preserve">layer0_hscroll              word ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer0_hscroll         word ? </v>
       </c>
       <c r="J68" t="str">
         <f>IF(B68&lt;&gt;"", "        public "&amp;VLOOKUP(B68,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A68)&amp;" = "&amp;C68&amp;";"&amp;IF(H68="",""," // "&amp;H68), IF(A68&lt;&gt;"","        // "&amp;A68,""))</f>
@@ -3091,7 +3076,7 @@
         <v>51</v>
       </c>
       <c r="B69" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -3105,16 +3090,16 @@
         <v>212</v>
       </c>
       <c r="F69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="G69" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I69" t="str">
-        <f>IF(B69="",IF(A69="","","; " &amp;A69),A69&amp;REPT(" ",MAX(F:F)-F69+1)&amp;B69&amp;" ? "&amp;IF(H69&lt;&gt;"","; "&amp;H69,""))</f>
-        <v xml:space="preserve">layer0_vscroll              word ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer0_vscroll         word ? </v>
       </c>
       <c r="J69" t="str">
         <f>IF(B69&lt;&gt;"", "        public "&amp;VLOOKUP(B69,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A69)&amp;" = "&amp;C69&amp;";"&amp;IF(H69="",""," // "&amp;H69), IF(A69&lt;&gt;"","        // "&amp;A69,""))</f>
@@ -3126,7 +3111,7 @@
         <v>52</v>
       </c>
       <c r="B70" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -3140,16 +3125,16 @@
         <v>213</v>
       </c>
       <c r="F70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="G70" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I70" t="str">
-        <f>IF(B70="",IF(A70="","","; " &amp;A70),A70&amp;REPT(" ",MAX(F:F)-F70+1)&amp;B70&amp;" ? "&amp;IF(H70&lt;&gt;"","; "&amp;H70,""))</f>
-        <v xml:space="preserve">layer0_mapHeight            byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer0_mapHeight       byte ? </v>
       </c>
       <c r="J70" t="str">
         <f>IF(B70&lt;&gt;"", "        public "&amp;VLOOKUP(B70,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A70)&amp;" = "&amp;C70&amp;";"&amp;IF(H70="",""," // "&amp;H70), IF(A70&lt;&gt;"","        // "&amp;A70,""))</f>
@@ -3161,7 +3146,7 @@
         <v>53</v>
       </c>
       <c r="B71" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -3175,16 +3160,16 @@
         <v>214</v>
       </c>
       <c r="F71">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I71" t="str">
-        <f>IF(B71="",IF(A71="","","; " &amp;A71),A71&amp;REPT(" ",MAX(F:F)-F71+1)&amp;B71&amp;" ? "&amp;IF(H71&lt;&gt;"","; "&amp;H71,""))</f>
-        <v xml:space="preserve">layer0_mapWidth             byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer0_mapWidth        byte ? </v>
       </c>
       <c r="J71" t="str">
         <f>IF(B71&lt;&gt;"", "        public "&amp;VLOOKUP(B71,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A71)&amp;" = "&amp;C71&amp;";"&amp;IF(H71="",""," // "&amp;H71), IF(A71&lt;&gt;"","        // "&amp;A71,""))</f>
@@ -3196,7 +3181,7 @@
         <v>54</v>
       </c>
       <c r="B72" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -3210,16 +3195,16 @@
         <v>215</v>
       </c>
       <c r="F72">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="G72" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I72" t="str">
-        <f>IF(B72="",IF(A72="","","; " &amp;A72),A72&amp;REPT(" ",MAX(F:F)-F72+1)&amp;B72&amp;" ? "&amp;IF(H72&lt;&gt;"","; "&amp;H72,""))</f>
-        <v xml:space="preserve">layer0_bitmapMode           byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer0_bitmapMode      byte ? </v>
       </c>
       <c r="J72" t="str">
         <f>IF(B72&lt;&gt;"", "        public "&amp;VLOOKUP(B72,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A72)&amp;" = "&amp;C72&amp;";"&amp;IF(H72="",""," // "&amp;H72), IF(A72&lt;&gt;"","        // "&amp;A72,""))</f>
@@ -3231,7 +3216,7 @@
         <v>55</v>
       </c>
       <c r="B73" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -3245,16 +3230,16 @@
         <v>216</v>
       </c>
       <c r="F73">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I73" t="str">
-        <f>IF(B73="",IF(A73="","","; " &amp;A73),A73&amp;REPT(" ",MAX(F:F)-F73+1)&amp;B73&amp;" ? "&amp;IF(H73&lt;&gt;"","; "&amp;H73,""))</f>
-        <v xml:space="preserve">layer0_colourDepth          byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer0_colourDepth     byte ? </v>
       </c>
       <c r="J73" t="str">
         <f>IF(B73&lt;&gt;"", "        public "&amp;VLOOKUP(B73,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A73)&amp;" = "&amp;C73&amp;";"&amp;IF(H73="",""," // "&amp;H73), IF(A73&lt;&gt;"","        // "&amp;A73,""))</f>
@@ -3266,7 +3251,7 @@
         <v>56</v>
       </c>
       <c r="B74" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -3280,16 +3265,16 @@
         <v>217</v>
       </c>
       <c r="F74">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="G74" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I74" t="str">
-        <f>IF(B74="",IF(A74="","","; " &amp;A74),A74&amp;REPT(" ",MAX(F:F)-F74+1)&amp;B74&amp;" ? "&amp;IF(H74&lt;&gt;"","; "&amp;H74,""))</f>
-        <v xml:space="preserve">layer0_tileHeight           byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer0_tileHeight      byte ? </v>
       </c>
       <c r="J74" t="str">
         <f>IF(B74&lt;&gt;"", "        public "&amp;VLOOKUP(B74,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A74)&amp;" = "&amp;C74&amp;";"&amp;IF(H74="",""," // "&amp;H74), IF(A74&lt;&gt;"","        // "&amp;A74,""))</f>
@@ -3301,7 +3286,7 @@
         <v>57</v>
       </c>
       <c r="B75" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -3315,16 +3300,16 @@
         <v>218</v>
       </c>
       <c r="F75">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I75" t="str">
-        <f>IF(B75="",IF(A75="","","; " &amp;A75),A75&amp;REPT(" ",MAX(F:F)-F75+1)&amp;B75&amp;" ? "&amp;IF(H75&lt;&gt;"","; "&amp;H75,""))</f>
-        <v xml:space="preserve">layer0_tileWidth            byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer0_tileWidth       byte ? </v>
       </c>
       <c r="J75" t="str">
         <f>IF(B75&lt;&gt;"", "        public "&amp;VLOOKUP(B75,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A75)&amp;" = "&amp;C75&amp;";"&amp;IF(H75="",""," // "&amp;H75), IF(A75&lt;&gt;"","        // "&amp;A75,""))</f>
@@ -3341,15 +3326,15 @@
         <v>218</v>
       </c>
       <c r="F76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G76" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I76" t="str">
-        <f>IF(B76="",IF(A76="","","; " &amp;A76),A76&amp;REPT(" ",MAX(F:F)-F76+1)&amp;B76&amp;" ? "&amp;IF(H76&lt;&gt;"","; "&amp;H76,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="J76" t="str">
@@ -3362,7 +3347,7 @@
         <v>58</v>
       </c>
       <c r="B77" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -3376,16 +3361,16 @@
         <v>219</v>
       </c>
       <c r="F77">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G77" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I77" t="str">
-        <f>IF(B77="",IF(A77="","","; " &amp;A77),A77&amp;REPT(" ",MAX(F:F)-F77+1)&amp;B77&amp;" ? "&amp;IF(H77&lt;&gt;"","; "&amp;H77,""))</f>
-        <v xml:space="preserve">cpu_waiting                 byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">cpu_waiting            byte ? </v>
       </c>
       <c r="J77" t="str">
         <f>IF(B77&lt;&gt;"", "        public "&amp;VLOOKUP(B77,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A77)&amp;" = "&amp;C77&amp;";"&amp;IF(H77="",""," // "&amp;H77), IF(A77&lt;&gt;"","        // "&amp;A77,""))</f>
@@ -3397,7 +3382,7 @@
         <v>59</v>
       </c>
       <c r="B78" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -3411,16 +3396,16 @@
         <v>220</v>
       </c>
       <c r="F78">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="G78" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I78" t="str">
-        <f>IF(B78="",IF(A78="","","; " &amp;A78),A78&amp;REPT(" ",MAX(F:F)-F78+1)&amp;B78&amp;" ? "&amp;IF(H78&lt;&gt;"","; "&amp;H78,""))</f>
-        <v xml:space="preserve">headless                    byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">headless               byte ? </v>
       </c>
       <c r="J78" t="str">
         <f>IF(B78&lt;&gt;"", "        public "&amp;VLOOKUP(B78,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A78)&amp;" = "&amp;C78&amp;";"&amp;IF(H78="",""," // "&amp;H78), IF(A78&lt;&gt;"","        // "&amp;A78,""))</f>
@@ -3437,15 +3422,15 @@
         <v>220</v>
       </c>
       <c r="F79">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G79" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I79" t="str">
-        <f>IF(B79="",IF(A79="","","; " &amp;A79),A79&amp;REPT(" ",MAX(F:F)-F79+1)&amp;B79&amp;" ? "&amp;IF(H79&lt;&gt;"","; "&amp;H79,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="J79" t="str">
@@ -3458,7 +3443,7 @@
         <v>60</v>
       </c>
       <c r="B80" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -3472,16 +3457,16 @@
         <v>224</v>
       </c>
       <c r="F80">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="G80" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I80" t="str">
-        <f>IF(B80="",IF(A80="","","; " &amp;A80),A80&amp;REPT(" ",MAX(F:F)-F80+1)&amp;B80&amp;" ? "&amp;IF(H80&lt;&gt;"","; "&amp;H80,""))</f>
-        <v xml:space="preserve">layer1_mapAddress           dword ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer1_mapAddress      dword ? </v>
       </c>
       <c r="J80" t="str">
         <f>IF(B80&lt;&gt;"", "        public "&amp;VLOOKUP(B80,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A80)&amp;" = "&amp;C80&amp;";"&amp;IF(H80="",""," // "&amp;H80), IF(A80&lt;&gt;"","        // "&amp;A80,""))</f>
@@ -3493,7 +3478,7 @@
         <v>61</v>
       </c>
       <c r="B81" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -3507,16 +3492,16 @@
         <v>228</v>
       </c>
       <c r="F81">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G81" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I81" t="str">
-        <f>IF(B81="",IF(A81="","","; " &amp;A81),A81&amp;REPT(" ",MAX(F:F)-F81+1)&amp;B81&amp;" ? "&amp;IF(H81&lt;&gt;"","; "&amp;H81,""))</f>
-        <v xml:space="preserve">layer1_tileAddress          dword ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer1_tileAddress     dword ? </v>
       </c>
       <c r="J81" t="str">
         <f>IF(B81&lt;&gt;"", "        public "&amp;VLOOKUP(B81,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A81)&amp;" = "&amp;C81&amp;";"&amp;IF(H81="",""," // "&amp;H81), IF(A81&lt;&gt;"","        // "&amp;A81,""))</f>
@@ -3528,7 +3513,7 @@
         <v>62</v>
       </c>
       <c r="B82" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -3542,16 +3527,16 @@
         <v>230</v>
       </c>
       <c r="F82">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="G82" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I82" t="str">
-        <f>IF(B82="",IF(A82="","","; " &amp;A82),A82&amp;REPT(" ",MAX(F:F)-F82+1)&amp;B82&amp;" ? "&amp;IF(H82&lt;&gt;"","; "&amp;H82,""))</f>
-        <v xml:space="preserve">layer1_hscroll              word ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer1_hscroll         word ? </v>
       </c>
       <c r="J82" t="str">
         <f>IF(B82&lt;&gt;"", "        public "&amp;VLOOKUP(B82,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A82)&amp;" = "&amp;C82&amp;";"&amp;IF(H82="",""," // "&amp;H82), IF(A82&lt;&gt;"","        // "&amp;A82,""))</f>
@@ -3563,7 +3548,7 @@
         <v>63</v>
       </c>
       <c r="B83" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -3577,16 +3562,16 @@
         <v>232</v>
       </c>
       <c r="F83">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="G83" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I83" t="str">
-        <f>IF(B83="",IF(A83="","","; " &amp;A83),A83&amp;REPT(" ",MAX(F:F)-F83+1)&amp;B83&amp;" ? "&amp;IF(H83&lt;&gt;"","; "&amp;H83,""))</f>
-        <v xml:space="preserve">layer1_vscroll              word ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer1_vscroll         word ? </v>
       </c>
       <c r="J83" t="str">
         <f>IF(B83&lt;&gt;"", "        public "&amp;VLOOKUP(B83,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A83)&amp;" = "&amp;C83&amp;";"&amp;IF(H83="",""," // "&amp;H83), IF(A83&lt;&gt;"","        // "&amp;A83,""))</f>
@@ -3598,7 +3583,7 @@
         <v>64</v>
       </c>
       <c r="B84" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -3612,16 +3597,16 @@
         <v>233</v>
       </c>
       <c r="F84">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="G84" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I84" t="str">
-        <f>IF(B84="",IF(A84="","","; " &amp;A84),A84&amp;REPT(" ",MAX(F:F)-F84+1)&amp;B84&amp;" ? "&amp;IF(H84&lt;&gt;"","; "&amp;H84,""))</f>
-        <v xml:space="preserve">layer1_mapHeight            byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer1_mapHeight       byte ? </v>
       </c>
       <c r="J84" t="str">
         <f>IF(B84&lt;&gt;"", "        public "&amp;VLOOKUP(B84,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A84)&amp;" = "&amp;C84&amp;";"&amp;IF(H84="",""," // "&amp;H84), IF(A84&lt;&gt;"","        // "&amp;A84,""))</f>
@@ -3633,7 +3618,7 @@
         <v>65</v>
       </c>
       <c r="B85" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -3647,16 +3632,16 @@
         <v>234</v>
       </c>
       <c r="F85">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="G85" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I85" t="str">
-        <f>IF(B85="",IF(A85="","","; " &amp;A85),A85&amp;REPT(" ",MAX(F:F)-F85+1)&amp;B85&amp;" ? "&amp;IF(H85&lt;&gt;"","; "&amp;H85,""))</f>
-        <v xml:space="preserve">layer1_mapWidth             byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer1_mapWidth        byte ? </v>
       </c>
       <c r="J85" t="str">
         <f>IF(B85&lt;&gt;"", "        public "&amp;VLOOKUP(B85,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A85)&amp;" = "&amp;C85&amp;";"&amp;IF(H85="",""," // "&amp;H85), IF(A85&lt;&gt;"","        // "&amp;A85,""))</f>
@@ -3668,7 +3653,7 @@
         <v>66</v>
       </c>
       <c r="B86" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -3682,16 +3667,16 @@
         <v>235</v>
       </c>
       <c r="F86">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="G86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I86" t="str">
-        <f>IF(B86="",IF(A86="","","; " &amp;A86),A86&amp;REPT(" ",MAX(F:F)-F86+1)&amp;B86&amp;" ? "&amp;IF(H86&lt;&gt;"","; "&amp;H86,""))</f>
-        <v xml:space="preserve">layer1_bitmapMode           byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer1_bitmapMode      byte ? </v>
       </c>
       <c r="J86" t="str">
         <f>IF(B86&lt;&gt;"", "        public "&amp;VLOOKUP(B86,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A86)&amp;" = "&amp;C86&amp;";"&amp;IF(H86="",""," // "&amp;H86), IF(A86&lt;&gt;"","        // "&amp;A86,""))</f>
@@ -3703,7 +3688,7 @@
         <v>67</v>
       </c>
       <c r="B87" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -3717,16 +3702,16 @@
         <v>236</v>
       </c>
       <c r="F87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G87" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I87" t="str">
-        <f>IF(B87="",IF(A87="","","; " &amp;A87),A87&amp;REPT(" ",MAX(F:F)-F87+1)&amp;B87&amp;" ? "&amp;IF(H87&lt;&gt;"","; "&amp;H87,""))</f>
-        <v xml:space="preserve">layer1_colourDepth          byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer1_colourDepth     byte ? </v>
       </c>
       <c r="J87" t="str">
         <f>IF(B87&lt;&gt;"", "        public "&amp;VLOOKUP(B87,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A87)&amp;" = "&amp;C87&amp;";"&amp;IF(H87="",""," // "&amp;H87), IF(A87&lt;&gt;"","        // "&amp;A87,""))</f>
@@ -3738,7 +3723,7 @@
         <v>68</v>
       </c>
       <c r="B88" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -3752,16 +3737,16 @@
         <v>237</v>
       </c>
       <c r="F88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="G88" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I88" t="str">
-        <f>IF(B88="",IF(A88="","","; " &amp;A88),A88&amp;REPT(" ",MAX(F:F)-F88+1)&amp;B88&amp;" ? "&amp;IF(H88&lt;&gt;"","; "&amp;H88,""))</f>
-        <v xml:space="preserve">layer1_tileHeight           byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer1_tileHeight      byte ? </v>
       </c>
       <c r="J88" t="str">
         <f>IF(B88&lt;&gt;"", "        public "&amp;VLOOKUP(B88,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A88)&amp;" = "&amp;C88&amp;";"&amp;IF(H88="",""," // "&amp;H88), IF(A88&lt;&gt;"","        // "&amp;A88,""))</f>
@@ -3773,7 +3758,7 @@
         <v>69</v>
       </c>
       <c r="B89" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -3787,16 +3772,16 @@
         <v>238</v>
       </c>
       <c r="F89">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="G89" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I89" t="str">
-        <f>IF(B89="",IF(A89="","","; " &amp;A89),A89&amp;REPT(" ",MAX(F:F)-F89+1)&amp;B89&amp;" ? "&amp;IF(H89&lt;&gt;"","; "&amp;H89,""))</f>
-        <v xml:space="preserve">layer1_tileWidth            byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">layer1_tileWidth       byte ? </v>
       </c>
       <c r="J89" t="str">
         <f>IF(B89&lt;&gt;"", "        public "&amp;VLOOKUP(B89,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A89)&amp;" = "&amp;C89&amp;";"&amp;IF(H89="",""," // "&amp;H89), IF(A89&lt;&gt;"","        // "&amp;A89,""))</f>
@@ -3813,15 +3798,15 @@
         <v>238</v>
       </c>
       <c r="F90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G90" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I90" t="str">
-        <f>IF(B90="",IF(A90="","","; " &amp;A90),A90&amp;REPT(" ",MAX(F:F)-F90+1)&amp;B90&amp;" ? "&amp;IF(H90&lt;&gt;"","; "&amp;H90,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="J90" t="str">
@@ -3834,7 +3819,7 @@
         <v>70</v>
       </c>
       <c r="B91" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -3848,16 +3833,16 @@
         <v>240</v>
       </c>
       <c r="F91">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="G91" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I91" t="str">
-        <f>IF(B91="",IF(A91="","","; " &amp;A91),A91&amp;REPT(" ",MAX(F:F)-F91+1)&amp;B91&amp;" ? "&amp;IF(H91&lt;&gt;"","; "&amp;H91,""))</f>
-        <v xml:space="preserve">interrupt_linenum           word ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">interrupt_linenum      word ? </v>
       </c>
       <c r="J91" t="str">
         <f>IF(B91&lt;&gt;"", "        public "&amp;VLOOKUP(B91,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A91)&amp;" = "&amp;C91&amp;";"&amp;IF(H91="",""," // "&amp;H91), IF(A91&lt;&gt;"","        // "&amp;A91,""))</f>
@@ -3869,7 +3854,7 @@
         <v>71</v>
       </c>
       <c r="B92" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -3883,16 +3868,16 @@
         <v>241</v>
       </c>
       <c r="F92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="G92" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I92" t="str">
-        <f>IF(B92="",IF(A92="","","; " &amp;A92),A92&amp;REPT(" ",MAX(F:F)-F92+1)&amp;B92&amp;" ? "&amp;IF(H92&lt;&gt;"","; "&amp;H92,""))</f>
-        <v xml:space="preserve">interrupt_aflow             byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">interrupt_aflow        byte ? </v>
       </c>
       <c r="J92" t="str">
         <f>IF(B92&lt;&gt;"", "        public "&amp;VLOOKUP(B92,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A92)&amp;" = "&amp;C92&amp;";"&amp;IF(H92="",""," // "&amp;H92), IF(A92&lt;&gt;"","        // "&amp;A92,""))</f>
@@ -3904,7 +3889,7 @@
         <v>72</v>
       </c>
       <c r="B93" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -3918,16 +3903,16 @@
         <v>242</v>
       </c>
       <c r="F93">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="G93" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I93" t="str">
-        <f>IF(B93="",IF(A93="","","; " &amp;A93),A93&amp;REPT(" ",MAX(F:F)-F93+1)&amp;B93&amp;" ? "&amp;IF(H93&lt;&gt;"","; "&amp;H93,""))</f>
-        <v xml:space="preserve">interrupt_spcol             byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">interrupt_spcol        byte ? </v>
       </c>
       <c r="J93" t="str">
         <f>IF(B93&lt;&gt;"", "        public "&amp;VLOOKUP(B93,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A93)&amp;" = "&amp;C93&amp;";"&amp;IF(H93="",""," // "&amp;H93), IF(A93&lt;&gt;"","        // "&amp;A93,""))</f>
@@ -3939,7 +3924,7 @@
         <v>73</v>
       </c>
       <c r="B94" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -3953,16 +3938,16 @@
         <v>243</v>
       </c>
       <c r="F94">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="G94" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I94" t="str">
-        <f>IF(B94="",IF(A94="","","; " &amp;A94),A94&amp;REPT(" ",MAX(F:F)-F94+1)&amp;B94&amp;" ? "&amp;IF(H94&lt;&gt;"","; "&amp;H94,""))</f>
-        <v xml:space="preserve">interrupt_line              byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">interrupt_line         byte ? </v>
       </c>
       <c r="J94" t="str">
         <f>IF(B94&lt;&gt;"", "        public "&amp;VLOOKUP(B94,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A94)&amp;" = "&amp;C94&amp;";"&amp;IF(H94="",""," // "&amp;H94), IF(A94&lt;&gt;"","        // "&amp;A94,""))</f>
@@ -3974,7 +3959,7 @@
         <v>74</v>
       </c>
       <c r="B95" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -3988,16 +3973,16 @@
         <v>244</v>
       </c>
       <c r="F95">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="G95" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I95" t="str">
-        <f>IF(B95="",IF(A95="","","; " &amp;A95),A95&amp;REPT(" ",MAX(F:F)-F95+1)&amp;B95&amp;" ? "&amp;IF(H95&lt;&gt;"","; "&amp;H95,""))</f>
-        <v xml:space="preserve">interrupt_vsync             byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">interrupt_vsync        byte ? </v>
       </c>
       <c r="J95" t="str">
         <f>IF(B95&lt;&gt;"", "        public "&amp;VLOOKUP(B95,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A95)&amp;" = "&amp;C95&amp;";"&amp;IF(H95="",""," // "&amp;H95), IF(A95&lt;&gt;"","        // "&amp;A95,""))</f>
@@ -4014,15 +3999,15 @@
         <v>244</v>
       </c>
       <c r="F96">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G96" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I96" t="str">
-        <f>IF(B96="",IF(A96="","","; " &amp;A96),A96&amp;REPT(" ",MAX(F:F)-F96+1)&amp;B96&amp;" ? "&amp;IF(H96&lt;&gt;"","; "&amp;H96,""))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="J96" t="str">
@@ -4035,7 +4020,7 @@
         <v>75</v>
       </c>
       <c r="B97" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -4049,16 +4034,16 @@
         <v>245</v>
       </c>
       <c r="F97">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G97" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I97" t="str">
-        <f>IF(B97="",IF(A97="","","; " &amp;A97),A97&amp;REPT(" ",MAX(F:F)-F97+1)&amp;B97&amp;" ? "&amp;IF(H97&lt;&gt;"","; "&amp;H97,""))</f>
-        <v xml:space="preserve">interrupt_line_hit          byte ? </v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">interrupt_line_hit     byte ? </v>
       </c>
       <c r="J97" t="str">
         <f>IF(B97&lt;&gt;"", "        public "&amp;VLOOKUP(B97,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A97)&amp;" = "&amp;C97&amp;";"&amp;IF(H97="",""," // "&amp;H97), IF(A97&lt;&gt;"","        // "&amp;A97,""))</f>
@@ -4070,7 +4055,7 @@
         <v>76</v>
       </c>
       <c r="B98" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -4084,16 +4069,16 @@
         <v>246</v>
       </c>
       <c r="F98">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="G98" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I98" t="str">
-        <f>IF(B98="",IF(A98="","","; " &amp;A98),A98&amp;REPT(" ",MAX(F:F)-F98+1)&amp;B98&amp;" ? "&amp;IF(H98&lt;&gt;"","; "&amp;H98,""))</f>
-        <v xml:space="preserve">interrupt_vsync_hit         byte ? </v>
+        <f t="shared" ref="I98:I129" si="7">IF(B98="",IF(A98="","","; " &amp;A98),A98&amp;REPT(" ",MAX(F:F)-F98+1)&amp;B98&amp;" ? "&amp;IF(H98&lt;&gt;"","; "&amp;H98,""))</f>
+        <v xml:space="preserve">interrupt_vsync_hit    byte ? </v>
       </c>
       <c r="J98" t="str">
         <f>IF(B98&lt;&gt;"", "        public "&amp;VLOOKUP(B98,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A98)&amp;" = "&amp;C98&amp;";"&amp;IF(H98="",""," // "&amp;H98), IF(A98&lt;&gt;"","        // "&amp;A98,""))</f>
@@ -4105,7 +4090,7 @@
         <v>77</v>
       </c>
       <c r="B99" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -4119,16 +4104,16 @@
         <v>247</v>
       </c>
       <c r="F99">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="G99" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I99" t="str">
-        <f>IF(B99="",IF(A99="","","; " &amp;A99),A99&amp;REPT(" ",MAX(F:F)-F99+1)&amp;B99&amp;" ? "&amp;IF(H99&lt;&gt;"","; "&amp;H99,""))</f>
-        <v xml:space="preserve">interrupt_spcol_hit         byte ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">interrupt_spcol_hit    byte ? </v>
       </c>
       <c r="J99" t="str">
         <f>IF(B99&lt;&gt;"", "        public "&amp;VLOOKUP(B99,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A99)&amp;" = "&amp;C99&amp;";"&amp;IF(H99="",""," // "&amp;H99), IF(A99&lt;&gt;"","        // "&amp;A99,""))</f>
@@ -4140,7 +4125,7 @@
         <v>78</v>
       </c>
       <c r="B100" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -4154,16 +4139,16 @@
         <v>248</v>
       </c>
       <c r="F100">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="G100" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I100" t="str">
-        <f>IF(B100="",IF(A100="","","; " &amp;A100),A100&amp;REPT(" ",MAX(F:F)-F100+1)&amp;B100&amp;" ? "&amp;IF(H100&lt;&gt;"","; "&amp;H100,""))</f>
-        <v xml:space="preserve">drawing                     byte ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">drawing                byte ? </v>
       </c>
       <c r="J100" t="str">
         <f>IF(B100&lt;&gt;"", "        public "&amp;VLOOKUP(B100,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A100)&amp;" = "&amp;C100&amp;";"&amp;IF(H100="",""," // "&amp;H100), IF(A100&lt;&gt;"","        // "&amp;A100,""))</f>
@@ -4180,15 +4165,15 @@
         <v>248</v>
       </c>
       <c r="F101">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G101" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I101" t="str">
-        <f>IF(B101="",IF(A101="","","; " &amp;A101),A101&amp;REPT(" ",MAX(F:F)-F101+1)&amp;B101&amp;" ? "&amp;IF(H101&lt;&gt;"","; "&amp;H101,""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J101" t="str">
@@ -4198,7 +4183,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D102" t="str">
         <f>IF(B102="", "", VLOOKUP(B102,Sheet2!A:B,2,FALSE))</f>
@@ -4209,15 +4194,15 @@
         <v>248</v>
       </c>
       <c r="F102">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="G102" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I102" t="str">
-        <f>IF(B102="",IF(A102="","","; " &amp;A102),A102&amp;REPT(" ",MAX(F:F)-F102+1)&amp;B102&amp;" ? "&amp;IF(H102&lt;&gt;"","; "&amp;H102,""))</f>
+        <f t="shared" si="7"/>
         <v>; Rendering</v>
       </c>
       <c r="J102" t="str">
@@ -4230,7 +4215,7 @@
         <v>79</v>
       </c>
       <c r="B103" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -4244,19 +4229,19 @@
         <v>252</v>
       </c>
       <c r="F103">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="G103" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H103" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="I103" t="str">
-        <f>IF(B103="",IF(A103="","","; " &amp;A103),A103&amp;REPT(" ",MAX(F:F)-F103+1)&amp;B103&amp;" ? "&amp;IF(H103&lt;&gt;"","; "&amp;H103,""))</f>
-        <v>display_position            dword ? ; needs to be inline with the cpu clock</v>
+        <f t="shared" si="7"/>
+        <v>display_position       dword ? ; needs to be inline with the cpu clock</v>
       </c>
       <c r="J103" t="str">
         <f>IF(B103&lt;&gt;"", "        public "&amp;VLOOKUP(B103,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A103)&amp;" = "&amp;C103&amp;";"&amp;IF(H103="",""," // "&amp;H103), IF(A103&lt;&gt;"","        // "&amp;A103,""))</f>
@@ -4268,7 +4253,7 @@
         <v>80</v>
       </c>
       <c r="B104" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -4282,16 +4267,16 @@
         <v>256</v>
       </c>
       <c r="F104">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G104" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I104" t="str">
-        <f>IF(B104="",IF(A104="","","; " &amp;A104),A104&amp;REPT(" ",MAX(F:F)-F104+1)&amp;B104&amp;" ? "&amp;IF(H104&lt;&gt;"","; "&amp;H104,""))</f>
-        <v xml:space="preserve">frame_count                 dword ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">frame_count            dword ? </v>
       </c>
       <c r="J104" t="str">
         <f>IF(B104&lt;&gt;"", "        public "&amp;VLOOKUP(B104,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A104)&amp;" = "&amp;C104&amp;";"&amp;IF(H104="",""," // "&amp;H104), IF(A104&lt;&gt;"","        // "&amp;A104,""))</f>
@@ -4303,7 +4288,7 @@
         <v>81</v>
       </c>
       <c r="B105" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -4317,16 +4302,16 @@
         <v>260</v>
       </c>
       <c r="F105">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="G105" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I105" t="str">
-        <f>IF(B105="",IF(A105="","","; " &amp;A105),A105&amp;REPT(" ",MAX(F:F)-F105+1)&amp;B105&amp;" ? "&amp;IF(H105&lt;&gt;"","; "&amp;H105,""))</f>
-        <v xml:space="preserve">buffer_render_position      dword ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">buffer_render_position dword ? </v>
       </c>
       <c r="J105" t="str">
         <f>IF(B105&lt;&gt;"", "        public "&amp;VLOOKUP(B105,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A105)&amp;" = "&amp;C105&amp;";"&amp;IF(H105="",""," // "&amp;H105), IF(A105&lt;&gt;"","        // "&amp;A105,""))</f>
@@ -4338,7 +4323,7 @@
         <v>82</v>
       </c>
       <c r="B106" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -4352,16 +4337,16 @@
         <v>264</v>
       </c>
       <c r="F106">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="G106" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I106" t="str">
-        <f>IF(B106="",IF(A106="","","; " &amp;A106),A106&amp;REPT(" ",MAX(F:F)-F106+1)&amp;B106&amp;" ? "&amp;IF(H106&lt;&gt;"","; "&amp;H106,""))</f>
-        <v xml:space="preserve">buffer_output_position      dword ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">buffer_output_position dword ? </v>
       </c>
       <c r="J106" t="str">
         <f>IF(B106&lt;&gt;"", "        public "&amp;VLOOKUP(B106,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A106)&amp;" = "&amp;C106&amp;";"&amp;IF(H106="",""," // "&amp;H106), IF(A106&lt;&gt;"","        // "&amp;A106,""))</f>
@@ -4373,7 +4358,7 @@
         <v>83</v>
       </c>
       <c r="B107" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -4387,16 +4372,16 @@
         <v>268</v>
       </c>
       <c r="F107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="G107" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I107" t="str">
-        <f>IF(B107="",IF(A107="","","; " &amp;A107),A107&amp;REPT(" ",MAX(F:F)-F107+1)&amp;B107&amp;" ? "&amp;IF(H107&lt;&gt;"","; "&amp;H107,""))</f>
-        <v xml:space="preserve">scale_x                     dword ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">scale_x                dword ? </v>
       </c>
       <c r="J107" t="str">
         <f>IF(B107&lt;&gt;"", "        public "&amp;VLOOKUP(B107,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A107)&amp;" = "&amp;C107&amp;";"&amp;IF(H107="",""," // "&amp;H107), IF(A107&lt;&gt;"","        // "&amp;A107,""))</f>
@@ -4408,7 +4393,7 @@
         <v>84</v>
       </c>
       <c r="B108" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -4422,16 +4407,16 @@
         <v>272</v>
       </c>
       <c r="F108">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="G108" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I108" t="str">
-        <f>IF(B108="",IF(A108="","","; " &amp;A108),A108&amp;REPT(" ",MAX(F:F)-F108+1)&amp;B108&amp;" ? "&amp;IF(H108&lt;&gt;"","; "&amp;H108,""))</f>
-        <v xml:space="preserve">scale_y                     dword ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">scale_y                dword ? </v>
       </c>
       <c r="J108" t="str">
         <f>IF(B108&lt;&gt;"", "        public "&amp;VLOOKUP(B108,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A108)&amp;" = "&amp;C108&amp;";"&amp;IF(H108="",""," // "&amp;H108), IF(A108&lt;&gt;"","        // "&amp;A108,""))</f>
@@ -4443,7 +4428,7 @@
         <v>85</v>
       </c>
       <c r="B109" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -4457,16 +4442,16 @@
         <v>274</v>
       </c>
       <c r="F109">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="G109" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I109" t="str">
-        <f>IF(B109="",IF(A109="","","; " &amp;A109),A109&amp;REPT(" ",MAX(F:F)-F109+1)&amp;B109&amp;" ? "&amp;IF(H109&lt;&gt;"","; "&amp;H109,""))</f>
-        <v xml:space="preserve">display_x                   word ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">display_x              word ? </v>
       </c>
       <c r="J109" t="str">
         <f>IF(B109&lt;&gt;"", "        public "&amp;VLOOKUP(B109,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A109)&amp;" = "&amp;C109&amp;";"&amp;IF(H109="",""," // "&amp;H109), IF(A109&lt;&gt;"","        // "&amp;A109,""))</f>
@@ -4478,7 +4463,7 @@
         <v>86</v>
       </c>
       <c r="B110" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -4492,16 +4477,16 @@
         <v>276</v>
       </c>
       <c r="F110">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="G110" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I110" t="str">
-        <f>IF(B110="",IF(A110="","","; " &amp;A110),A110&amp;REPT(" ",MAX(F:F)-F110+1)&amp;B110&amp;" ? "&amp;IF(H110&lt;&gt;"","; "&amp;H110,""))</f>
-        <v xml:space="preserve">display_y                   word ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">display_y              word ? </v>
       </c>
       <c r="J110" t="str">
         <f>IF(B110&lt;&gt;"", "        public "&amp;VLOOKUP(B110,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A110)&amp;" = "&amp;C110&amp;";"&amp;IF(H110="",""," // "&amp;H110), IF(A110&lt;&gt;"","        // "&amp;A110,""))</f>
@@ -4518,15 +4503,15 @@
         <v>276</v>
       </c>
       <c r="F111">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G111" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I111" t="str">
-        <f>IF(B111="",IF(A111="","","; " &amp;A111),A111&amp;REPT(" ",MAX(F:F)-F111+1)&amp;B111&amp;" ? "&amp;IF(H111&lt;&gt;"","; "&amp;H111,""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J111" t="str">
@@ -4536,7 +4521,7 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D112" t="str">
         <f>IF(B112="", "", VLOOKUP(B112,Sheet2!A:B,2,FALSE))</f>
@@ -4547,15 +4532,15 @@
         <v>276</v>
       </c>
       <c r="F112">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="G112" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I112" t="str">
-        <f>IF(B112="",IF(A112="","","; " &amp;A112),A112&amp;REPT(" ",MAX(F:F)-F112+1)&amp;B112&amp;" ? "&amp;IF(H112&lt;&gt;"","; "&amp;H112,""))</f>
+        <f t="shared" si="7"/>
         <v>; Layer 0</v>
       </c>
       <c r="J112" t="str">
@@ -4568,7 +4553,7 @@
         <v>87</v>
       </c>
       <c r="B113" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -4582,16 +4567,16 @@
         <v>278</v>
       </c>
       <c r="F113">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G113" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I113" t="str">
-        <f>IF(B113="",IF(A113="","","; " &amp;A113),A113&amp;REPT(" ",MAX(F:F)-F113+1)&amp;B113&amp;" ? "&amp;IF(H113&lt;&gt;"","; "&amp;H113,""))</f>
-        <v xml:space="preserve">layer0_next_render          word ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">layer0_next_render     word ? </v>
       </c>
       <c r="J113" t="str">
         <f>IF(B113&lt;&gt;"", "        public "&amp;VLOOKUP(B113,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A113)&amp;" = "&amp;C113&amp;";"&amp;IF(H113="",""," // "&amp;H113), IF(A113&lt;&gt;"","        // "&amp;A113,""))</f>
@@ -4603,7 +4588,7 @@
         <v>88</v>
       </c>
       <c r="B114" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -4617,16 +4602,16 @@
         <v>280</v>
       </c>
       <c r="F114">
-        <f t="shared" ref="F114:F153" si="2">LEN(A114)</f>
+        <f t="shared" ref="F114:F153" si="8">LEN(A114)</f>
         <v>18</v>
       </c>
       <c r="G114" t="str">
-        <f t="shared" ref="G114:G153" si="3">IF(B114="", "", IF(E114/D114&lt;&gt;FLOOR(E114/D114,1),"ERROR",""))</f>
+        <f t="shared" ref="G114:G153" si="9">IF(B114="", "", IF(E114/D114&lt;&gt;FLOOR(E114/D114,1),"ERROR",""))</f>
         <v/>
       </c>
       <c r="I114" t="str">
-        <f>IF(B114="",IF(A114="","","; " &amp;A114),A114&amp;REPT(" ",MAX(F:F)-F114+1)&amp;B114&amp;" ? "&amp;IF(H114&lt;&gt;"","; "&amp;H114,""))</f>
-        <v xml:space="preserve">layer0_tile_hshift          word ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">layer0_tile_hshift     word ? </v>
       </c>
       <c r="J114" t="str">
         <f>IF(B114&lt;&gt;"", "        public "&amp;VLOOKUP(B114,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A114)&amp;" = "&amp;C114&amp;";"&amp;IF(H114="",""," // "&amp;H114), IF(A114&lt;&gt;"","        // "&amp;A114,""))</f>
@@ -4638,7 +4623,7 @@
         <v>89</v>
       </c>
       <c r="B115" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -4652,16 +4637,16 @@
         <v>282</v>
       </c>
       <c r="F115">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="G115" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I115" t="str">
-        <f>IF(B115="",IF(A115="","","; " &amp;A115),A115&amp;REPT(" ",MAX(F:F)-F115+1)&amp;B115&amp;" ? "&amp;IF(H115&lt;&gt;"","; "&amp;H115,""))</f>
-        <v xml:space="preserve">layer0_tile_vshift          word ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">layer0_tile_vshift     word ? </v>
       </c>
       <c r="J115" t="str">
         <f>IF(B115&lt;&gt;"", "        public "&amp;VLOOKUP(B115,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A115)&amp;" = "&amp;C115&amp;";"&amp;IF(H115="",""," // "&amp;H115), IF(A115&lt;&gt;"","        // "&amp;A115,""))</f>
@@ -4673,7 +4658,7 @@
         <v>90</v>
       </c>
       <c r="B116" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -4687,16 +4672,16 @@
         <v>284</v>
       </c>
       <c r="F116">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="G116" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I116" t="str">
-        <f>IF(B116="",IF(A116="","","; " &amp;A116),A116&amp;REPT(" ",MAX(F:F)-F116+1)&amp;B116&amp;" ? "&amp;IF(H116&lt;&gt;"","; "&amp;H116,""))</f>
-        <v xml:space="preserve">layer0_map_hshift           word ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">layer0_map_hshift      word ? </v>
       </c>
       <c r="J116" t="str">
         <f>IF(B116&lt;&gt;"", "        public "&amp;VLOOKUP(B116,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A116)&amp;" = "&amp;C116&amp;";"&amp;IF(H116="",""," // "&amp;H116), IF(A116&lt;&gt;"","        // "&amp;A116,""))</f>
@@ -4708,7 +4693,7 @@
         <v>91</v>
       </c>
       <c r="B117" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -4722,16 +4707,16 @@
         <v>286</v>
       </c>
       <c r="F117">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="G117" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I117" t="str">
-        <f>IF(B117="",IF(A117="","","; " &amp;A117),A117&amp;REPT(" ",MAX(F:F)-F117+1)&amp;B117&amp;" ? "&amp;IF(H117&lt;&gt;"","; "&amp;H117,""))</f>
-        <v xml:space="preserve">layer0_map_vshift           word ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">layer0_map_vshift      word ? </v>
       </c>
       <c r="J117" t="str">
         <f>IF(B117&lt;&gt;"", "        public "&amp;VLOOKUP(B117,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A117)&amp;" = "&amp;C117&amp;";"&amp;IF(H117="",""," // "&amp;H117), IF(A117&lt;&gt;"","        // "&amp;A117,""))</f>
@@ -4748,15 +4733,15 @@
         <v>286</v>
       </c>
       <c r="F118">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G118" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I118" t="str">
-        <f>IF(B118="",IF(A118="","","; " &amp;A118),A118&amp;REPT(" ",MAX(F:F)-F118+1)&amp;B118&amp;" ? "&amp;IF(H118&lt;&gt;"","; "&amp;H118,""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J118" t="str">
@@ -4774,15 +4759,15 @@
         <v>286</v>
       </c>
       <c r="F119">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G119" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I119" t="str">
-        <f>IF(B119="",IF(A119="","","; " &amp;A119),A119&amp;REPT(" ",MAX(F:F)-F119+1)&amp;B119&amp;" ? "&amp;IF(H119&lt;&gt;"","; "&amp;H119,""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J119" t="str">
@@ -4792,7 +4777,7 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D120" t="str">
         <f>IF(B120="", "", VLOOKUP(B120,Sheet2!A:B,2,FALSE))</f>
@@ -4803,15 +4788,15 @@
         <v>286</v>
       </c>
       <c r="F120">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="G120" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I120" t="str">
-        <f>IF(B120="",IF(A120="","","; " &amp;A120),A120&amp;REPT(" ",MAX(F:F)-F120+1)&amp;B120&amp;" ? "&amp;IF(H120&lt;&gt;"","; "&amp;H120,""))</f>
+        <f t="shared" si="7"/>
         <v>; Layer 1</v>
       </c>
       <c r="J120" t="str">
@@ -4824,7 +4809,7 @@
         <v>92</v>
       </c>
       <c r="B121" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -4838,16 +4823,16 @@
         <v>288</v>
       </c>
       <c r="F121">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="G121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I121" t="str">
-        <f>IF(B121="",IF(A121="","","; " &amp;A121),A121&amp;REPT(" ",MAX(F:F)-F121+1)&amp;B121&amp;" ? "&amp;IF(H121&lt;&gt;"","; "&amp;H121,""))</f>
-        <v xml:space="preserve">layer1_next_render          word ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">layer1_next_render     word ? </v>
       </c>
       <c r="J121" t="str">
         <f>IF(B121&lt;&gt;"", "        public "&amp;VLOOKUP(B121,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A121)&amp;" = "&amp;C121&amp;";"&amp;IF(H121="",""," // "&amp;H121), IF(A121&lt;&gt;"","        // "&amp;A121,""))</f>
@@ -4859,7 +4844,7 @@
         <v>93</v>
       </c>
       <c r="B122" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -4873,16 +4858,16 @@
         <v>290</v>
       </c>
       <c r="F122">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="G122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I122" t="str">
-        <f>IF(B122="",IF(A122="","","; " &amp;A122),A122&amp;REPT(" ",MAX(F:F)-F122+1)&amp;B122&amp;" ? "&amp;IF(H122&lt;&gt;"","; "&amp;H122,""))</f>
-        <v xml:space="preserve">layer1_tile_hshift          word ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">layer1_tile_hshift     word ? </v>
       </c>
       <c r="J122" t="str">
         <f>IF(B122&lt;&gt;"", "        public "&amp;VLOOKUP(B122,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A122)&amp;" = "&amp;C122&amp;";"&amp;IF(H122="",""," // "&amp;H122), IF(A122&lt;&gt;"","        // "&amp;A122,""))</f>
@@ -4894,7 +4879,7 @@
         <v>94</v>
       </c>
       <c r="B123" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -4908,16 +4893,16 @@
         <v>292</v>
       </c>
       <c r="F123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="G123" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I123" t="str">
-        <f>IF(B123="",IF(A123="","","; " &amp;A123),A123&amp;REPT(" ",MAX(F:F)-F123+1)&amp;B123&amp;" ? "&amp;IF(H123&lt;&gt;"","; "&amp;H123,""))</f>
-        <v xml:space="preserve">layer1_tile_vshift          word ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">layer1_tile_vshift     word ? </v>
       </c>
       <c r="J123" t="str">
         <f>IF(B123&lt;&gt;"", "        public "&amp;VLOOKUP(B123,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A123)&amp;" = "&amp;C123&amp;";"&amp;IF(H123="",""," // "&amp;H123), IF(A123&lt;&gt;"","        // "&amp;A123,""))</f>
@@ -4929,7 +4914,7 @@
         <v>95</v>
       </c>
       <c r="B124" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -4943,16 +4928,16 @@
         <v>294</v>
       </c>
       <c r="F124">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="G124" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I124" t="str">
-        <f>IF(B124="",IF(A124="","","; " &amp;A124),A124&amp;REPT(" ",MAX(F:F)-F124+1)&amp;B124&amp;" ? "&amp;IF(H124&lt;&gt;"","; "&amp;H124,""))</f>
-        <v xml:space="preserve">layer1_map_hshift           word ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">layer1_map_hshift      word ? </v>
       </c>
       <c r="J124" t="str">
         <f>IF(B124&lt;&gt;"", "        public "&amp;VLOOKUP(B124,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A124)&amp;" = "&amp;C124&amp;";"&amp;IF(H124="",""," // "&amp;H124), IF(A124&lt;&gt;"","        // "&amp;A124,""))</f>
@@ -4964,7 +4949,7 @@
         <v>96</v>
       </c>
       <c r="B125" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C125">
         <v>0</v>
@@ -4978,16 +4963,16 @@
         <v>296</v>
       </c>
       <c r="F125">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="G125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I125" t="str">
-        <f>IF(B125="",IF(A125="","","; " &amp;A125),A125&amp;REPT(" ",MAX(F:F)-F125+1)&amp;B125&amp;" ? "&amp;IF(H125&lt;&gt;"","; "&amp;H125,""))</f>
-        <v xml:space="preserve">layer1_map_vshift           word ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">layer1_map_vshift      word ? </v>
       </c>
       <c r="J125" t="str">
         <f>IF(B125&lt;&gt;"", "        public "&amp;VLOOKUP(B125,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A125)&amp;" = "&amp;C125&amp;";"&amp;IF(H125="",""," // "&amp;H125), IF(A125&lt;&gt;"","        // "&amp;A125,""))</f>
@@ -5004,15 +4989,15 @@
         <v>296</v>
       </c>
       <c r="F126">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G126" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I126" t="str">
-        <f>IF(B126="",IF(A126="","","; " &amp;A126),A126&amp;REPT(" ",MAX(F:F)-F126+1)&amp;B126&amp;" ? "&amp;IF(H126&lt;&gt;"","; "&amp;H126,""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J126" t="str">
@@ -5022,7 +5007,7 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D127" t="str">
         <f>IF(B127="", "", VLOOKUP(B127,Sheet2!A:B,2,FALSE))</f>
@@ -5033,15 +5018,15 @@
         <v>296</v>
       </c>
       <c r="F127">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="G127" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I127" t="str">
-        <f>IF(B127="",IF(A127="","","; " &amp;A127),A127&amp;REPT(" ",MAX(F:F)-F127+1)&amp;B127&amp;" ? "&amp;IF(H127&lt;&gt;"","; "&amp;H127,""))</f>
+        <f t="shared" si="7"/>
         <v>; VIA 1</v>
       </c>
       <c r="J127" t="str">
@@ -5054,7 +5039,7 @@
         <v>97</v>
       </c>
       <c r="B128" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C128">
         <v>0</v>
@@ -5068,16 +5053,16 @@
         <v>298</v>
       </c>
       <c r="F128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="G128" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I128" t="str">
-        <f>IF(B128="",IF(A128="","","; " &amp;A128),A128&amp;REPT(" ",MAX(F:F)-F128+1)&amp;B128&amp;" ? "&amp;IF(H128&lt;&gt;"","; "&amp;H128,""))</f>
-        <v xml:space="preserve">via_t1counter_latch         word ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">via_t1counter_latch    word ? </v>
       </c>
       <c r="J128" t="str">
         <f>IF(B128&lt;&gt;"", "        public "&amp;VLOOKUP(B128,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A128)&amp;" = "&amp;C128&amp;";"&amp;IF(H128="",""," // "&amp;H128), IF(A128&lt;&gt;"","        // "&amp;A128,""))</f>
@@ -5089,7 +5074,7 @@
         <v>98</v>
       </c>
       <c r="B129" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C129">
         <v>0</v>
@@ -5103,16 +5088,16 @@
         <v>300</v>
       </c>
       <c r="F129">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="G129" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I129" t="str">
-        <f>IF(B129="",IF(A129="","","; " &amp;A129),A129&amp;REPT(" ",MAX(F:F)-F129+1)&amp;B129&amp;" ? "&amp;IF(H129&lt;&gt;"","; "&amp;H129,""))</f>
-        <v xml:space="preserve">via_t1counter_value         word ? </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">via_t1counter_value    word ? </v>
       </c>
       <c r="J129" t="str">
         <f>IF(B129&lt;&gt;"", "        public "&amp;VLOOKUP(B129,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A129)&amp;" = "&amp;C129&amp;";"&amp;IF(H129="",""," // "&amp;H129), IF(A129&lt;&gt;"","        // "&amp;A129,""))</f>
@@ -5124,7 +5109,7 @@
         <v>99</v>
       </c>
       <c r="B130" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C130">
         <v>0</v>
@@ -5138,16 +5123,16 @@
         <v>302</v>
       </c>
       <c r="F130">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="G130" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I130" t="str">
-        <f>IF(B130="",IF(A130="","","; " &amp;A130),A130&amp;REPT(" ",MAX(F:F)-F130+1)&amp;B130&amp;" ? "&amp;IF(H130&lt;&gt;"","; "&amp;H130,""))</f>
-        <v xml:space="preserve">via_t2counter_latch         word ? </v>
+        <f t="shared" ref="I130:I153" si="10">IF(B130="",IF(A130="","","; " &amp;A130),A130&amp;REPT(" ",MAX(F:F)-F130+1)&amp;B130&amp;" ? "&amp;IF(H130&lt;&gt;"","; "&amp;H130,""))</f>
+        <v xml:space="preserve">via_t2counter_latch    word ? </v>
       </c>
       <c r="J130" t="str">
         <f>IF(B130&lt;&gt;"", "        public "&amp;VLOOKUP(B130,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A130)&amp;" = "&amp;C130&amp;";"&amp;IF(H130="",""," // "&amp;H130), IF(A130&lt;&gt;"","        // "&amp;A130,""))</f>
@@ -5159,7 +5144,7 @@
         <v>100</v>
       </c>
       <c r="B131" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C131">
         <v>0</v>
@@ -5173,16 +5158,16 @@
         <v>304</v>
       </c>
       <c r="F131">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="G131" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I131" t="str">
-        <f>IF(B131="",IF(A131="","","; " &amp;A131),A131&amp;REPT(" ",MAX(F:F)-F131+1)&amp;B131&amp;" ? "&amp;IF(H131&lt;&gt;"","; "&amp;H131,""))</f>
-        <v xml:space="preserve">via_t2counter_value         word ? </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">via_t2counter_value    word ? </v>
       </c>
       <c r="J131" t="str">
         <f>IF(B131&lt;&gt;"", "        public "&amp;VLOOKUP(B131,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A131)&amp;" = "&amp;C131&amp;";"&amp;IF(H131="",""," // "&amp;H131), IF(A131&lt;&gt;"","        // "&amp;A131,""))</f>
@@ -5199,15 +5184,15 @@
         <v>304</v>
       </c>
       <c r="F132">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G132" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I132" t="str">
-        <f>IF(B132="",IF(A132="","","; " &amp;A132),A132&amp;REPT(" ",MAX(F:F)-F132+1)&amp;B132&amp;" ? "&amp;IF(H132&lt;&gt;"","; "&amp;H132,""))</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="J132" t="str">
@@ -5217,10 +5202,10 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>101</v>
+        <v>140</v>
       </c>
       <c r="B133" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -5234,28 +5219,28 @@
         <v>305</v>
       </c>
       <c r="F133">
-        <f t="shared" si="2"/>
-        <v>20</v>
+        <f t="shared" si="8"/>
+        <v>18</v>
       </c>
       <c r="G133" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I133" t="str">
-        <f>IF(B133="",IF(A133="","","; " &amp;A133),A133&amp;REPT(" ",MAX(F:F)-F133+1)&amp;B133&amp;" ? "&amp;IF(H133&lt;&gt;"","; "&amp;H133,""))</f>
-        <v xml:space="preserve">via_interrupt_timer1        byte ? </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">register_a_outdata     byte ? </v>
       </c>
       <c r="J133" t="str">
         <f>IF(B133&lt;&gt;"", "        public "&amp;VLOOKUP(B133,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A133)&amp;" = "&amp;C133&amp;";"&amp;IF(H133="",""," // "&amp;H133), IF(A133&lt;&gt;"","        // "&amp;A133,""))</f>
-        <v xml:space="preserve">        public byte Via_Interrupt_Timer1 = 0;</v>
+        <v xml:space="preserve">        public byte Register_A_Outdata = 0;</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>102</v>
+        <v>139</v>
       </c>
       <c r="B134" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -5269,195 +5254,165 @@
         <v>306</v>
       </c>
       <c r="F134">
-        <f t="shared" si="2"/>
-        <v>20</v>
+        <f t="shared" si="8"/>
+        <v>17</v>
       </c>
       <c r="G134" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I134" t="str">
-        <f>IF(B134="",IF(A134="","","; " &amp;A134),A134&amp;REPT(" ",MAX(F:F)-F134+1)&amp;B134&amp;" ? "&amp;IF(H134&lt;&gt;"","; "&amp;H134,""))</f>
-        <v xml:space="preserve">via_interrupt_timer2        byte ? </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">register_a_indata      byte ? </v>
       </c>
       <c r="J134" t="str">
         <f>IF(B134&lt;&gt;"", "        public "&amp;VLOOKUP(B134,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A134)&amp;" = "&amp;C134&amp;";"&amp;IF(H134="",""," // "&amp;H134), IF(A134&lt;&gt;"","        // "&amp;A134,""))</f>
-        <v xml:space="preserve">        public byte Via_Interrupt_Timer2 = 0;</v>
+        <v xml:space="preserve">        public byte Register_A_Indata = 0;</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>103</v>
-      </c>
-      <c r="B135" t="s">
-        <v>121</v>
-      </c>
       <c r="C135">
         <v>0</v>
       </c>
-      <c r="D135">
+      <c r="D135" t="str">
         <f>IF(B135="", "", VLOOKUP(B135,Sheet2!A:B,2,FALSE))</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="E135">
         <f>IF(B135="",E134,VLOOKUP(B135,Sheet2!A:B,2,FALSE)+E134)</f>
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F135">
-        <f t="shared" si="2"/>
-        <v>17</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="G135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I135" t="str">
-        <f>IF(B135="",IF(A135="","","; " &amp;A135),A135&amp;REPT(" ",MAX(F:F)-F135+1)&amp;B135&amp;" ? "&amp;IF(H135&lt;&gt;"","; "&amp;H135,""))</f>
-        <v xml:space="preserve">via_interrupt_cb1           byte ? </v>
+        <f t="shared" si="10"/>
+        <v/>
       </c>
       <c r="J135" t="str">
         <f>IF(B135&lt;&gt;"", "        public "&amp;VLOOKUP(B135,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A135)&amp;" = "&amp;C135&amp;";"&amp;IF(H135="",""," // "&amp;H135), IF(A135&lt;&gt;"","        // "&amp;A135,""))</f>
-        <v xml:space="preserve">        public byte Via_Interrupt_Cb1 = 0;</v>
+        <v/>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>104</v>
-      </c>
-      <c r="B136" t="s">
-        <v>121</v>
-      </c>
       <c r="C136">
         <v>0</v>
       </c>
-      <c r="D136">
+      <c r="D136" t="str">
         <f>IF(B136="", "", VLOOKUP(B136,Sheet2!A:B,2,FALSE))</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="E136">
         <f>IF(B136="",E135,VLOOKUP(B136,Sheet2!A:B,2,FALSE)+E135)</f>
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F136">
-        <f t="shared" si="2"/>
-        <v>17</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="G136" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I136" t="str">
-        <f>IF(B136="",IF(A136="","","; " &amp;A136),A136&amp;REPT(" ",MAX(F:F)-F136+1)&amp;B136&amp;" ? "&amp;IF(H136&lt;&gt;"","; "&amp;H136,""))</f>
-        <v xml:space="preserve">via_interrupt_cb2           byte ? </v>
+        <f t="shared" si="10"/>
+        <v/>
       </c>
       <c r="J136" t="str">
         <f>IF(B136&lt;&gt;"", "        public "&amp;VLOOKUP(B136,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A136)&amp;" = "&amp;C136&amp;";"&amp;IF(H136="",""," // "&amp;H136), IF(A136&lt;&gt;"","        // "&amp;A136,""))</f>
-        <v xml:space="preserve">        public byte Via_Interrupt_Cb2 = 0;</v>
+        <v/>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>105</v>
-      </c>
-      <c r="B137" t="s">
-        <v>121</v>
-      </c>
       <c r="C137">
         <v>0</v>
       </c>
-      <c r="D137">
+      <c r="D137" t="str">
         <f>IF(B137="", "", VLOOKUP(B137,Sheet2!A:B,2,FALSE))</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="E137">
         <f>IF(B137="",E136,VLOOKUP(B137,Sheet2!A:B,2,FALSE)+E136)</f>
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="F137">
-        <f t="shared" si="2"/>
-        <v>27</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="G137" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I137" t="str">
-        <f>IF(B137="",IF(A137="","","; " &amp;A137),A137&amp;REPT(" ",MAX(F:F)-F137+1)&amp;B137&amp;" ? "&amp;IF(H137&lt;&gt;"","; "&amp;H137,""))</f>
-        <v xml:space="preserve">via_interrupt_shiftregister byte ? </v>
+        <f t="shared" si="10"/>
+        <v/>
       </c>
       <c r="J137" t="str">
         <f>IF(B137&lt;&gt;"", "        public "&amp;VLOOKUP(B137,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A137)&amp;" = "&amp;C137&amp;";"&amp;IF(H137="",""," // "&amp;H137), IF(A137&lt;&gt;"","        // "&amp;A137,""))</f>
-        <v xml:space="preserve">        public byte Via_Interrupt_Shiftregister = 0;</v>
+        <v/>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>106</v>
-      </c>
-      <c r="B138" t="s">
-        <v>121</v>
-      </c>
       <c r="C138">
         <v>0</v>
       </c>
-      <c r="D138">
+      <c r="D138" t="str">
         <f>IF(B138="", "", VLOOKUP(B138,Sheet2!A:B,2,FALSE))</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="E138">
         <f>IF(B138="",E137,VLOOKUP(B138,Sheet2!A:B,2,FALSE)+E137)</f>
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F138">
-        <f t="shared" si="2"/>
-        <v>17</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="G138" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I138" t="str">
-        <f>IF(B138="",IF(A138="","","; " &amp;A138),A138&amp;REPT(" ",MAX(F:F)-F138+1)&amp;B138&amp;" ? "&amp;IF(H138&lt;&gt;"","; "&amp;H138,""))</f>
-        <v xml:space="preserve">via_interrupt_ca1           byte ? </v>
+        <f t="shared" si="10"/>
+        <v/>
       </c>
       <c r="J138" t="str">
         <f>IF(B138&lt;&gt;"", "        public "&amp;VLOOKUP(B138,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A138)&amp;" = "&amp;C138&amp;";"&amp;IF(H138="",""," // "&amp;H138), IF(A138&lt;&gt;"","        // "&amp;A138,""))</f>
-        <v xml:space="preserve">        public byte Via_Interrupt_Ca1 = 0;</v>
+        <v/>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>107</v>
-      </c>
-      <c r="B139" t="s">
-        <v>121</v>
-      </c>
       <c r="C139">
         <v>0</v>
       </c>
-      <c r="D139">
+      <c r="D139" t="str">
         <f>IF(B139="", "", VLOOKUP(B139,Sheet2!A:B,2,FALSE))</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="E139">
         <f>IF(B139="",E138,VLOOKUP(B139,Sheet2!A:B,2,FALSE)+E138)</f>
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="F139">
-        <f t="shared" si="2"/>
-        <v>17</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="G139" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I139" t="str">
-        <f>IF(B139="",IF(A139="","","; " &amp;A139),A139&amp;REPT(" ",MAX(F:F)-F139+1)&amp;B139&amp;" ? "&amp;IF(H139&lt;&gt;"","; "&amp;H139,""))</f>
-        <v xml:space="preserve">via_interrupt_ca2           byte ? </v>
+        <f t="shared" si="10"/>
+        <v/>
       </c>
       <c r="J139" t="str">
         <f>IF(B139&lt;&gt;"", "        public "&amp;VLOOKUP(B139,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A139)&amp;" = "&amp;C139&amp;";"&amp;IF(H139="",""," // "&amp;H139), IF(A139&lt;&gt;"","        // "&amp;A139,""))</f>
-        <v xml:space="preserve">        public byte Via_Interrupt_Ca2 = 0;</v>
+        <v/>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
@@ -5467,18 +5422,18 @@
       </c>
       <c r="E140">
         <f>IF(B140="",E139,VLOOKUP(B140,Sheet2!A:B,2,FALSE)+E139)</f>
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="F140">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G140" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I140" t="str">
-        <f>IF(B140="",IF(A140="","","; " &amp;A140),A140&amp;REPT(" ",MAX(F:F)-F140+1)&amp;B140&amp;" ? "&amp;IF(H140&lt;&gt;"","; "&amp;H140,""))</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="J140" t="str">
@@ -5488,10 +5443,10 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B141" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C141">
         <v>0</v>
@@ -5502,19 +5457,19 @@
       </c>
       <c r="E141">
         <f>IF(B141="",E140,VLOOKUP(B141,Sheet2!A:B,2,FALSE)+E140)</f>
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="F141">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="G141" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I141" t="str">
-        <f>IF(B141="",IF(A141="","","; " &amp;A141),A141&amp;REPT(" ",MAX(F:F)-F141+1)&amp;B141&amp;" ? "&amp;IF(H141&lt;&gt;"","; "&amp;H141,""))</f>
-        <v xml:space="preserve">via_timer1_continuous       byte ? </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">via_timer1_continuous  byte ? </v>
       </c>
       <c r="J141" t="str">
         <f>IF(B141&lt;&gt;"", "        public "&amp;VLOOKUP(B141,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A141)&amp;" = "&amp;C141&amp;";"&amp;IF(H141="",""," // "&amp;H141), IF(A141&lt;&gt;"","        // "&amp;A141,""))</f>
@@ -5523,10 +5478,10 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B142" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C142">
         <v>0</v>
@@ -5537,19 +5492,19 @@
       </c>
       <c r="E142">
         <f>IF(B142="",E141,VLOOKUP(B142,Sheet2!A:B,2,FALSE)+E141)</f>
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="F142">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="G142" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I142" t="str">
-        <f>IF(B142="",IF(A142="","","; " &amp;A142),A142&amp;REPT(" ",MAX(F:F)-F142+1)&amp;B142&amp;" ? "&amp;IF(H142&lt;&gt;"","; "&amp;H142,""))</f>
-        <v xml:space="preserve">via_timer1_pb7              byte ? </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">via_timer1_pb7         byte ? </v>
       </c>
       <c r="J142" t="str">
         <f>IF(B142&lt;&gt;"", "        public "&amp;VLOOKUP(B142,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A142)&amp;" = "&amp;C142&amp;";"&amp;IF(H142="",""," // "&amp;H142), IF(A142&lt;&gt;"","        // "&amp;A142,""))</f>
@@ -5558,10 +5513,10 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B143" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C143">
         <v>0</v>
@@ -5572,19 +5527,19 @@
       </c>
       <c r="E143">
         <f>IF(B143="",E142,VLOOKUP(B143,Sheet2!A:B,2,FALSE)+E142)</f>
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="F143">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="G143" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I143" t="str">
-        <f>IF(B143="",IF(A143="","","; " &amp;A143),A143&amp;REPT(" ",MAX(F:F)-F143+1)&amp;B143&amp;" ? "&amp;IF(H143&lt;&gt;"","; "&amp;H143,""))</f>
-        <v xml:space="preserve">via_timer1_running          byte ? </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">via_timer1_running     byte ? </v>
       </c>
       <c r="J143" t="str">
         <f>IF(B143&lt;&gt;"", "        public "&amp;VLOOKUP(B143,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A143)&amp;" = "&amp;C143&amp;";"&amp;IF(H143="",""," // "&amp;H143), IF(A143&lt;&gt;"","        // "&amp;A143,""))</f>
@@ -5598,18 +5553,18 @@
       </c>
       <c r="E144">
         <f>IF(B144="",E143,VLOOKUP(B144,Sheet2!A:B,2,FALSE)+E143)</f>
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="F144">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G144" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I144" t="str">
-        <f>IF(B144="",IF(A144="","","; " &amp;A144),A144&amp;REPT(" ",MAX(F:F)-F144+1)&amp;B144&amp;" ? "&amp;IF(H144&lt;&gt;"","; "&amp;H144,""))</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="J144" t="str">
@@ -5619,10 +5574,10 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B145" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C145">
         <v>0</v>
@@ -5633,19 +5588,19 @@
       </c>
       <c r="E145">
         <f>IF(B145="",E144,VLOOKUP(B145,Sheet2!A:B,2,FALSE)+E144)</f>
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F145">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="G145" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I145" t="str">
-        <f>IF(B145="",IF(A145="","","; " &amp;A145),A145&amp;REPT(" ",MAX(F:F)-F145+1)&amp;B145&amp;" ? "&amp;IF(H145&lt;&gt;"","; "&amp;H145,""))</f>
-        <v xml:space="preserve">via_timer2_pulsecount       byte ? </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">via_timer2_pulsecount  byte ? </v>
       </c>
       <c r="J145" t="str">
         <f>IF(B145&lt;&gt;"", "        public "&amp;VLOOKUP(B145,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A145)&amp;" = "&amp;C145&amp;";"&amp;IF(H145="",""," // "&amp;H145), IF(A145&lt;&gt;"","        // "&amp;A145,""))</f>
@@ -5654,10 +5609,10 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B146" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C146">
         <v>0</v>
@@ -5668,19 +5623,19 @@
       </c>
       <c r="E146">
         <f>IF(B146="",E145,VLOOKUP(B146,Sheet2!A:B,2,FALSE)+E145)</f>
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="F146">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="G146" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I146" t="str">
-        <f>IF(B146="",IF(A146="","","; " &amp;A146),A146&amp;REPT(" ",MAX(F:F)-F146+1)&amp;B146&amp;" ? "&amp;IF(H146&lt;&gt;"","; "&amp;H146,""))</f>
-        <v xml:space="preserve">via_timer2_running          byte ? </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">via_timer2_running     byte ? </v>
       </c>
       <c r="J146" t="str">
         <f>IF(B146&lt;&gt;"", "        public "&amp;VLOOKUP(B146,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A146)&amp;" = "&amp;C146&amp;";"&amp;IF(H146="",""," // "&amp;H146), IF(A146&lt;&gt;"","        // "&amp;A146,""))</f>
@@ -5694,18 +5649,18 @@
       </c>
       <c r="E147">
         <f>IF(B147="",E146,VLOOKUP(B147,Sheet2!A:B,2,FALSE)+E146)</f>
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="F147">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G147" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I147" t="str">
-        <f>IF(B147="",IF(A147="","","; " &amp;A147),A147&amp;REPT(" ",MAX(F:F)-F147+1)&amp;B147&amp;" ? "&amp;IF(H147&lt;&gt;"","; "&amp;H147,""))</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="J147" t="str">
@@ -5715,7 +5670,7 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D148" t="str">
         <f>IF(B148="", "", VLOOKUP(B148,Sheet2!A:B,2,FALSE))</f>
@@ -5723,18 +5678,18 @@
       </c>
       <c r="E148">
         <f>IF(B148="",E147,VLOOKUP(B148,Sheet2!A:B,2,FALSE)+E147)</f>
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="F148">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="G148" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I148" t="str">
-        <f>IF(B148="",IF(A148="","","; " &amp;A148),A148&amp;REPT(" ",MAX(F:F)-F148+1)&amp;B148&amp;" ? "&amp;IF(H148&lt;&gt;"","; "&amp;H148,""))</f>
+        <f t="shared" si="10"/>
         <v>; L2C</v>
       </c>
       <c r="J148" t="str">
@@ -5744,10 +5699,10 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
+        <v>106</v>
+      </c>
+      <c r="B149" t="s">
         <v>113</v>
-      </c>
-      <c r="B149" t="s">
-        <v>120</v>
       </c>
       <c r="C149">
         <v>0</v>
@@ -5758,22 +5713,22 @@
       </c>
       <c r="E149">
         <f>IF(B149="",E148,VLOOKUP(B149,Sheet2!A:B,2,FALSE)+E148)</f>
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="F149">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="G149" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <f t="shared" si="9"/>
+        <v>ERROR</v>
       </c>
       <c r="H149" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="I149" t="str">
-        <f>IF(B149="",IF(A149="","","; " &amp;A149),A149&amp;REPT(" ",MAX(F:F)-F149+1)&amp;B149&amp;" ? "&amp;IF(H149&lt;&gt;"","; "&amp;H149,""))</f>
-        <v>i2c_address                 word ? ; 7 bit address of destination</v>
+        <f t="shared" si="10"/>
+        <v>i2c_address            word ? ; 7 bit address of destination</v>
       </c>
       <c r="J149" t="str">
         <f>IF(B149&lt;&gt;"", "        public "&amp;VLOOKUP(B149,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A149)&amp;" = "&amp;C149&amp;";"&amp;IF(H149="",""," // "&amp;H149), IF(A149&lt;&gt;"","        // "&amp;A149,""))</f>
@@ -5782,10 +5737,10 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
+        <v>107</v>
+      </c>
+      <c r="B150" t="s">
         <v>114</v>
-      </c>
-      <c r="B150" t="s">
-        <v>121</v>
       </c>
       <c r="C150">
         <v>0</v>
@@ -5796,22 +5751,22 @@
       </c>
       <c r="E150">
         <f>IF(B150="",E149,VLOOKUP(B150,Sheet2!A:B,2,FALSE)+E149)</f>
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="F150">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="G150" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="H150" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="I150" t="str">
-        <f>IF(B150="",IF(A150="","","; " &amp;A150),A150&amp;REPT(" ",MAX(F:F)-F150+1)&amp;B150&amp;" ? "&amp;IF(H150&lt;&gt;"","; "&amp;H150,""))</f>
-        <v>i2c_state                   byte ? ; enum of where we are in the message</v>
+        <f t="shared" si="10"/>
+        <v>i2c_state              byte ? ; enum of where we are in the message</v>
       </c>
       <c r="J150" t="str">
         <f>IF(B150&lt;&gt;"", "        public "&amp;VLOOKUP(B150,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A150)&amp;" = "&amp;C150&amp;";"&amp;IF(H150="",""," // "&amp;H150), IF(A150&lt;&gt;"","        // "&amp;A150,""))</f>
@@ -5820,10 +5775,10 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B151" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C151">
         <v>0</v>
@@ -5834,19 +5789,19 @@
       </c>
       <c r="E151">
         <f>IF(B151="",E150,VLOOKUP(B151,Sheet2!A:B,2,FALSE)+E150)</f>
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F151">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="G151" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I151" t="str">
-        <f>IF(B151="",IF(A151="","","; " &amp;A151),A151&amp;REPT(" ",MAX(F:F)-F151+1)&amp;B151&amp;" ? "&amp;IF(H151&lt;&gt;"","; "&amp;H151,""))</f>
-        <v xml:space="preserve">i2c_sending                 byte ? </v>
+        <f t="shared" si="10"/>
+        <v xml:space="preserve">i2c_sending            byte ? </v>
       </c>
       <c r="J151" t="str">
         <f>IF(B151&lt;&gt;"", "        public "&amp;VLOOKUP(B151,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A151)&amp;" = "&amp;C151&amp;";"&amp;IF(H151="",""," // "&amp;H151), IF(A151&lt;&gt;"","        // "&amp;A151,""))</f>
@@ -5855,10 +5810,10 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B152" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C152">
         <v>0</v>
@@ -5869,22 +5824,22 @@
       </c>
       <c r="E152">
         <f>IF(B152="",E151,VLOOKUP(B152,Sheet2!A:B,2,FALSE)+E151)</f>
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="F152">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="G152" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="H152" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="I152" t="str">
-        <f>IF(B152="",IF(A152="","","; " &amp;A152),A152&amp;REPT(" ",MAX(F:F)-F152+1)&amp;B152&amp;" ? "&amp;IF(H152&lt;&gt;"","; "&amp;H152,""))</f>
-        <v>i2c_data                    byte ? ; data that is being transmitted</v>
+        <f t="shared" si="10"/>
+        <v>i2c_data               byte ? ; data that is being transmitted</v>
       </c>
       <c r="J152" t="str">
         <f>IF(B152&lt;&gt;"", "        public "&amp;VLOOKUP(B152,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A152)&amp;" = "&amp;C152&amp;";"&amp;IF(H152="",""," // "&amp;H152), IF(A152&lt;&gt;"","        // "&amp;A152,""))</f>
@@ -5893,10 +5848,10 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B153" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C153">
         <v>0</v>
@@ -5907,22 +5862,22 @@
       </c>
       <c r="E153">
         <f>IF(B153="",E152,VLOOKUP(B153,Sheet2!A:B,2,FALSE)+E152)</f>
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="F153">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="G153" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="H153" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="I153" t="str">
-        <f>IF(B153="",IF(A153="","","; " &amp;A153),A153&amp;REPT(" ",MAX(F:F)-F153+1)&amp;B153&amp;" ? "&amp;IF(H153&lt;&gt;"","; "&amp;H153,""))</f>
-        <v>i2c_pos                     byte ? ; position in that data</v>
+        <f t="shared" si="10"/>
+        <v>i2c_pos                byte ? ; position in that data</v>
       </c>
       <c r="J153" t="str">
         <f>IF(B153&lt;&gt;"", "        public "&amp;VLOOKUP(B153,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A153)&amp;" = "&amp;C153&amp;";"&amp;IF(H153="",""," // "&amp;H153), IF(A153&lt;&gt;"","        // "&amp;A153,""))</f>
@@ -5947,46 +5902,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B1">
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B2">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds rw handling to VIA, and doesn't redraw the screen if nothing has changed
</commit_message>
<xml_diff>
--- a/BitMagic.X16Emulator/state_object.xlsx
+++ b/BitMagic.X16Emulator/state_object.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Source\BitMagic\BitMagic.X16Emulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE2C78F-4B6A-422D-9346-BF9B1BA40333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D140FA-4844-41E9-83C3-E2299EC4BA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{E785A1AE-7179-42D9-8B33-8945211A7A0B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="143">
   <si>
     <t>memory_ptr</t>
   </si>
@@ -458,6 +458,12 @@
   </si>
   <si>
     <t>register_a_outdata</t>
+  </si>
+  <si>
+    <t>dirty</t>
+  </si>
+  <si>
+    <t>rendering_spacing</t>
   </si>
 </sst>
 </file>
@@ -818,20 +824,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{102E5AB3-C033-4619-AF24-70A987B6E98D}">
-  <dimension ref="A1:J153"/>
+  <dimension ref="A1:J157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A134" sqref="A134"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.140625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="9.140625" customWidth="1"/>
     <col min="8" max="8" width="67" customWidth="1"/>
     <col min="9" max="9" width="70.42578125" customWidth="1"/>
     <col min="10" max="10" width="69.140625" bestFit="1" customWidth="1"/>
@@ -894,7 +898,7 @@
         <v/>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I33" si="2">IF(B2="",IF(A2="","","; " &amp;A2),A2&amp;REPT(" ",MAX(F:F)-F2+1)&amp;B2&amp;" ? "&amp;IF(H2&lt;&gt;"","; "&amp;H2,""))</f>
+        <f>IF(B2="",IF(A2="","","; " &amp;A2),A2&amp;REPT(" ",MAX(F:F)-F2+1)&amp;B2&amp;" ? "&amp;IF(H2&lt;&gt;"","; "&amp;H2,""))</f>
         <v xml:space="preserve">memory_ptr             qword ? </v>
       </c>
       <c r="J2" t="str">
@@ -929,7 +933,7 @@
         <v/>
       </c>
       <c r="I3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B3="",IF(A3="","","; " &amp;A3),A3&amp;REPT(" ",MAX(F:F)-F3+1)&amp;B3&amp;" ? "&amp;IF(H3&lt;&gt;"","; "&amp;H3,""))</f>
         <v xml:space="preserve">rom_ptr                qword ? </v>
       </c>
       <c r="J3" t="str">
@@ -964,7 +968,7 @@
         <v/>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B4="",IF(A4="","","; " &amp;A4),A4&amp;REPT(" ",MAX(F:F)-F4+1)&amp;B4&amp;" ? "&amp;IF(H4&lt;&gt;"","; "&amp;H4,""))</f>
         <v xml:space="preserve">rambank_ptr            qword ? </v>
       </c>
       <c r="J4" t="str">
@@ -999,7 +1003,7 @@
         <v/>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B5="",IF(A5="","","; " &amp;A5),A5&amp;REPT(" ",MAX(F:F)-F5+1)&amp;B5&amp;" ? "&amp;IF(H5&lt;&gt;"","; "&amp;H5,""))</f>
         <v xml:space="preserve">display_ptr            qword ? </v>
       </c>
       <c r="J5" t="str">
@@ -1034,7 +1038,7 @@
         <v/>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B6="",IF(A6="","","; " &amp;A6),A6&amp;REPT(" ",MAX(F:F)-F6+1)&amp;B6&amp;" ? "&amp;IF(H6&lt;&gt;"","; "&amp;H6,""))</f>
         <v xml:space="preserve">display_buffer_ptr     qword ? </v>
       </c>
       <c r="J6" t="str">
@@ -1069,7 +1073,7 @@
         <v/>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B7="",IF(A7="","","; " &amp;A7),A7&amp;REPT(" ",MAX(F:F)-F7+1)&amp;B7&amp;" ? "&amp;IF(H7&lt;&gt;"","; "&amp;H7,""))</f>
         <v xml:space="preserve">history_ptr            qword ? </v>
       </c>
       <c r="J7" t="str">
@@ -1095,7 +1099,7 @@
         <v/>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B8="",IF(A8="","","; " &amp;A8),A8&amp;REPT(" ",MAX(F:F)-F8+1)&amp;B8&amp;" ? "&amp;IF(H8&lt;&gt;"","; "&amp;H8,""))</f>
         <v/>
       </c>
       <c r="J8" t="str">
@@ -1124,7 +1128,7 @@
         <v/>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B9="",IF(A9="","","; " &amp;A9),A9&amp;REPT(" ",MAX(F:F)-F9+1)&amp;B9&amp;" ? "&amp;IF(H9&lt;&gt;"","; "&amp;H9,""))</f>
         <v>; Vera</v>
       </c>
       <c r="J9" t="str">
@@ -1159,7 +1163,7 @@
         <v/>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B10="",IF(A10="","","; " &amp;A10),A10&amp;REPT(" ",MAX(F:F)-F10+1)&amp;B10&amp;" ? "&amp;IF(H10&lt;&gt;"","; "&amp;H10,""))</f>
         <v xml:space="preserve">vram_ptr               qword ? </v>
       </c>
       <c r="J10" t="str">
@@ -1194,7 +1198,7 @@
         <v/>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B11="",IF(A11="","","; " &amp;A11),A11&amp;REPT(" ",MAX(F:F)-F11+1)&amp;B11&amp;" ? "&amp;IF(H11&lt;&gt;"","; "&amp;H11,""))</f>
         <v xml:space="preserve">palette_ptr            qword ? </v>
       </c>
       <c r="J11" t="str">
@@ -1220,7 +1224,7 @@
         <v/>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B12="",IF(A12="","","; " &amp;A12),A12&amp;REPT(" ",MAX(F:F)-F12+1)&amp;B12&amp;" ? "&amp;IF(H12&lt;&gt;"","; "&amp;H12,""))</f>
         <v/>
       </c>
       <c r="J12" t="str">
@@ -1255,7 +1259,7 @@
         <v/>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B13="",IF(A13="","","; " &amp;A13),A13&amp;REPT(" ",MAX(F:F)-F13+1)&amp;B13&amp;" ? "&amp;IF(H13&lt;&gt;"","; "&amp;H13,""))</f>
         <v xml:space="preserve">data0_address          qword ? </v>
       </c>
       <c r="J13" t="str">
@@ -1290,7 +1294,7 @@
         <v/>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B14="",IF(A14="","","; " &amp;A14),A14&amp;REPT(" ",MAX(F:F)-F14+1)&amp;B14&amp;" ? "&amp;IF(H14&lt;&gt;"","; "&amp;H14,""))</f>
         <v xml:space="preserve">data1_address          qword ? </v>
       </c>
       <c r="J14" t="str">
@@ -1325,7 +1329,7 @@
         <v/>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B15="",IF(A15="","","; " &amp;A15),A15&amp;REPT(" ",MAX(F:F)-F15+1)&amp;B15&amp;" ? "&amp;IF(H15&lt;&gt;"","; "&amp;H15,""))</f>
         <v xml:space="preserve">data0_step             qword ? </v>
       </c>
       <c r="J15" t="str">
@@ -1360,7 +1364,7 @@
         <v/>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B16="",IF(A16="","","; " &amp;A16),A16&amp;REPT(" ",MAX(F:F)-F16+1)&amp;B16&amp;" ? "&amp;IF(H16&lt;&gt;"","; "&amp;H16,""))</f>
         <v xml:space="preserve">data1_step             qword ? </v>
       </c>
       <c r="J16" t="str">
@@ -1386,7 +1390,7 @@
         <v/>
       </c>
       <c r="I17" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B17="",IF(A17="","","; " &amp;A17),A17&amp;REPT(" ",MAX(F:F)-F17+1)&amp;B17&amp;" ? "&amp;IF(H17&lt;&gt;"","; "&amp;H17,""))</f>
         <v/>
       </c>
       <c r="J17" t="str">
@@ -1421,7 +1425,7 @@
         <v/>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B18="",IF(A18="","","; " &amp;A18),A18&amp;REPT(" ",MAX(F:F)-F18+1)&amp;B18&amp;" ? "&amp;IF(H18&lt;&gt;"","; "&amp;H18,""))</f>
         <v xml:space="preserve">clock_previous         qword ? </v>
       </c>
       <c r="J18" t="str">
@@ -1456,7 +1460,7 @@
         <v/>
       </c>
       <c r="I19" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B19="",IF(A19="","","; " &amp;A19),A19&amp;REPT(" ",MAX(F:F)-F19+1)&amp;B19&amp;" ? "&amp;IF(H19&lt;&gt;"","; "&amp;H19,""))</f>
         <v xml:space="preserve">clock                  qword ? </v>
       </c>
       <c r="J19" t="str">
@@ -1491,7 +1495,7 @@
         <v/>
       </c>
       <c r="I20" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B20="",IF(A20="","","; " &amp;A20),A20&amp;REPT(" ",MAX(F:F)-F20+1)&amp;B20&amp;" ? "&amp;IF(H20&lt;&gt;"","; "&amp;H20,""))</f>
         <v xml:space="preserve">vera_clock             qword ? </v>
       </c>
       <c r="J20" t="str">
@@ -1517,7 +1521,7 @@
         <v/>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B21="",IF(A21="","","; " &amp;A21),A21&amp;REPT(" ",MAX(F:F)-F21+1)&amp;B21&amp;" ? "&amp;IF(H21&lt;&gt;"","; "&amp;H21,""))</f>
         <v/>
       </c>
       <c r="J21" t="str">
@@ -1552,7 +1556,7 @@
         <v/>
       </c>
       <c r="I22" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B22="",IF(A22="","","; " &amp;A22),A22&amp;REPT(" ",MAX(F:F)-F22+1)&amp;B22&amp;" ? "&amp;IF(H22&lt;&gt;"","; "&amp;H22,""))</f>
         <v xml:space="preserve">history_pos            qword ? </v>
       </c>
       <c r="J22" t="str">
@@ -1578,7 +1582,7 @@
         <v/>
       </c>
       <c r="I23" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B23="",IF(A23="","","; " &amp;A23),A23&amp;REPT(" ",MAX(F:F)-F23+1)&amp;B23&amp;" ? "&amp;IF(H23&lt;&gt;"","; "&amp;H23,""))</f>
         <v/>
       </c>
       <c r="J23" t="str">
@@ -1613,7 +1617,7 @@
         <v/>
       </c>
       <c r="I24" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B24="",IF(A24="","","; " &amp;A24),A24&amp;REPT(" ",MAX(F:F)-F24+1)&amp;B24&amp;" ? "&amp;IF(H24&lt;&gt;"","; "&amp;H24,""))</f>
         <v xml:space="preserve">layer0_jmp             qword ? </v>
       </c>
       <c r="J24" t="str">
@@ -1648,7 +1652,7 @@
         <v/>
       </c>
       <c r="I25" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B25="",IF(A25="","","; " &amp;A25),A25&amp;REPT(" ",MAX(F:F)-F25+1)&amp;B25&amp;" ? "&amp;IF(H25&lt;&gt;"","; "&amp;H25,""))</f>
         <v xml:space="preserve">layer0_rtn             qword ? </v>
       </c>
       <c r="J25" t="str">
@@ -1683,7 +1687,7 @@
         <v/>
       </c>
       <c r="I26" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B26="",IF(A26="","","; " &amp;A26),A26&amp;REPT(" ",MAX(F:F)-F26+1)&amp;B26&amp;" ? "&amp;IF(H26&lt;&gt;"","; "&amp;H26,""))</f>
         <v xml:space="preserve">layer1_jmp             qword ? </v>
       </c>
       <c r="J26" t="str">
@@ -1718,7 +1722,7 @@
         <v/>
       </c>
       <c r="I27" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B27="",IF(A27="","","; " &amp;A27),A27&amp;REPT(" ",MAX(F:F)-F27+1)&amp;B27&amp;" ? "&amp;IF(H27&lt;&gt;"","; "&amp;H27,""))</f>
         <v xml:space="preserve">layer1_rtn             qword ? </v>
       </c>
       <c r="J27" t="str">
@@ -1744,7 +1748,7 @@
         <v/>
       </c>
       <c r="I28" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B28="",IF(A28="","","; " &amp;A28),A28&amp;REPT(" ",MAX(F:F)-F28+1)&amp;B28&amp;" ? "&amp;IF(H28&lt;&gt;"","; "&amp;H28,""))</f>
         <v/>
       </c>
       <c r="J28" t="str">
@@ -1779,7 +1783,7 @@
         <v/>
       </c>
       <c r="I29" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B29="",IF(A29="","","; " &amp;A29),A29&amp;REPT(" ",MAX(F:F)-F29+1)&amp;B29&amp;" ? "&amp;IF(H29&lt;&gt;"","; "&amp;H29,""))</f>
         <v xml:space="preserve">dc_hscale              dword ? </v>
       </c>
       <c r="J29" t="str">
@@ -1814,7 +1818,7 @@
         <v/>
       </c>
       <c r="I30" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B30="",IF(A30="","","; " &amp;A30),A30&amp;REPT(" ",MAX(F:F)-F30+1)&amp;B30&amp;" ? "&amp;IF(H30&lt;&gt;"","; "&amp;H30,""))</f>
         <v xml:space="preserve">dc_vscale              dword ? </v>
       </c>
       <c r="J30" t="str">
@@ -1840,7 +1844,7 @@
         <v/>
       </c>
       <c r="I31" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B31="",IF(A31="","","; " &amp;A31),A31&amp;REPT(" ",MAX(F:F)-F31+1)&amp;B31&amp;" ? "&amp;IF(H31&lt;&gt;"","; "&amp;H31,""))</f>
         <v/>
       </c>
       <c r="J31" t="str">
@@ -1875,7 +1879,7 @@
         <v/>
       </c>
       <c r="I32" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B32="",IF(A32="","","; " &amp;A32),A32&amp;REPT(" ",MAX(F:F)-F32+1)&amp;B32&amp;" ? "&amp;IF(H32&lt;&gt;"","; "&amp;H32,""))</f>
         <v xml:space="preserve">register_pc            word ? </v>
       </c>
       <c r="J32" t="str">
@@ -1910,7 +1914,7 @@
         <v/>
       </c>
       <c r="I33" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B33="",IF(A33="","","; " &amp;A33),A33&amp;REPT(" ",MAX(F:F)-F33+1)&amp;B33&amp;" ? "&amp;IF(H33&lt;&gt;"","; "&amp;H33,""))</f>
         <v xml:space="preserve">stackpointer           word ? </v>
       </c>
       <c r="J33" t="str">
@@ -1936,7 +1940,7 @@
         <v/>
       </c>
       <c r="I34" t="str">
-        <f t="shared" ref="I34:I65" si="3">IF(B34="",IF(A34="","","; " &amp;A34),A34&amp;REPT(" ",MAX(F:F)-F34+1)&amp;B34&amp;" ? "&amp;IF(H34&lt;&gt;"","; "&amp;H34,""))</f>
+        <f>IF(B34="",IF(A34="","","; " &amp;A34),A34&amp;REPT(" ",MAX(F:F)-F34+1)&amp;B34&amp;" ? "&amp;IF(H34&lt;&gt;"","; "&amp;H34,""))</f>
         <v/>
       </c>
       <c r="J34" t="str">
@@ -1971,7 +1975,7 @@
         <v/>
       </c>
       <c r="I35" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B35="",IF(A35="","","; " &amp;A35),A35&amp;REPT(" ",MAX(F:F)-F35+1)&amp;B35&amp;" ? "&amp;IF(H35&lt;&gt;"","; "&amp;H35,""))</f>
         <v xml:space="preserve">register_a             byte ? </v>
       </c>
       <c r="J35" t="str">
@@ -2006,7 +2010,7 @@
         <v/>
       </c>
       <c r="I36" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B36="",IF(A36="","","; " &amp;A36),A36&amp;REPT(" ",MAX(F:F)-F36+1)&amp;B36&amp;" ? "&amp;IF(H36&lt;&gt;"","; "&amp;H36,""))</f>
         <v xml:space="preserve">register_x             byte ? </v>
       </c>
       <c r="J36" t="str">
@@ -2041,7 +2045,7 @@
         <v/>
       </c>
       <c r="I37" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B37="",IF(A37="","","; " &amp;A37),A37&amp;REPT(" ",MAX(F:F)-F37+1)&amp;B37&amp;" ? "&amp;IF(H37&lt;&gt;"","; "&amp;H37,""))</f>
         <v xml:space="preserve">register_y             byte ? </v>
       </c>
       <c r="J37" t="str">
@@ -2067,7 +2071,7 @@
         <v/>
       </c>
       <c r="I38" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B38="",IF(A38="","","; " &amp;A38),A38&amp;REPT(" ",MAX(F:F)-F38+1)&amp;B38&amp;" ? "&amp;IF(H38&lt;&gt;"","; "&amp;H38,""))</f>
         <v/>
       </c>
       <c r="J38" t="str">
@@ -2102,7 +2106,7 @@
         <v/>
       </c>
       <c r="I39" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B39="",IF(A39="","","; " &amp;A39),A39&amp;REPT(" ",MAX(F:F)-F39+1)&amp;B39&amp;" ? "&amp;IF(H39&lt;&gt;"","; "&amp;H39,""))</f>
         <v xml:space="preserve">flags_decimal          byte ? </v>
       </c>
       <c r="J39" t="str">
@@ -2137,7 +2141,7 @@
         <v/>
       </c>
       <c r="I40" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B40="",IF(A40="","","; " &amp;A40),A40&amp;REPT(" ",MAX(F:F)-F40+1)&amp;B40&amp;" ? "&amp;IF(H40&lt;&gt;"","; "&amp;H40,""))</f>
         <v xml:space="preserve">flags_break            byte ? </v>
       </c>
       <c r="J40" t="str">
@@ -2172,7 +2176,7 @@
         <v/>
       </c>
       <c r="I41" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B41="",IF(A41="","","; " &amp;A41),A41&amp;REPT(" ",MAX(F:F)-F41+1)&amp;B41&amp;" ? "&amp;IF(H41&lt;&gt;"","; "&amp;H41,""))</f>
         <v xml:space="preserve">flags_overflow         byte ? </v>
       </c>
       <c r="J41" t="str">
@@ -2207,7 +2211,7 @@
         <v/>
       </c>
       <c r="I42" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B42="",IF(A42="","","; " &amp;A42),A42&amp;REPT(" ",MAX(F:F)-F42+1)&amp;B42&amp;" ? "&amp;IF(H42&lt;&gt;"","; "&amp;H42,""))</f>
         <v xml:space="preserve">flags_negative         byte ? </v>
       </c>
       <c r="J42" t="str">
@@ -2242,7 +2246,7 @@
         <v/>
       </c>
       <c r="I43" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B43="",IF(A43="","","; " &amp;A43),A43&amp;REPT(" ",MAX(F:F)-F43+1)&amp;B43&amp;" ? "&amp;IF(H43&lt;&gt;"","; "&amp;H43,""))</f>
         <v xml:space="preserve">flags_carry            byte ? </v>
       </c>
       <c r="J43" t="str">
@@ -2277,7 +2281,7 @@
         <v/>
       </c>
       <c r="I44" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B44="",IF(A44="","","; " &amp;A44),A44&amp;REPT(" ",MAX(F:F)-F44+1)&amp;B44&amp;" ? "&amp;IF(H44&lt;&gt;"","; "&amp;H44,""))</f>
         <v xml:space="preserve">flags_zero             byte ? </v>
       </c>
       <c r="J44" t="str">
@@ -2312,7 +2316,7 @@
         <v/>
       </c>
       <c r="I45" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B45="",IF(A45="","","; " &amp;A45),A45&amp;REPT(" ",MAX(F:F)-F45+1)&amp;B45&amp;" ? "&amp;IF(H45&lt;&gt;"","; "&amp;H45,""))</f>
         <v xml:space="preserve">flags_interruptDisable byte ? </v>
       </c>
       <c r="J45" t="str">
@@ -2338,7 +2342,7 @@
         <v/>
       </c>
       <c r="I46" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B46="",IF(A46="","","; " &amp;A46),A46&amp;REPT(" ",MAX(F:F)-F46+1)&amp;B46&amp;" ? "&amp;IF(H46&lt;&gt;"","; "&amp;H46,""))</f>
         <v/>
       </c>
       <c r="J46" t="str">
@@ -2373,7 +2377,7 @@
         <v/>
       </c>
       <c r="I47" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B47="",IF(A47="","","; " &amp;A47),A47&amp;REPT(" ",MAX(F:F)-F47+1)&amp;B47&amp;" ? "&amp;IF(H47&lt;&gt;"","; "&amp;H47,""))</f>
         <v xml:space="preserve">interrupt              byte ? </v>
       </c>
       <c r="J47" t="str">
@@ -2408,7 +2412,7 @@
         <v/>
       </c>
       <c r="I48" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B48="",IF(A48="","","; " &amp;A48),A48&amp;REPT(" ",MAX(F:F)-F48+1)&amp;B48&amp;" ? "&amp;IF(H48&lt;&gt;"","; "&amp;H48,""))</f>
         <v xml:space="preserve">nmi                    byte ? </v>
       </c>
       <c r="J48" t="str">
@@ -2443,7 +2447,7 @@
         <v/>
       </c>
       <c r="I49" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B49="",IF(A49="","","; " &amp;A49),A49&amp;REPT(" ",MAX(F:F)-F49+1)&amp;B49&amp;" ? "&amp;IF(H49&lt;&gt;"","; "&amp;H49,""))</f>
         <v xml:space="preserve">nmi_previous           byte ? </v>
       </c>
       <c r="J49" t="str">
@@ -2461,15 +2465,15 @@
         <v>185</v>
       </c>
       <c r="F50">
-        <f t="shared" ref="F50:F113" si="4">LEN(A50)</f>
+        <f t="shared" ref="F50:F117" si="2">LEN(A50)</f>
         <v>0</v>
       </c>
       <c r="G50" t="str">
-        <f t="shared" ref="G50:G113" si="5">IF(B50="", "", IF(E50/D50&lt;&gt;FLOOR(E50/D50,1),"ERROR",""))</f>
+        <f t="shared" ref="G50:G117" si="3">IF(B50="", "", IF(E50/D50&lt;&gt;FLOOR(E50/D50,1),"ERROR",""))</f>
         <v/>
       </c>
       <c r="I50" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B50="",IF(A50="","","; " &amp;A50),A50&amp;REPT(" ",MAX(F:F)-F50+1)&amp;B50&amp;" ? "&amp;IF(H50&lt;&gt;"","; "&amp;H50,""))</f>
         <v/>
       </c>
       <c r="J50" t="str">
@@ -2496,15 +2500,15 @@
         <v>186</v>
       </c>
       <c r="F51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="G51" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I51" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B51="",IF(A51="","","; " &amp;A51),A51&amp;REPT(" ",MAX(F:F)-F51+1)&amp;B51&amp;" ? "&amp;IF(H51&lt;&gt;"","; "&amp;H51,""))</f>
         <v xml:space="preserve">addrsel                byte ? </v>
       </c>
       <c r="J51" t="str">
@@ -2531,15 +2535,15 @@
         <v>187</v>
       </c>
       <c r="F52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="G52" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I52" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B52="",IF(A52="","","; " &amp;A52),A52&amp;REPT(" ",MAX(F:F)-F52+1)&amp;B52&amp;" ? "&amp;IF(H52&lt;&gt;"","; "&amp;H52,""))</f>
         <v xml:space="preserve">dcsel                  byte ? </v>
       </c>
       <c r="J52" t="str">
@@ -2566,15 +2570,15 @@
         <v>188</v>
       </c>
       <c r="F53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G53" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I53" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B53="",IF(A53="","","; " &amp;A53),A53&amp;REPT(" ",MAX(F:F)-F53+1)&amp;B53&amp;" ? "&amp;IF(H53&lt;&gt;"","; "&amp;H53,""))</f>
         <v xml:space="preserve">dc_border              byte ? </v>
       </c>
       <c r="J53" t="str">
@@ -2592,15 +2596,15 @@
         <v>188</v>
       </c>
       <c r="F54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G54" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I54" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B54="",IF(A54="","","; " &amp;A54),A54&amp;REPT(" ",MAX(F:F)-F54+1)&amp;B54&amp;" ? "&amp;IF(H54&lt;&gt;"","; "&amp;H54,""))</f>
         <v/>
       </c>
       <c r="J54" t="str">
@@ -2627,15 +2631,15 @@
         <v>190</v>
       </c>
       <c r="F55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G55" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I55" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B55="",IF(A55="","","; " &amp;A55),A55&amp;REPT(" ",MAX(F:F)-F55+1)&amp;B55&amp;" ? "&amp;IF(H55&lt;&gt;"","; "&amp;H55,""))</f>
         <v xml:space="preserve">dc_hstart              word ? </v>
       </c>
       <c r="J55" t="str">
@@ -2662,15 +2666,15 @@
         <v>192</v>
       </c>
       <c r="F56">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="G56" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I56" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B56="",IF(A56="","","; " &amp;A56),A56&amp;REPT(" ",MAX(F:F)-F56+1)&amp;B56&amp;" ? "&amp;IF(H56&lt;&gt;"","; "&amp;H56,""))</f>
         <v xml:space="preserve">dc_hstop               word ? </v>
       </c>
       <c r="J56" t="str">
@@ -2697,15 +2701,15 @@
         <v>194</v>
       </c>
       <c r="F57">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G57" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I57" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B57="",IF(A57="","","; " &amp;A57),A57&amp;REPT(" ",MAX(F:F)-F57+1)&amp;B57&amp;" ? "&amp;IF(H57&lt;&gt;"","; "&amp;H57,""))</f>
         <v xml:space="preserve">dc_vstart              word ? </v>
       </c>
       <c r="J57" t="str">
@@ -2732,15 +2736,15 @@
         <v>196</v>
       </c>
       <c r="F58">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="G58" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I58" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B58="",IF(A58="","","; " &amp;A58),A58&amp;REPT(" ",MAX(F:F)-F58+1)&amp;B58&amp;" ? "&amp;IF(H58&lt;&gt;"","; "&amp;H58,""))</f>
         <v xml:space="preserve">dc_vstop               word ? </v>
       </c>
       <c r="J58" t="str">
@@ -2758,15 +2762,15 @@
         <v>196</v>
       </c>
       <c r="F59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G59" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I59" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B59="",IF(A59="","","; " &amp;A59),A59&amp;REPT(" ",MAX(F:F)-F59+1)&amp;B59&amp;" ? "&amp;IF(H59&lt;&gt;"","; "&amp;H59,""))</f>
         <v/>
       </c>
       <c r="J59" t="str">
@@ -2793,15 +2797,15 @@
         <v>197</v>
       </c>
       <c r="F60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="G60" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I60" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B60="",IF(A60="","","; " &amp;A60),A60&amp;REPT(" ",MAX(F:F)-F60+1)&amp;B60&amp;" ? "&amp;IF(H60&lt;&gt;"","; "&amp;H60,""))</f>
         <v xml:space="preserve">sprite_enable          byte ? </v>
       </c>
       <c r="J60" t="str">
@@ -2828,15 +2832,15 @@
         <v>198</v>
       </c>
       <c r="F61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="G61" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I61" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B61="",IF(A61="","","; " &amp;A61),A61&amp;REPT(" ",MAX(F:F)-F61+1)&amp;B61&amp;" ? "&amp;IF(H61&lt;&gt;"","; "&amp;H61,""))</f>
         <v xml:space="preserve">layer0_enable          byte ? </v>
       </c>
       <c r="J61" t="str">
@@ -2863,15 +2867,15 @@
         <v>199</v>
       </c>
       <c r="F62">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="G62" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I62" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B62="",IF(A62="","","; " &amp;A62),A62&amp;REPT(" ",MAX(F:F)-F62+1)&amp;B62&amp;" ? "&amp;IF(H62&lt;&gt;"","; "&amp;H62,""))</f>
         <v xml:space="preserve">layer1_enable          byte ? </v>
       </c>
       <c r="J62" t="str">
@@ -2889,15 +2893,15 @@
         <v>199</v>
       </c>
       <c r="F63">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G63" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I63" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B63="",IF(A63="","","; " &amp;A63),A63&amp;REPT(" ",MAX(F:F)-F63+1)&amp;B63&amp;" ? "&amp;IF(H63&lt;&gt;"","; "&amp;H63,""))</f>
         <v/>
       </c>
       <c r="J63" t="str">
@@ -2924,15 +2928,15 @@
         <v>200</v>
       </c>
       <c r="F64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="G64" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I64" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B64="",IF(A64="","","; " &amp;A64),A64&amp;REPT(" ",MAX(F:F)-F64+1)&amp;B64&amp;" ? "&amp;IF(H64&lt;&gt;"","; "&amp;H64,""))</f>
         <v xml:space="preserve">display_carry          byte ? </v>
       </c>
       <c r="J64" t="str">
@@ -2950,15 +2954,15 @@
         <v>200</v>
       </c>
       <c r="F65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G65" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I65" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(B65="",IF(A65="","","; " &amp;A65),A65&amp;REPT(" ",MAX(F:F)-F65+1)&amp;B65&amp;" ? "&amp;IF(H65&lt;&gt;"","; "&amp;H65,""))</f>
         <v/>
       </c>
       <c r="J65" t="str">
@@ -2985,15 +2989,15 @@
         <v>204</v>
       </c>
       <c r="F66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I66" t="str">
-        <f t="shared" ref="I66:I97" si="6">IF(B66="",IF(A66="","","; " &amp;A66),A66&amp;REPT(" ",MAX(F:F)-F66+1)&amp;B66&amp;" ? "&amp;IF(H66&lt;&gt;"","; "&amp;H66,""))</f>
+        <f>IF(B66="",IF(A66="","","; " &amp;A66),A66&amp;REPT(" ",MAX(F:F)-F66+1)&amp;B66&amp;" ? "&amp;IF(H66&lt;&gt;"","; "&amp;H66,""))</f>
         <v xml:space="preserve">layer0_mapAddress      dword ? </v>
       </c>
       <c r="J66" t="str">
@@ -3020,15 +3024,15 @@
         <v>208</v>
       </c>
       <c r="F67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I67" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B67="",IF(A67="","","; " &amp;A67),A67&amp;REPT(" ",MAX(F:F)-F67+1)&amp;B67&amp;" ? "&amp;IF(H67&lt;&gt;"","; "&amp;H67,""))</f>
         <v xml:space="preserve">layer0_tileAddress     dword ? </v>
       </c>
       <c r="J67" t="str">
@@ -3055,15 +3059,15 @@
         <v>210</v>
       </c>
       <c r="F68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="G68" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I68" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B68="",IF(A68="","","; " &amp;A68),A68&amp;REPT(" ",MAX(F:F)-F68+1)&amp;B68&amp;" ? "&amp;IF(H68&lt;&gt;"","; "&amp;H68,""))</f>
         <v xml:space="preserve">layer0_hscroll         word ? </v>
       </c>
       <c r="J68" t="str">
@@ -3090,15 +3094,15 @@
         <v>212</v>
       </c>
       <c r="F69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="G69" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I69" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B69="",IF(A69="","","; " &amp;A69),A69&amp;REPT(" ",MAX(F:F)-F69+1)&amp;B69&amp;" ? "&amp;IF(H69&lt;&gt;"","; "&amp;H69,""))</f>
         <v xml:space="preserve">layer0_vscroll         word ? </v>
       </c>
       <c r="J69" t="str">
@@ -3125,15 +3129,15 @@
         <v>213</v>
       </c>
       <c r="F70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G70" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I70" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B70="",IF(A70="","","; " &amp;A70),A70&amp;REPT(" ",MAX(F:F)-F70+1)&amp;B70&amp;" ? "&amp;IF(H70&lt;&gt;"","; "&amp;H70,""))</f>
         <v xml:space="preserve">layer0_mapHeight       byte ? </v>
       </c>
       <c r="J70" t="str">
@@ -3160,15 +3164,15 @@
         <v>214</v>
       </c>
       <c r="F71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I71" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B71="",IF(A71="","","; " &amp;A71),A71&amp;REPT(" ",MAX(F:F)-F71+1)&amp;B71&amp;" ? "&amp;IF(H71&lt;&gt;"","; "&amp;H71,""))</f>
         <v xml:space="preserve">layer0_mapWidth        byte ? </v>
       </c>
       <c r="J71" t="str">
@@ -3195,15 +3199,15 @@
         <v>215</v>
       </c>
       <c r="F72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="G72" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I72" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B72="",IF(A72="","","; " &amp;A72),A72&amp;REPT(" ",MAX(F:F)-F72+1)&amp;B72&amp;" ? "&amp;IF(H72&lt;&gt;"","; "&amp;H72,""))</f>
         <v xml:space="preserve">layer0_bitmapMode      byte ? </v>
       </c>
       <c r="J72" t="str">
@@ -3230,15 +3234,15 @@
         <v>216</v>
       </c>
       <c r="F73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I73" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B73="",IF(A73="","","; " &amp;A73),A73&amp;REPT(" ",MAX(F:F)-F73+1)&amp;B73&amp;" ? "&amp;IF(H73&lt;&gt;"","; "&amp;H73,""))</f>
         <v xml:space="preserve">layer0_colourDepth     byte ? </v>
       </c>
       <c r="J73" t="str">
@@ -3265,15 +3269,15 @@
         <v>217</v>
       </c>
       <c r="F74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="G74" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I74" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B74="",IF(A74="","","; " &amp;A74),A74&amp;REPT(" ",MAX(F:F)-F74+1)&amp;B74&amp;" ? "&amp;IF(H74&lt;&gt;"","; "&amp;H74,""))</f>
         <v xml:space="preserve">layer0_tileHeight      byte ? </v>
       </c>
       <c r="J74" t="str">
@@ -3300,15 +3304,15 @@
         <v>218</v>
       </c>
       <c r="F75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I75" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B75="",IF(A75="","","; " &amp;A75),A75&amp;REPT(" ",MAX(F:F)-F75+1)&amp;B75&amp;" ? "&amp;IF(H75&lt;&gt;"","; "&amp;H75,""))</f>
         <v xml:space="preserve">layer0_tileWidth       byte ? </v>
       </c>
       <c r="J75" t="str">
@@ -3326,15 +3330,15 @@
         <v>218</v>
       </c>
       <c r="F76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G76" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I76" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B76="",IF(A76="","","; " &amp;A76),A76&amp;REPT(" ",MAX(F:F)-F76+1)&amp;B76&amp;" ? "&amp;IF(H76&lt;&gt;"","; "&amp;H76,""))</f>
         <v/>
       </c>
       <c r="J76" t="str">
@@ -3361,15 +3365,15 @@
         <v>219</v>
       </c>
       <c r="F77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G77" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I77" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B77="",IF(A77="","","; " &amp;A77),A77&amp;REPT(" ",MAX(F:F)-F77+1)&amp;B77&amp;" ? "&amp;IF(H77&lt;&gt;"","; "&amp;H77,""))</f>
         <v xml:space="preserve">cpu_waiting            byte ? </v>
       </c>
       <c r="J77" t="str">
@@ -3396,15 +3400,15 @@
         <v>220</v>
       </c>
       <c r="F78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="G78" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I78" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B78="",IF(A78="","","; " &amp;A78),A78&amp;REPT(" ",MAX(F:F)-F78+1)&amp;B78&amp;" ? "&amp;IF(H78&lt;&gt;"","; "&amp;H78,""))</f>
         <v xml:space="preserve">headless               byte ? </v>
       </c>
       <c r="J78" t="str">
@@ -3422,15 +3426,15 @@
         <v>220</v>
       </c>
       <c r="F79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G79" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I79" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B79="",IF(A79="","","; " &amp;A79),A79&amp;REPT(" ",MAX(F:F)-F79+1)&amp;B79&amp;" ? "&amp;IF(H79&lt;&gt;"","; "&amp;H79,""))</f>
         <v/>
       </c>
       <c r="J79" t="str">
@@ -3457,15 +3461,15 @@
         <v>224</v>
       </c>
       <c r="F80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="G80" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I80" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B80="",IF(A80="","","; " &amp;A80),A80&amp;REPT(" ",MAX(F:F)-F80+1)&amp;B80&amp;" ? "&amp;IF(H80&lt;&gt;"","; "&amp;H80,""))</f>
         <v xml:space="preserve">layer1_mapAddress      dword ? </v>
       </c>
       <c r="J80" t="str">
@@ -3492,15 +3496,15 @@
         <v>228</v>
       </c>
       <c r="F81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G81" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I81" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B81="",IF(A81="","","; " &amp;A81),A81&amp;REPT(" ",MAX(F:F)-F81+1)&amp;B81&amp;" ? "&amp;IF(H81&lt;&gt;"","; "&amp;H81,""))</f>
         <v xml:space="preserve">layer1_tileAddress     dword ? </v>
       </c>
       <c r="J81" t="str">
@@ -3527,15 +3531,15 @@
         <v>230</v>
       </c>
       <c r="F82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="G82" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I82" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B82="",IF(A82="","","; " &amp;A82),A82&amp;REPT(" ",MAX(F:F)-F82+1)&amp;B82&amp;" ? "&amp;IF(H82&lt;&gt;"","; "&amp;H82,""))</f>
         <v xml:space="preserve">layer1_hscroll         word ? </v>
       </c>
       <c r="J82" t="str">
@@ -3562,15 +3566,15 @@
         <v>232</v>
       </c>
       <c r="F83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="G83" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I83" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B83="",IF(A83="","","; " &amp;A83),A83&amp;REPT(" ",MAX(F:F)-F83+1)&amp;B83&amp;" ? "&amp;IF(H83&lt;&gt;"","; "&amp;H83,""))</f>
         <v xml:space="preserve">layer1_vscroll         word ? </v>
       </c>
       <c r="J83" t="str">
@@ -3597,15 +3601,15 @@
         <v>233</v>
       </c>
       <c r="F84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G84" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I84" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B84="",IF(A84="","","; " &amp;A84),A84&amp;REPT(" ",MAX(F:F)-F84+1)&amp;B84&amp;" ? "&amp;IF(H84&lt;&gt;"","; "&amp;H84,""))</f>
         <v xml:space="preserve">layer1_mapHeight       byte ? </v>
       </c>
       <c r="J84" t="str">
@@ -3632,15 +3636,15 @@
         <v>234</v>
       </c>
       <c r="F85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="G85" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I85" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B85="",IF(A85="","","; " &amp;A85),A85&amp;REPT(" ",MAX(F:F)-F85+1)&amp;B85&amp;" ? "&amp;IF(H85&lt;&gt;"","; "&amp;H85,""))</f>
         <v xml:space="preserve">layer1_mapWidth        byte ? </v>
       </c>
       <c r="J85" t="str">
@@ -3667,15 +3671,15 @@
         <v>235</v>
       </c>
       <c r="F86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="G86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I86" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B86="",IF(A86="","","; " &amp;A86),A86&amp;REPT(" ",MAX(F:F)-F86+1)&amp;B86&amp;" ? "&amp;IF(H86&lt;&gt;"","; "&amp;H86,""))</f>
         <v xml:space="preserve">layer1_bitmapMode      byte ? </v>
       </c>
       <c r="J86" t="str">
@@ -3702,15 +3706,15 @@
         <v>236</v>
       </c>
       <c r="F87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I87" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B87="",IF(A87="","","; " &amp;A87),A87&amp;REPT(" ",MAX(F:F)-F87+1)&amp;B87&amp;" ? "&amp;IF(H87&lt;&gt;"","; "&amp;H87,""))</f>
         <v xml:space="preserve">layer1_colourDepth     byte ? </v>
       </c>
       <c r="J87" t="str">
@@ -3737,15 +3741,15 @@
         <v>237</v>
       </c>
       <c r="F88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="G88" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I88" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B88="",IF(A88="","","; " &amp;A88),A88&amp;REPT(" ",MAX(F:F)-F88+1)&amp;B88&amp;" ? "&amp;IF(H88&lt;&gt;"","; "&amp;H88,""))</f>
         <v xml:space="preserve">layer1_tileHeight      byte ? </v>
       </c>
       <c r="J88" t="str">
@@ -3772,15 +3776,15 @@
         <v>238</v>
       </c>
       <c r="F89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G89" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I89" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B89="",IF(A89="","","; " &amp;A89),A89&amp;REPT(" ",MAX(F:F)-F89+1)&amp;B89&amp;" ? "&amp;IF(H89&lt;&gt;"","; "&amp;H89,""))</f>
         <v xml:space="preserve">layer1_tileWidth       byte ? </v>
       </c>
       <c r="J89" t="str">
@@ -3798,15 +3802,15 @@
         <v>238</v>
       </c>
       <c r="F90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G90" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I90" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B90="",IF(A90="","","; " &amp;A90),A90&amp;REPT(" ",MAX(F:F)-F90+1)&amp;B90&amp;" ? "&amp;IF(H90&lt;&gt;"","; "&amp;H90,""))</f>
         <v/>
       </c>
       <c r="J90" t="str">
@@ -3833,15 +3837,15 @@
         <v>240</v>
       </c>
       <c r="F91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="G91" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I91" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B91="",IF(A91="","","; " &amp;A91),A91&amp;REPT(" ",MAX(F:F)-F91+1)&amp;B91&amp;" ? "&amp;IF(H91&lt;&gt;"","; "&amp;H91,""))</f>
         <v xml:space="preserve">interrupt_linenum      word ? </v>
       </c>
       <c r="J91" t="str">
@@ -3868,15 +3872,15 @@
         <v>241</v>
       </c>
       <c r="F92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="G92" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I92" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B92="",IF(A92="","","; " &amp;A92),A92&amp;REPT(" ",MAX(F:F)-F92+1)&amp;B92&amp;" ? "&amp;IF(H92&lt;&gt;"","; "&amp;H92,""))</f>
         <v xml:space="preserve">interrupt_aflow        byte ? </v>
       </c>
       <c r="J92" t="str">
@@ -3903,15 +3907,15 @@
         <v>242</v>
       </c>
       <c r="F93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="G93" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I93" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B93="",IF(A93="","","; " &amp;A93),A93&amp;REPT(" ",MAX(F:F)-F93+1)&amp;B93&amp;" ? "&amp;IF(H93&lt;&gt;"","; "&amp;H93,""))</f>
         <v xml:space="preserve">interrupt_spcol        byte ? </v>
       </c>
       <c r="J93" t="str">
@@ -3938,15 +3942,15 @@
         <v>243</v>
       </c>
       <c r="F94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="G94" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I94" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B94="",IF(A94="","","; " &amp;A94),A94&amp;REPT(" ",MAX(F:F)-F94+1)&amp;B94&amp;" ? "&amp;IF(H94&lt;&gt;"","; "&amp;H94,""))</f>
         <v xml:space="preserve">interrupt_line         byte ? </v>
       </c>
       <c r="J94" t="str">
@@ -3973,15 +3977,15 @@
         <v>244</v>
       </c>
       <c r="F95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="G95" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I95" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B95="",IF(A95="","","; " &amp;A95),A95&amp;REPT(" ",MAX(F:F)-F95+1)&amp;B95&amp;" ? "&amp;IF(H95&lt;&gt;"","; "&amp;H95,""))</f>
         <v xml:space="preserve">interrupt_vsync        byte ? </v>
       </c>
       <c r="J95" t="str">
@@ -3999,15 +4003,15 @@
         <v>244</v>
       </c>
       <c r="F96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G96" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I96" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B96="",IF(A96="","","; " &amp;A96),A96&amp;REPT(" ",MAX(F:F)-F96+1)&amp;B96&amp;" ? "&amp;IF(H96&lt;&gt;"","; "&amp;H96,""))</f>
         <v/>
       </c>
       <c r="J96" t="str">
@@ -4034,15 +4038,15 @@
         <v>245</v>
       </c>
       <c r="F97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G97" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I97" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(B97="",IF(A97="","","; " &amp;A97),A97&amp;REPT(" ",MAX(F:F)-F97+1)&amp;B97&amp;" ? "&amp;IF(H97&lt;&gt;"","; "&amp;H97,""))</f>
         <v xml:space="preserve">interrupt_line_hit     byte ? </v>
       </c>
       <c r="J97" t="str">
@@ -4069,15 +4073,15 @@
         <v>246</v>
       </c>
       <c r="F98">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="G98" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I98" t="str">
-        <f t="shared" ref="I98:I129" si="7">IF(B98="",IF(A98="","","; " &amp;A98),A98&amp;REPT(" ",MAX(F:F)-F98+1)&amp;B98&amp;" ? "&amp;IF(H98&lt;&gt;"","; "&amp;H98,""))</f>
+        <f>IF(B98="",IF(A98="","","; " &amp;A98),A98&amp;REPT(" ",MAX(F:F)-F98+1)&amp;B98&amp;" ? "&amp;IF(H98&lt;&gt;"","; "&amp;H98,""))</f>
         <v xml:space="preserve">interrupt_vsync_hit    byte ? </v>
       </c>
       <c r="J98" t="str">
@@ -4104,15 +4108,15 @@
         <v>247</v>
       </c>
       <c r="F99">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="G99" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I99" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(B99="",IF(A99="","","; " &amp;A99),A99&amp;REPT(" ",MAX(F:F)-F99+1)&amp;B99&amp;" ? "&amp;IF(H99&lt;&gt;"","; "&amp;H99,""))</f>
         <v xml:space="preserve">interrupt_spcol_hit    byte ? </v>
       </c>
       <c r="J99" t="str">
@@ -4139,15 +4143,15 @@
         <v>248</v>
       </c>
       <c r="F100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="G100" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I100" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(B100="",IF(A100="","","; " &amp;A100),A100&amp;REPT(" ",MAX(F:F)-F100+1)&amp;B100&amp;" ? "&amp;IF(H100&lt;&gt;"","; "&amp;H100,""))</f>
         <v xml:space="preserve">drawing                byte ? </v>
       </c>
       <c r="J100" t="str">
@@ -4165,15 +4169,15 @@
         <v>248</v>
       </c>
       <c r="F101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G101" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I101" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(B101="",IF(A101="","","; " &amp;A101),A101&amp;REPT(" ",MAX(F:F)-F101+1)&amp;B101&amp;" ? "&amp;IF(H101&lt;&gt;"","; "&amp;H101,""))</f>
         <v/>
       </c>
       <c r="J101" t="str">
@@ -4194,15 +4198,15 @@
         <v>248</v>
       </c>
       <c r="F102">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G102" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I102" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(B102="",IF(A102="","","; " &amp;A102),A102&amp;REPT(" ",MAX(F:F)-F102+1)&amp;B102&amp;" ? "&amp;IF(H102&lt;&gt;"","; "&amp;H102,""))</f>
         <v>; Rendering</v>
       </c>
       <c r="J102" t="str">
@@ -4229,18 +4233,18 @@
         <v>252</v>
       </c>
       <c r="F103">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="G103" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H103" t="s">
         <v>132</v>
       </c>
       <c r="I103" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(B103="",IF(A103="","","; " &amp;A103),A103&amp;REPT(" ",MAX(F:F)-F103+1)&amp;B103&amp;" ? "&amp;IF(H103&lt;&gt;"","; "&amp;H103,""))</f>
         <v>display_position       dword ? ; needs to be inline with the cpu clock</v>
       </c>
       <c r="J103" t="str">
@@ -4267,15 +4271,15 @@
         <v>256</v>
       </c>
       <c r="F104">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G104" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I104" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(B104="",IF(A104="","","; " &amp;A104),A104&amp;REPT(" ",MAX(F:F)-F104+1)&amp;B104&amp;" ? "&amp;IF(H104&lt;&gt;"","; "&amp;H104,""))</f>
         <v xml:space="preserve">frame_count            dword ? </v>
       </c>
       <c r="J104" t="str">
@@ -4302,15 +4306,15 @@
         <v>260</v>
       </c>
       <c r="F105">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="G105" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I105" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(B105="",IF(A105="","","; " &amp;A105),A105&amp;REPT(" ",MAX(F:F)-F105+1)&amp;B105&amp;" ? "&amp;IF(H105&lt;&gt;"","; "&amp;H105,""))</f>
         <v xml:space="preserve">buffer_render_position dword ? </v>
       </c>
       <c r="J105" t="str">
@@ -4337,15 +4341,15 @@
         <v>264</v>
       </c>
       <c r="F106">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="G106" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I106" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(B106="",IF(A106="","","; " &amp;A106),A106&amp;REPT(" ",MAX(F:F)-F106+1)&amp;B106&amp;" ? "&amp;IF(H106&lt;&gt;"","; "&amp;H106,""))</f>
         <v xml:space="preserve">buffer_output_position dword ? </v>
       </c>
       <c r="J106" t="str">
@@ -4372,15 +4376,15 @@
         <v>268</v>
       </c>
       <c r="F107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="G107" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I107" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(B107="",IF(A107="","","; " &amp;A107),A107&amp;REPT(" ",MAX(F:F)-F107+1)&amp;B107&amp;" ? "&amp;IF(H107&lt;&gt;"","; "&amp;H107,""))</f>
         <v xml:space="preserve">scale_x                dword ? </v>
       </c>
       <c r="J107" t="str">
@@ -4407,15 +4411,15 @@
         <v>272</v>
       </c>
       <c r="F108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="G108" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I108" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(B108="",IF(A108="","","; " &amp;A108),A108&amp;REPT(" ",MAX(F:F)-F108+1)&amp;B108&amp;" ? "&amp;IF(H108&lt;&gt;"","; "&amp;H108,""))</f>
         <v xml:space="preserve">scale_y                dword ? </v>
       </c>
       <c r="J108" t="str">
@@ -4442,15 +4446,15 @@
         <v>274</v>
       </c>
       <c r="F109">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G109" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I109" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(B109="",IF(A109="","","; " &amp;A109),A109&amp;REPT(" ",MAX(F:F)-F109+1)&amp;B109&amp;" ? "&amp;IF(H109&lt;&gt;"","; "&amp;H109,""))</f>
         <v xml:space="preserve">display_x              word ? </v>
       </c>
       <c r="J109" t="str">
@@ -4477,15 +4481,15 @@
         <v>276</v>
       </c>
       <c r="F110">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G110" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I110" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(B110="",IF(A110="","","; " &amp;A110),A110&amp;REPT(" ",MAX(F:F)-F110+1)&amp;B110&amp;" ? "&amp;IF(H110&lt;&gt;"","; "&amp;H110,""))</f>
         <v xml:space="preserve">display_y              word ? </v>
       </c>
       <c r="J110" t="str">
@@ -4494,73 +4498,69 @@
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D111" t="str">
+      <c r="A111" t="s">
+        <v>141</v>
+      </c>
+      <c r="B111" t="s">
+        <v>114</v>
+      </c>
+      <c r="D111">
         <f>IF(B111="", "", VLOOKUP(B111,Sheet2!A:B,2,FALSE))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E111">
         <f>IF(B111="",E110,VLOOKUP(B111,Sheet2!A:B,2,FALSE)+E110)</f>
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F111">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G111" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I111" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <f>IF(B111="",IF(A111="","","; " &amp;A111),A111&amp;REPT(" ",MAX(F:F)-F111+1)&amp;B111&amp;" ? "&amp;IF(H111&lt;&gt;"","; "&amp;H111,""))</f>
+        <v xml:space="preserve">dirty                  byte ? </v>
       </c>
       <c r="J111" t="str">
         <f>IF(B111&lt;&gt;"", "        public "&amp;VLOOKUP(B111,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A111)&amp;" = "&amp;C111&amp;";"&amp;IF(H111="",""," // "&amp;H111), IF(A111&lt;&gt;"","        // "&amp;A111,""))</f>
-        <v/>
+        <v xml:space="preserve">        public byte Dirty = ;</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>136</v>
-      </c>
-      <c r="D112" t="str">
+        <v>142</v>
+      </c>
+      <c r="B112" t="s">
+        <v>114</v>
+      </c>
+      <c r="D112">
         <f>IF(B112="", "", VLOOKUP(B112,Sheet2!A:B,2,FALSE))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E112">
         <f>IF(B112="",E111,VLOOKUP(B112,Sheet2!A:B,2,FALSE)+E111)</f>
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="F112">
-        <f t="shared" si="4"/>
-        <v>7</v>
+        <f t="shared" ref="F112:F115" si="4">LEN(A112)</f>
+        <v>17</v>
       </c>
       <c r="G112" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I112" t="str">
-        <f t="shared" si="7"/>
-        <v>; Layer 0</v>
-      </c>
-      <c r="J112" t="str">
-        <f>IF(B112&lt;&gt;"", "        public "&amp;VLOOKUP(B112,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A112)&amp;" = "&amp;C112&amp;";"&amp;IF(H112="",""," // "&amp;H112), IF(A112&lt;&gt;"","        // "&amp;A112,""))</f>
-        <v xml:space="preserve">        // Layer 0</v>
+        <f>IF(B112="",IF(A112="","","; " &amp;A112),A112&amp;REPT(" ",MAX(F:F)-F112+1)&amp;B112&amp;" ? "&amp;IF(H112&lt;&gt;"","; "&amp;H112,""))</f>
+        <v xml:space="preserve">rendering_spacing      byte ? </v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>87</v>
-      </c>
-      <c r="B113" t="s">
-        <v>113</v>
-      </c>
-      <c r="C113">
-        <v>0</v>
-      </c>
-      <c r="D113">
+      <c r="D113" t="str">
         <f>IF(B113="", "", VLOOKUP(B113,Sheet2!A:B,2,FALSE))</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="E113">
         <f>IF(B113="",E112,VLOOKUP(B113,Sheet2!A:B,2,FALSE)+E112)</f>
@@ -4568,129 +4568,69 @@
       </c>
       <c r="F113">
         <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="G113" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I113" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">layer0_next_render     word ? </v>
-      </c>
-      <c r="J113" t="str">
-        <f>IF(B113&lt;&gt;"", "        public "&amp;VLOOKUP(B113,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A113)&amp;" = "&amp;C113&amp;";"&amp;IF(H113="",""," // "&amp;H113), IF(A113&lt;&gt;"","        // "&amp;A113,""))</f>
-        <v xml:space="preserve">        public ushort Layer0_Next_Render = 0;</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>88</v>
-      </c>
-      <c r="B114" t="s">
-        <v>113</v>
-      </c>
-      <c r="C114">
-        <v>0</v>
-      </c>
-      <c r="D114">
+      <c r="D114" t="str">
         <f>IF(B114="", "", VLOOKUP(B114,Sheet2!A:B,2,FALSE))</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="E114">
         <f>IF(B114="",E113,VLOOKUP(B114,Sheet2!A:B,2,FALSE)+E113)</f>
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F114">
-        <f t="shared" ref="F114:F153" si="8">LEN(A114)</f>
-        <v>18</v>
-      </c>
-      <c r="G114" t="str">
-        <f t="shared" ref="G114:G153" si="9">IF(B114="", "", IF(E114/D114&lt;&gt;FLOOR(E114/D114,1),"ERROR",""))</f>
-        <v/>
-      </c>
-      <c r="I114" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">layer0_tile_hshift     word ? </v>
-      </c>
-      <c r="J114" t="str">
-        <f>IF(B114&lt;&gt;"", "        public "&amp;VLOOKUP(B114,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A114)&amp;" = "&amp;C114&amp;";"&amp;IF(H114="",""," // "&amp;H114), IF(A114&lt;&gt;"","        // "&amp;A114,""))</f>
-        <v xml:space="preserve">        public ushort Layer0_Tile_Hshift = 0;</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>89</v>
-      </c>
-      <c r="B115" t="s">
-        <v>113</v>
-      </c>
-      <c r="C115">
-        <v>0</v>
-      </c>
-      <c r="D115">
+      <c r="D115" t="str">
         <f>IF(B115="", "", VLOOKUP(B115,Sheet2!A:B,2,FALSE))</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="E115">
         <f>IF(B115="",E114,VLOOKUP(B115,Sheet2!A:B,2,FALSE)+E114)</f>
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F115">
-        <f t="shared" si="8"/>
-        <v>18</v>
-      </c>
-      <c r="G115" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="I115" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">layer0_tile_vshift     word ? </v>
-      </c>
-      <c r="J115" t="str">
-        <f>IF(B115&lt;&gt;"", "        public "&amp;VLOOKUP(B115,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A115)&amp;" = "&amp;C115&amp;";"&amp;IF(H115="",""," // "&amp;H115), IF(A115&lt;&gt;"","        // "&amp;A115,""))</f>
-        <v xml:space="preserve">        public ushort Layer0_Tile_Vshift = 0;</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>90</v>
-      </c>
-      <c r="B116" t="s">
-        <v>113</v>
-      </c>
-      <c r="C116">
-        <v>0</v>
-      </c>
-      <c r="D116">
+        <v>136</v>
+      </c>
+      <c r="D116" t="str">
         <f>IF(B116="", "", VLOOKUP(B116,Sheet2!A:B,2,FALSE))</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="E116">
         <f>IF(B116="",E115,VLOOKUP(B116,Sheet2!A:B,2,FALSE)+E115)</f>
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="F116">
-        <f t="shared" si="8"/>
-        <v>17</v>
+        <f t="shared" ref="F116:F157" si="5">LEN(A116)</f>
+        <v>7</v>
       </c>
       <c r="G116" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I116" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">layer0_map_hshift      word ? </v>
+        <f>IF(B116="",IF(A116="","","; " &amp;A116),A116&amp;REPT(" ",MAX(F:F)-F116+1)&amp;B116&amp;" ? "&amp;IF(H116&lt;&gt;"","; "&amp;H116,""))</f>
+        <v>; Layer 0</v>
       </c>
       <c r="J116" t="str">
         <f>IF(B116&lt;&gt;"", "        public "&amp;VLOOKUP(B116,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A116)&amp;" = "&amp;C116&amp;";"&amp;IF(H116="",""," // "&amp;H116), IF(A116&lt;&gt;"","        // "&amp;A116,""))</f>
-        <v xml:space="preserve">        public ushort Layer0_Map_Hshift = 0;</v>
+        <v xml:space="preserve">        // Layer 0</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B117" t="s">
         <v>113</v>
@@ -4704,109 +4644,133 @@
       </c>
       <c r="E117">
         <f>IF(B117="",E116,VLOOKUP(B117,Sheet2!A:B,2,FALSE)+E116)</f>
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="F117">
-        <f t="shared" si="8"/>
-        <v>17</v>
+        <f t="shared" si="5"/>
+        <v>18</v>
       </c>
       <c r="G117" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I117" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">layer0_map_vshift      word ? </v>
+        <f>IF(B117="",IF(A117="","","; " &amp;A117),A117&amp;REPT(" ",MAX(F:F)-F117+1)&amp;B117&amp;" ? "&amp;IF(H117&lt;&gt;"","; "&amp;H117,""))</f>
+        <v xml:space="preserve">layer0_next_render     word ? </v>
       </c>
       <c r="J117" t="str">
         <f>IF(B117&lt;&gt;"", "        public "&amp;VLOOKUP(B117,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A117)&amp;" = "&amp;C117&amp;";"&amp;IF(H117="",""," // "&amp;H117), IF(A117&lt;&gt;"","        // "&amp;A117,""))</f>
-        <v xml:space="preserve">        public ushort Layer0_Map_Vshift = 0;</v>
+        <v xml:space="preserve">        public ushort Layer0_Next_Render = 0;</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D118" t="str">
+      <c r="A118" t="s">
+        <v>88</v>
+      </c>
+      <c r="B118" t="s">
+        <v>113</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+      <c r="D118">
         <f>IF(B118="", "", VLOOKUP(B118,Sheet2!A:B,2,FALSE))</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="E118">
         <f>IF(B118="",E117,VLOOKUP(B118,Sheet2!A:B,2,FALSE)+E117)</f>
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F118">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>18</v>
       </c>
       <c r="G118" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="G118:G157" si="6">IF(B118="", "", IF(E118/D118&lt;&gt;FLOOR(E118/D118,1),"ERROR",""))</f>
         <v/>
       </c>
       <c r="I118" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <f>IF(B118="",IF(A118="","","; " &amp;A118),A118&amp;REPT(" ",MAX(F:F)-F118+1)&amp;B118&amp;" ? "&amp;IF(H118&lt;&gt;"","; "&amp;H118,""))</f>
+        <v xml:space="preserve">layer0_tile_hshift     word ? </v>
       </c>
       <c r="J118" t="str">
         <f>IF(B118&lt;&gt;"", "        public "&amp;VLOOKUP(B118,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A118)&amp;" = "&amp;C118&amp;";"&amp;IF(H118="",""," // "&amp;H118), IF(A118&lt;&gt;"","        // "&amp;A118,""))</f>
-        <v/>
+        <v xml:space="preserve">        public ushort Layer0_Tile_Hshift = 0;</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D119" t="str">
+      <c r="A119" t="s">
+        <v>89</v>
+      </c>
+      <c r="B119" t="s">
+        <v>113</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+      <c r="D119">
         <f>IF(B119="", "", VLOOKUP(B119,Sheet2!A:B,2,FALSE))</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="E119">
         <f>IF(B119="",E118,VLOOKUP(B119,Sheet2!A:B,2,FALSE)+E118)</f>
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F119">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>18</v>
       </c>
       <c r="G119" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I119" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <f>IF(B119="",IF(A119="","","; " &amp;A119),A119&amp;REPT(" ",MAX(F:F)-F119+1)&amp;B119&amp;" ? "&amp;IF(H119&lt;&gt;"","; "&amp;H119,""))</f>
+        <v xml:space="preserve">layer0_tile_vshift     word ? </v>
       </c>
       <c r="J119" t="str">
         <f>IF(B119&lt;&gt;"", "        public "&amp;VLOOKUP(B119,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A119)&amp;" = "&amp;C119&amp;";"&amp;IF(H119="",""," // "&amp;H119), IF(A119&lt;&gt;"","        // "&amp;A119,""))</f>
-        <v/>
+        <v xml:space="preserve">        public ushort Layer0_Tile_Vshift = 0;</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>135</v>
-      </c>
-      <c r="D120" t="str">
+        <v>90</v>
+      </c>
+      <c r="B120" t="s">
+        <v>113</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
         <f>IF(B120="", "", VLOOKUP(B120,Sheet2!A:B,2,FALSE))</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="E120">
         <f>IF(B120="",E119,VLOOKUP(B120,Sheet2!A:B,2,FALSE)+E119)</f>
         <v>286</v>
       </c>
       <c r="F120">
-        <f t="shared" si="8"/>
-        <v>7</v>
+        <f t="shared" si="5"/>
+        <v>17</v>
       </c>
       <c r="G120" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I120" t="str">
-        <f t="shared" si="7"/>
-        <v>; Layer 1</v>
+        <f>IF(B120="",IF(A120="","","; " &amp;A120),A120&amp;REPT(" ",MAX(F:F)-F120+1)&amp;B120&amp;" ? "&amp;IF(H120&lt;&gt;"","; "&amp;H120,""))</f>
+        <v xml:space="preserve">layer0_map_hshift      word ? </v>
       </c>
       <c r="J120" t="str">
         <f>IF(B120&lt;&gt;"", "        public "&amp;VLOOKUP(B120,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A120)&amp;" = "&amp;C120&amp;";"&amp;IF(H120="",""," // "&amp;H120), IF(A120&lt;&gt;"","        // "&amp;A120,""))</f>
-        <v xml:space="preserve">        // Layer 1</v>
+        <v xml:space="preserve">        public ushort Layer0_Map_Hshift = 0;</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B121" t="s">
         <v>113</v>
@@ -4823,130 +4787,106 @@
         <v>288</v>
       </c>
       <c r="F121">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f t="shared" si="5"/>
+        <v>17</v>
       </c>
       <c r="G121" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I121" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">layer1_next_render     word ? </v>
+        <f>IF(B121="",IF(A121="","","; " &amp;A121),A121&amp;REPT(" ",MAX(F:F)-F121+1)&amp;B121&amp;" ? "&amp;IF(H121&lt;&gt;"","; "&amp;H121,""))</f>
+        <v xml:space="preserve">layer0_map_vshift      word ? </v>
       </c>
       <c r="J121" t="str">
         <f>IF(B121&lt;&gt;"", "        public "&amp;VLOOKUP(B121,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A121)&amp;" = "&amp;C121&amp;";"&amp;IF(H121="",""," // "&amp;H121), IF(A121&lt;&gt;"","        // "&amp;A121,""))</f>
-        <v xml:space="preserve">        public ushort Layer1_Next_Render = 0;</v>
+        <v xml:space="preserve">        public ushort Layer0_Map_Vshift = 0;</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>93</v>
-      </c>
-      <c r="B122" t="s">
-        <v>113</v>
-      </c>
-      <c r="C122">
-        <v>0</v>
-      </c>
-      <c r="D122">
+      <c r="D122" t="str">
         <f>IF(B122="", "", VLOOKUP(B122,Sheet2!A:B,2,FALSE))</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="E122">
         <f>IF(B122="",E121,VLOOKUP(B122,Sheet2!A:B,2,FALSE)+E121)</f>
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F122">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="G122" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I122" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">layer1_tile_hshift     word ? </v>
+        <f>IF(B122="",IF(A122="","","; " &amp;A122),A122&amp;REPT(" ",MAX(F:F)-F122+1)&amp;B122&amp;" ? "&amp;IF(H122&lt;&gt;"","; "&amp;H122,""))</f>
+        <v/>
       </c>
       <c r="J122" t="str">
         <f>IF(B122&lt;&gt;"", "        public "&amp;VLOOKUP(B122,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A122)&amp;" = "&amp;C122&amp;";"&amp;IF(H122="",""," // "&amp;H122), IF(A122&lt;&gt;"","        // "&amp;A122,""))</f>
-        <v xml:space="preserve">        public ushort Layer1_Tile_Hshift = 0;</v>
+        <v/>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>94</v>
-      </c>
-      <c r="B123" t="s">
-        <v>113</v>
-      </c>
-      <c r="C123">
-        <v>0</v>
-      </c>
-      <c r="D123">
+      <c r="D123" t="str">
         <f>IF(B123="", "", VLOOKUP(B123,Sheet2!A:B,2,FALSE))</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="E123">
         <f>IF(B123="",E122,VLOOKUP(B123,Sheet2!A:B,2,FALSE)+E122)</f>
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F123">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="G123" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I123" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">layer1_tile_vshift     word ? </v>
+        <f>IF(B123="",IF(A123="","","; " &amp;A123),A123&amp;REPT(" ",MAX(F:F)-F123+1)&amp;B123&amp;" ? "&amp;IF(H123&lt;&gt;"","; "&amp;H123,""))</f>
+        <v/>
       </c>
       <c r="J123" t="str">
         <f>IF(B123&lt;&gt;"", "        public "&amp;VLOOKUP(B123,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A123)&amp;" = "&amp;C123&amp;";"&amp;IF(H123="",""," // "&amp;H123), IF(A123&lt;&gt;"","        // "&amp;A123,""))</f>
-        <v xml:space="preserve">        public ushort Layer1_Tile_Vshift = 0;</v>
+        <v/>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>95</v>
-      </c>
-      <c r="B124" t="s">
-        <v>113</v>
-      </c>
-      <c r="C124">
-        <v>0</v>
-      </c>
-      <c r="D124">
+        <v>135</v>
+      </c>
+      <c r="D124" t="str">
         <f>IF(B124="", "", VLOOKUP(B124,Sheet2!A:B,2,FALSE))</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="E124">
         <f>IF(B124="",E123,VLOOKUP(B124,Sheet2!A:B,2,FALSE)+E123)</f>
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="F124">
-        <f t="shared" si="8"/>
-        <v>17</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="G124" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I124" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">layer1_map_hshift      word ? </v>
+        <f>IF(B124="",IF(A124="","","; " &amp;A124),A124&amp;REPT(" ",MAX(F:F)-F124+1)&amp;B124&amp;" ? "&amp;IF(H124&lt;&gt;"","; "&amp;H124,""))</f>
+        <v>; Layer 1</v>
       </c>
       <c r="J124" t="str">
         <f>IF(B124&lt;&gt;"", "        public "&amp;VLOOKUP(B124,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A124)&amp;" = "&amp;C124&amp;";"&amp;IF(H124="",""," // "&amp;H124), IF(A124&lt;&gt;"","        // "&amp;A124,""))</f>
-        <v xml:space="preserve">        public ushort Layer1_Map_Hshift = 0;</v>
+        <v xml:space="preserve">        // Layer 1</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B125" t="s">
         <v>113</v>
@@ -4960,83 +4900,98 @@
       </c>
       <c r="E125">
         <f>IF(B125="",E124,VLOOKUP(B125,Sheet2!A:B,2,FALSE)+E124)</f>
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="F125">
-        <f t="shared" si="8"/>
-        <v>17</v>
+        <f t="shared" si="5"/>
+        <v>18</v>
       </c>
       <c r="G125" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I125" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">layer1_map_vshift      word ? </v>
+        <f>IF(B125="",IF(A125="","","; " &amp;A125),A125&amp;REPT(" ",MAX(F:F)-F125+1)&amp;B125&amp;" ? "&amp;IF(H125&lt;&gt;"","; "&amp;H125,""))</f>
+        <v xml:space="preserve">layer1_next_render     word ? </v>
       </c>
       <c r="J125" t="str">
         <f>IF(B125&lt;&gt;"", "        public "&amp;VLOOKUP(B125,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A125)&amp;" = "&amp;C125&amp;";"&amp;IF(H125="",""," // "&amp;H125), IF(A125&lt;&gt;"","        // "&amp;A125,""))</f>
-        <v xml:space="preserve">        public ushort Layer1_Map_Vshift = 0;</v>
+        <v xml:space="preserve">        public ushort Layer1_Next_Render = 0;</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D126" t="str">
+      <c r="A126" t="s">
+        <v>93</v>
+      </c>
+      <c r="B126" t="s">
+        <v>113</v>
+      </c>
+      <c r="C126">
+        <v>0</v>
+      </c>
+      <c r="D126">
         <f>IF(B126="", "", VLOOKUP(B126,Sheet2!A:B,2,FALSE))</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="E126">
         <f>IF(B126="",E125,VLOOKUP(B126,Sheet2!A:B,2,FALSE)+E125)</f>
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F126">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>18</v>
       </c>
       <c r="G126" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I126" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <f>IF(B126="",IF(A126="","","; " &amp;A126),A126&amp;REPT(" ",MAX(F:F)-F126+1)&amp;B126&amp;" ? "&amp;IF(H126&lt;&gt;"","; "&amp;H126,""))</f>
+        <v xml:space="preserve">layer1_tile_hshift     word ? </v>
       </c>
       <c r="J126" t="str">
         <f>IF(B126&lt;&gt;"", "        public "&amp;VLOOKUP(B126,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A126)&amp;" = "&amp;C126&amp;";"&amp;IF(H126="",""," // "&amp;H126), IF(A126&lt;&gt;"","        // "&amp;A126,""))</f>
-        <v/>
+        <v xml:space="preserve">        public ushort Layer1_Tile_Hshift = 0;</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>134</v>
-      </c>
-      <c r="D127" t="str">
+        <v>94</v>
+      </c>
+      <c r="B127" t="s">
+        <v>113</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+      <c r="D127">
         <f>IF(B127="", "", VLOOKUP(B127,Sheet2!A:B,2,FALSE))</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="E127">
         <f>IF(B127="",E126,VLOOKUP(B127,Sheet2!A:B,2,FALSE)+E126)</f>
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F127">
-        <f t="shared" si="8"/>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>18</v>
       </c>
       <c r="G127" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I127" t="str">
-        <f t="shared" si="7"/>
-        <v>; VIA 1</v>
+        <f>IF(B127="",IF(A127="","","; " &amp;A127),A127&amp;REPT(" ",MAX(F:F)-F127+1)&amp;B127&amp;" ? "&amp;IF(H127&lt;&gt;"","; "&amp;H127,""))</f>
+        <v xml:space="preserve">layer1_tile_vshift     word ? </v>
       </c>
       <c r="J127" t="str">
         <f>IF(B127&lt;&gt;"", "        public "&amp;VLOOKUP(B127,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A127)&amp;" = "&amp;C127&amp;";"&amp;IF(H127="",""," // "&amp;H127), IF(A127&lt;&gt;"","        // "&amp;A127,""))</f>
-        <v xml:space="preserve">        // VIA 1</v>
+        <v xml:space="preserve">        public ushort Layer1_Tile_Vshift = 0;</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B128" t="s">
         <v>113</v>
@@ -5050,28 +5005,28 @@
       </c>
       <c r="E128">
         <f>IF(B128="",E127,VLOOKUP(B128,Sheet2!A:B,2,FALSE)+E127)</f>
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F128">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <f t="shared" si="5"/>
+        <v>17</v>
       </c>
       <c r="G128" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I128" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">via_t1counter_latch    word ? </v>
+        <f>IF(B128="",IF(A128="","","; " &amp;A128),A128&amp;REPT(" ",MAX(F:F)-F128+1)&amp;B128&amp;" ? "&amp;IF(H128&lt;&gt;"","; "&amp;H128,""))</f>
+        <v xml:space="preserve">layer1_map_hshift      word ? </v>
       </c>
       <c r="J128" t="str">
         <f>IF(B128&lt;&gt;"", "        public "&amp;VLOOKUP(B128,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A128)&amp;" = "&amp;C128&amp;";"&amp;IF(H128="",""," // "&amp;H128), IF(A128&lt;&gt;"","        // "&amp;A128,""))</f>
-        <v xml:space="preserve">        public ushort Via_T1Counter_Latch = 0;</v>
+        <v xml:space="preserve">        public ushort Layer1_Map_Hshift = 0;</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B129" t="s">
         <v>113</v>
@@ -5085,224 +5040,221 @@
       </c>
       <c r="E129">
         <f>IF(B129="",E128,VLOOKUP(B129,Sheet2!A:B,2,FALSE)+E128)</f>
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F129">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <f t="shared" si="5"/>
+        <v>17</v>
       </c>
       <c r="G129" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I129" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">via_t1counter_value    word ? </v>
+        <f>IF(B129="",IF(A129="","","; " &amp;A129),A129&amp;REPT(" ",MAX(F:F)-F129+1)&amp;B129&amp;" ? "&amp;IF(H129&lt;&gt;"","; "&amp;H129,""))</f>
+        <v xml:space="preserve">layer1_map_vshift      word ? </v>
       </c>
       <c r="J129" t="str">
         <f>IF(B129&lt;&gt;"", "        public "&amp;VLOOKUP(B129,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A129)&amp;" = "&amp;C129&amp;";"&amp;IF(H129="",""," // "&amp;H129), IF(A129&lt;&gt;"","        // "&amp;A129,""))</f>
-        <v xml:space="preserve">        public ushort Via_T1Counter_Value = 0;</v>
+        <v xml:space="preserve">        public ushort Layer1_Map_Vshift = 0;</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>99</v>
-      </c>
-      <c r="B130" t="s">
-        <v>113</v>
-      </c>
-      <c r="C130">
-        <v>0</v>
-      </c>
-      <c r="D130">
+      <c r="D130" t="str">
         <f>IF(B130="", "", VLOOKUP(B130,Sheet2!A:B,2,FALSE))</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="E130">
         <f>IF(B130="",E129,VLOOKUP(B130,Sheet2!A:B,2,FALSE)+E129)</f>
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F130">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="G130" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I130" t="str">
-        <f t="shared" ref="I130:I153" si="10">IF(B130="",IF(A130="","","; " &amp;A130),A130&amp;REPT(" ",MAX(F:F)-F130+1)&amp;B130&amp;" ? "&amp;IF(H130&lt;&gt;"","; "&amp;H130,""))</f>
-        <v xml:space="preserve">via_t2counter_latch    word ? </v>
+        <f>IF(B130="",IF(A130="","","; " &amp;A130),A130&amp;REPT(" ",MAX(F:F)-F130+1)&amp;B130&amp;" ? "&amp;IF(H130&lt;&gt;"","; "&amp;H130,""))</f>
+        <v/>
       </c>
       <c r="J130" t="str">
         <f>IF(B130&lt;&gt;"", "        public "&amp;VLOOKUP(B130,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A130)&amp;" = "&amp;C130&amp;";"&amp;IF(H130="",""," // "&amp;H130), IF(A130&lt;&gt;"","        // "&amp;A130,""))</f>
-        <v xml:space="preserve">        public ushort Via_T2Counter_Latch = 0;</v>
+        <v/>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>100</v>
-      </c>
-      <c r="B131" t="s">
-        <v>113</v>
-      </c>
-      <c r="C131">
-        <v>0</v>
-      </c>
-      <c r="D131">
+        <v>134</v>
+      </c>
+      <c r="D131" t="str">
         <f>IF(B131="", "", VLOOKUP(B131,Sheet2!A:B,2,FALSE))</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="E131">
         <f>IF(B131="",E130,VLOOKUP(B131,Sheet2!A:B,2,FALSE)+E130)</f>
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="F131">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="G131" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I131" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve">via_t2counter_value    word ? </v>
+        <f>IF(B131="",IF(A131="","","; " &amp;A131),A131&amp;REPT(" ",MAX(F:F)-F131+1)&amp;B131&amp;" ? "&amp;IF(H131&lt;&gt;"","; "&amp;H131,""))</f>
+        <v>; VIA 1</v>
       </c>
       <c r="J131" t="str">
         <f>IF(B131&lt;&gt;"", "        public "&amp;VLOOKUP(B131,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A131)&amp;" = "&amp;C131&amp;";"&amp;IF(H131="",""," // "&amp;H131), IF(A131&lt;&gt;"","        // "&amp;A131,""))</f>
-        <v xml:space="preserve">        public ushort Via_T2Counter_Value = 0;</v>
+        <v xml:space="preserve">        // VIA 1</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D132" t="str">
+      <c r="A132" t="s">
+        <v>97</v>
+      </c>
+      <c r="B132" t="s">
+        <v>113</v>
+      </c>
+      <c r="C132">
+        <v>0</v>
+      </c>
+      <c r="D132">
         <f>IF(B132="", "", VLOOKUP(B132,Sheet2!A:B,2,FALSE))</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="E132">
         <f>IF(B132="",E131,VLOOKUP(B132,Sheet2!A:B,2,FALSE)+E131)</f>
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="F132">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>19</v>
       </c>
       <c r="G132" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I132" t="str">
-        <f t="shared" si="10"/>
-        <v/>
+        <f>IF(B132="",IF(A132="","","; " &amp;A132),A132&amp;REPT(" ",MAX(F:F)-F132+1)&amp;B132&amp;" ? "&amp;IF(H132&lt;&gt;"","; "&amp;H132,""))</f>
+        <v xml:space="preserve">via_t1counter_latch    word ? </v>
       </c>
       <c r="J132" t="str">
         <f>IF(B132&lt;&gt;"", "        public "&amp;VLOOKUP(B132,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A132)&amp;" = "&amp;C132&amp;";"&amp;IF(H132="",""," // "&amp;H132), IF(A132&lt;&gt;"","        // "&amp;A132,""))</f>
-        <v/>
+        <v xml:space="preserve">        public ushort Via_T1Counter_Latch = 0;</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>140</v>
+        <v>98</v>
       </c>
       <c r="B133" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C133">
         <v>0</v>
       </c>
       <c r="D133">
         <f>IF(B133="", "", VLOOKUP(B133,Sheet2!A:B,2,FALSE))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E133">
         <f>IF(B133="",E132,VLOOKUP(B133,Sheet2!A:B,2,FALSE)+E132)</f>
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F133">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f t="shared" si="5"/>
+        <v>19</v>
       </c>
       <c r="G133" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I133" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve">register_a_outdata     byte ? </v>
+        <f>IF(B133="",IF(A133="","","; " &amp;A133),A133&amp;REPT(" ",MAX(F:F)-F133+1)&amp;B133&amp;" ? "&amp;IF(H133&lt;&gt;"","; "&amp;H133,""))</f>
+        <v xml:space="preserve">via_t1counter_value    word ? </v>
       </c>
       <c r="J133" t="str">
         <f>IF(B133&lt;&gt;"", "        public "&amp;VLOOKUP(B133,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A133)&amp;" = "&amp;C133&amp;";"&amp;IF(H133="",""," // "&amp;H133), IF(A133&lt;&gt;"","        // "&amp;A133,""))</f>
-        <v xml:space="preserve">        public byte Register_A_Outdata = 0;</v>
+        <v xml:space="preserve">        public ushort Via_T1Counter_Value = 0;</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>139</v>
+        <v>99</v>
       </c>
       <c r="B134" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C134">
         <v>0</v>
       </c>
       <c r="D134">
         <f>IF(B134="", "", VLOOKUP(B134,Sheet2!A:B,2,FALSE))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E134">
         <f>IF(B134="",E133,VLOOKUP(B134,Sheet2!A:B,2,FALSE)+E133)</f>
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F134">
-        <f t="shared" si="8"/>
-        <v>17</v>
+        <f t="shared" si="5"/>
+        <v>19</v>
       </c>
       <c r="G134" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I134" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve">register_a_indata      byte ? </v>
+        <f>IF(B134="",IF(A134="","","; " &amp;A134),A134&amp;REPT(" ",MAX(F:F)-F134+1)&amp;B134&amp;" ? "&amp;IF(H134&lt;&gt;"","; "&amp;H134,""))</f>
+        <v xml:space="preserve">via_t2counter_latch    word ? </v>
       </c>
       <c r="J134" t="str">
         <f>IF(B134&lt;&gt;"", "        public "&amp;VLOOKUP(B134,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A134)&amp;" = "&amp;C134&amp;";"&amp;IF(H134="",""," // "&amp;H134), IF(A134&lt;&gt;"","        // "&amp;A134,""))</f>
-        <v xml:space="preserve">        public byte Register_A_Indata = 0;</v>
+        <v xml:space="preserve">        public ushort Via_T2Counter_Latch = 0;</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>100</v>
+      </c>
+      <c r="B135" t="s">
+        <v>113</v>
+      </c>
       <c r="C135">
         <v>0</v>
       </c>
-      <c r="D135" t="str">
+      <c r="D135">
         <f>IF(B135="", "", VLOOKUP(B135,Sheet2!A:B,2,FALSE))</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="E135">
         <f>IF(B135="",E134,VLOOKUP(B135,Sheet2!A:B,2,FALSE)+E134)</f>
         <v>306</v>
       </c>
       <c r="F135">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>19</v>
       </c>
       <c r="G135" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I135" t="str">
-        <f t="shared" si="10"/>
-        <v/>
+        <f>IF(B135="",IF(A135="","","; " &amp;A135),A135&amp;REPT(" ",MAX(F:F)-F135+1)&amp;B135&amp;" ? "&amp;IF(H135&lt;&gt;"","; "&amp;H135,""))</f>
+        <v xml:space="preserve">via_t2counter_value    word ? </v>
       </c>
       <c r="J135" t="str">
         <f>IF(B135&lt;&gt;"", "        public "&amp;VLOOKUP(B135,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A135)&amp;" = "&amp;C135&amp;";"&amp;IF(H135="",""," // "&amp;H135), IF(A135&lt;&gt;"","        // "&amp;A135,""))</f>
-        <v/>
+        <v xml:space="preserve">        public ushort Via_T2Counter_Value = 0;</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C136">
-        <v>0</v>
-      </c>
       <c r="D136" t="str">
         <f>IF(B136="", "", VLOOKUP(B136,Sheet2!A:B,2,FALSE))</f>
         <v/>
@@ -5312,15 +5264,15 @@
         <v>306</v>
       </c>
       <c r="F136">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G136" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I136" t="str">
-        <f t="shared" si="10"/>
+        <f>IF(B136="",IF(A136="","","; " &amp;A136),A136&amp;REPT(" ",MAX(F:F)-F136+1)&amp;B136&amp;" ? "&amp;IF(H136&lt;&gt;"","; "&amp;H136,""))</f>
         <v/>
       </c>
       <c r="J136" t="str">
@@ -5329,61 +5281,73 @@
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>140</v>
+      </c>
+      <c r="B137" t="s">
+        <v>114</v>
+      </c>
       <c r="C137">
         <v>0</v>
       </c>
-      <c r="D137" t="str">
+      <c r="D137">
         <f>IF(B137="", "", VLOOKUP(B137,Sheet2!A:B,2,FALSE))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E137">
         <f>IF(B137="",E136,VLOOKUP(B137,Sheet2!A:B,2,FALSE)+E136)</f>
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F137">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>18</v>
       </c>
       <c r="G137" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I137" t="str">
-        <f t="shared" si="10"/>
-        <v/>
+        <f>IF(B137="",IF(A137="","","; " &amp;A137),A137&amp;REPT(" ",MAX(F:F)-F137+1)&amp;B137&amp;" ? "&amp;IF(H137&lt;&gt;"","; "&amp;H137,""))</f>
+        <v xml:space="preserve">register_a_outdata     byte ? </v>
       </c>
       <c r="J137" t="str">
         <f>IF(B137&lt;&gt;"", "        public "&amp;VLOOKUP(B137,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A137)&amp;" = "&amp;C137&amp;";"&amp;IF(H137="",""," // "&amp;H137), IF(A137&lt;&gt;"","        // "&amp;A137,""))</f>
-        <v/>
+        <v xml:space="preserve">        public byte Register_A_Outdata = 0;</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>139</v>
+      </c>
+      <c r="B138" t="s">
+        <v>114</v>
+      </c>
       <c r="C138">
         <v>0</v>
       </c>
-      <c r="D138" t="str">
+      <c r="D138">
         <f>IF(B138="", "", VLOOKUP(B138,Sheet2!A:B,2,FALSE))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E138">
         <f>IF(B138="",E137,VLOOKUP(B138,Sheet2!A:B,2,FALSE)+E137)</f>
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="F138">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>17</v>
       </c>
       <c r="G138" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I138" t="str">
-        <f t="shared" si="10"/>
-        <v/>
+        <f>IF(B138="",IF(A138="","","; " &amp;A138),A138&amp;REPT(" ",MAX(F:F)-F138+1)&amp;B138&amp;" ? "&amp;IF(H138&lt;&gt;"","; "&amp;H138,""))</f>
+        <v xml:space="preserve">register_a_indata      byte ? </v>
       </c>
       <c r="J138" t="str">
         <f>IF(B138&lt;&gt;"", "        public "&amp;VLOOKUP(B138,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A138)&amp;" = "&amp;C138&amp;";"&amp;IF(H138="",""," // "&amp;H138), IF(A138&lt;&gt;"","        // "&amp;A138,""))</f>
-        <v/>
+        <v xml:space="preserve">        public byte Register_A_Indata = 0;</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
@@ -5396,18 +5360,18 @@
       </c>
       <c r="E139">
         <f>IF(B139="",E138,VLOOKUP(B139,Sheet2!A:B,2,FALSE)+E138)</f>
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="F139">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G139" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I139" t="str">
-        <f t="shared" si="10"/>
+        <f>IF(B139="",IF(A139="","","; " &amp;A139),A139&amp;REPT(" ",MAX(F:F)-F139+1)&amp;B139&amp;" ? "&amp;IF(H139&lt;&gt;"","; "&amp;H139,""))</f>
         <v/>
       </c>
       <c r="J139" t="str">
@@ -5416,24 +5380,27 @@
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C140">
+        <v>0</v>
+      </c>
       <c r="D140" t="str">
         <f>IF(B140="", "", VLOOKUP(B140,Sheet2!A:B,2,FALSE))</f>
         <v/>
       </c>
       <c r="E140">
         <f>IF(B140="",E139,VLOOKUP(B140,Sheet2!A:B,2,FALSE)+E139)</f>
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="F140">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G140" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I140" t="str">
-        <f t="shared" si="10"/>
+        <f>IF(B140="",IF(A140="","","; " &amp;A140),A140&amp;REPT(" ",MAX(F:F)-F140+1)&amp;B140&amp;" ? "&amp;IF(H140&lt;&gt;"","; "&amp;H140,""))</f>
         <v/>
       </c>
       <c r="J140" t="str">
@@ -5442,108 +5409,90 @@
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>101</v>
-      </c>
-      <c r="B141" t="s">
-        <v>114</v>
-      </c>
       <c r="C141">
         <v>0</v>
       </c>
-      <c r="D141">
+      <c r="D141" t="str">
         <f>IF(B141="", "", VLOOKUP(B141,Sheet2!A:B,2,FALSE))</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="E141">
         <f>IF(B141="",E140,VLOOKUP(B141,Sheet2!A:B,2,FALSE)+E140)</f>
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F141">
-        <f t="shared" si="8"/>
-        <v>21</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="G141" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I141" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve">via_timer1_continuous  byte ? </v>
+        <f>IF(B141="",IF(A141="","","; " &amp;A141),A141&amp;REPT(" ",MAX(F:F)-F141+1)&amp;B141&amp;" ? "&amp;IF(H141&lt;&gt;"","; "&amp;H141,""))</f>
+        <v/>
       </c>
       <c r="J141" t="str">
         <f>IF(B141&lt;&gt;"", "        public "&amp;VLOOKUP(B141,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A141)&amp;" = "&amp;C141&amp;";"&amp;IF(H141="",""," // "&amp;H141), IF(A141&lt;&gt;"","        // "&amp;A141,""))</f>
-        <v xml:space="preserve">        public byte Via_Timer1_Continuous = 0;</v>
+        <v/>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>102</v>
-      </c>
-      <c r="B142" t="s">
-        <v>114</v>
-      </c>
       <c r="C142">
         <v>0</v>
       </c>
-      <c r="D142">
+      <c r="D142" t="str">
         <f>IF(B142="", "", VLOOKUP(B142,Sheet2!A:B,2,FALSE))</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="E142">
         <f>IF(B142="",E141,VLOOKUP(B142,Sheet2!A:B,2,FALSE)+E141)</f>
         <v>308</v>
       </c>
       <c r="F142">
-        <f t="shared" si="8"/>
-        <v>14</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="G142" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I142" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve">via_timer1_pb7         byte ? </v>
+        <f>IF(B142="",IF(A142="","","; " &amp;A142),A142&amp;REPT(" ",MAX(F:F)-F142+1)&amp;B142&amp;" ? "&amp;IF(H142&lt;&gt;"","; "&amp;H142,""))</f>
+        <v/>
       </c>
       <c r="J142" t="str">
         <f>IF(B142&lt;&gt;"", "        public "&amp;VLOOKUP(B142,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A142)&amp;" = "&amp;C142&amp;";"&amp;IF(H142="",""," // "&amp;H142), IF(A142&lt;&gt;"","        // "&amp;A142,""))</f>
-        <v xml:space="preserve">        public byte Via_Timer1_Pb7 = 0;</v>
+        <v/>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>103</v>
-      </c>
-      <c r="B143" t="s">
-        <v>114</v>
-      </c>
       <c r="C143">
         <v>0</v>
       </c>
-      <c r="D143">
+      <c r="D143" t="str">
         <f>IF(B143="", "", VLOOKUP(B143,Sheet2!A:B,2,FALSE))</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="E143">
         <f>IF(B143="",E142,VLOOKUP(B143,Sheet2!A:B,2,FALSE)+E142)</f>
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F143">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="G143" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I143" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve">via_timer1_running     byte ? </v>
+        <f>IF(B143="",IF(A143="","","; " &amp;A143),A143&amp;REPT(" ",MAX(F:F)-F143+1)&amp;B143&amp;" ? "&amp;IF(H143&lt;&gt;"","; "&amp;H143,""))</f>
+        <v/>
       </c>
       <c r="J143" t="str">
         <f>IF(B143&lt;&gt;"", "        public "&amp;VLOOKUP(B143,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A143)&amp;" = "&amp;C143&amp;";"&amp;IF(H143="",""," // "&amp;H143), IF(A143&lt;&gt;"","        // "&amp;A143,""))</f>
-        <v xml:space="preserve">        public byte Via_Timer1_Running = 0;</v>
+        <v/>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
@@ -5553,18 +5502,18 @@
       </c>
       <c r="E144">
         <f>IF(B144="",E143,VLOOKUP(B144,Sheet2!A:B,2,FALSE)+E143)</f>
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F144">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G144" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I144" t="str">
-        <f t="shared" si="10"/>
+        <f>IF(B144="",IF(A144="","","; " &amp;A144),A144&amp;REPT(" ",MAX(F:F)-F144+1)&amp;B144&amp;" ? "&amp;IF(H144&lt;&gt;"","; "&amp;H144,""))</f>
         <v/>
       </c>
       <c r="J144" t="str">
@@ -5574,7 +5523,7 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B145" t="s">
         <v>114</v>
@@ -5588,28 +5537,28 @@
       </c>
       <c r="E145">
         <f>IF(B145="",E144,VLOOKUP(B145,Sheet2!A:B,2,FALSE)+E144)</f>
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F145">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="G145" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I145" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve">via_timer2_pulsecount  byte ? </v>
+        <f>IF(B145="",IF(A145="","","; " &amp;A145),A145&amp;REPT(" ",MAX(F:F)-F145+1)&amp;B145&amp;" ? "&amp;IF(H145&lt;&gt;"","; "&amp;H145,""))</f>
+        <v xml:space="preserve">via_timer1_continuous  byte ? </v>
       </c>
       <c r="J145" t="str">
         <f>IF(B145&lt;&gt;"", "        public "&amp;VLOOKUP(B145,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A145)&amp;" = "&amp;C145&amp;";"&amp;IF(H145="",""," // "&amp;H145), IF(A145&lt;&gt;"","        // "&amp;A145,""))</f>
-        <v xml:space="preserve">        public byte Via_Timer2_Pulsecount = 0;</v>
+        <v xml:space="preserve">        public byte Via_Timer1_Continuous = 0;</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B146" t="s">
         <v>114</v>
@@ -5623,55 +5572,61 @@
       </c>
       <c r="E146">
         <f>IF(B146="",E145,VLOOKUP(B146,Sheet2!A:B,2,FALSE)+E145)</f>
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F146">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f t="shared" si="5"/>
+        <v>14</v>
       </c>
       <c r="G146" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I146" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve">via_timer2_running     byte ? </v>
+        <f>IF(B146="",IF(A146="","","; " &amp;A146),A146&amp;REPT(" ",MAX(F:F)-F146+1)&amp;B146&amp;" ? "&amp;IF(H146&lt;&gt;"","; "&amp;H146,""))</f>
+        <v xml:space="preserve">via_timer1_pb7         byte ? </v>
       </c>
       <c r="J146" t="str">
         <f>IF(B146&lt;&gt;"", "        public "&amp;VLOOKUP(B146,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A146)&amp;" = "&amp;C146&amp;";"&amp;IF(H146="",""," // "&amp;H146), IF(A146&lt;&gt;"","        // "&amp;A146,""))</f>
-        <v xml:space="preserve">        public byte Via_Timer2_Running = 0;</v>
+        <v xml:space="preserve">        public byte Via_Timer1_Pb7 = 0;</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D147" t="str">
+      <c r="A147" t="s">
+        <v>103</v>
+      </c>
+      <c r="B147" t="s">
+        <v>114</v>
+      </c>
+      <c r="C147">
+        <v>0</v>
+      </c>
+      <c r="D147">
         <f>IF(B147="", "", VLOOKUP(B147,Sheet2!A:B,2,FALSE))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E147">
         <f>IF(B147="",E146,VLOOKUP(B147,Sheet2!A:B,2,FALSE)+E146)</f>
         <v>311</v>
       </c>
       <c r="F147">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>18</v>
       </c>
       <c r="G147" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I147" t="str">
-        <f t="shared" si="10"/>
-        <v/>
+        <f>IF(B147="",IF(A147="","","; " &amp;A147),A147&amp;REPT(" ",MAX(F:F)-F147+1)&amp;B147&amp;" ? "&amp;IF(H147&lt;&gt;"","; "&amp;H147,""))</f>
+        <v xml:space="preserve">via_timer1_running     byte ? </v>
       </c>
       <c r="J147" t="str">
         <f>IF(B147&lt;&gt;"", "        public "&amp;VLOOKUP(B147,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A147)&amp;" = "&amp;C147&amp;";"&amp;IF(H147="",""," // "&amp;H147), IF(A147&lt;&gt;"","        // "&amp;A147,""))</f>
-        <v/>
+        <v xml:space="preserve">        public byte Via_Timer1_Running = 0;</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>137</v>
-      </c>
       <c r="D148" t="str">
         <f>IF(B148="", "", VLOOKUP(B148,Sheet2!A:B,2,FALSE))</f>
         <v/>
@@ -5681,63 +5636,60 @@
         <v>311</v>
       </c>
       <c r="F148">
-        <f t="shared" si="8"/>
-        <v>3</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="G148" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I148" t="str">
-        <f t="shared" si="10"/>
-        <v>; L2C</v>
+        <f>IF(B148="",IF(A148="","","; " &amp;A148),A148&amp;REPT(" ",MAX(F:F)-F148+1)&amp;B148&amp;" ? "&amp;IF(H148&lt;&gt;"","; "&amp;H148,""))</f>
+        <v/>
       </c>
       <c r="J148" t="str">
         <f>IF(B148&lt;&gt;"", "        public "&amp;VLOOKUP(B148,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A148)&amp;" = "&amp;C148&amp;";"&amp;IF(H148="",""," // "&amp;H148), IF(A148&lt;&gt;"","        // "&amp;A148,""))</f>
-        <v xml:space="preserve">        // L2C</v>
+        <v/>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B149" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C149">
         <v>0</v>
       </c>
       <c r="D149">
         <f>IF(B149="", "", VLOOKUP(B149,Sheet2!A:B,2,FALSE))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E149">
         <f>IF(B149="",E148,VLOOKUP(B149,Sheet2!A:B,2,FALSE)+E148)</f>
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F149">
-        <f t="shared" si="8"/>
-        <v>11</v>
+        <f t="shared" si="5"/>
+        <v>21</v>
       </c>
       <c r="G149" t="str">
-        <f t="shared" si="9"/>
-        <v>ERROR</v>
-      </c>
-      <c r="H149" t="s">
-        <v>121</v>
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="I149" t="str">
-        <f t="shared" si="10"/>
-        <v>i2c_address            word ? ; 7 bit address of destination</v>
+        <f>IF(B149="",IF(A149="","","; " &amp;A149),A149&amp;REPT(" ",MAX(F:F)-F149+1)&amp;B149&amp;" ? "&amp;IF(H149&lt;&gt;"","; "&amp;H149,""))</f>
+        <v xml:space="preserve">via_timer2_pulsecount  byte ? </v>
       </c>
       <c r="J149" t="str">
         <f>IF(B149&lt;&gt;"", "        public "&amp;VLOOKUP(B149,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A149)&amp;" = "&amp;C149&amp;";"&amp;IF(H149="",""," // "&amp;H149), IF(A149&lt;&gt;"","        // "&amp;A149,""))</f>
-        <v xml:space="preserve">        public ushort I2C_Address = 0; // 7 bit address of destination</v>
+        <v xml:space="preserve">        public byte Via_Timer2_Pulsecount = 0;</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B150" t="s">
         <v>114</v>
@@ -5751,136 +5703,264 @@
       </c>
       <c r="E150">
         <f>IF(B150="",E149,VLOOKUP(B150,Sheet2!A:B,2,FALSE)+E149)</f>
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F150">
-        <f t="shared" si="8"/>
-        <v>9</v>
+        <f t="shared" si="5"/>
+        <v>18</v>
       </c>
       <c r="G150" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="H150" t="s">
-        <v>122</v>
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="I150" t="str">
-        <f t="shared" si="10"/>
-        <v>i2c_state              byte ? ; enum of where we are in the message</v>
+        <f>IF(B150="",IF(A150="","","; " &amp;A150),A150&amp;REPT(" ",MAX(F:F)-F150+1)&amp;B150&amp;" ? "&amp;IF(H150&lt;&gt;"","; "&amp;H150,""))</f>
+        <v xml:space="preserve">via_timer2_running     byte ? </v>
       </c>
       <c r="J150" t="str">
         <f>IF(B150&lt;&gt;"", "        public "&amp;VLOOKUP(B150,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A150)&amp;" = "&amp;C150&amp;";"&amp;IF(H150="",""," // "&amp;H150), IF(A150&lt;&gt;"","        // "&amp;A150,""))</f>
-        <v xml:space="preserve">        public byte I2C_State = 0; // enum of where we are in the message</v>
+        <v xml:space="preserve">        public byte Via_Timer2_Running = 0;</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>108</v>
-      </c>
-      <c r="B151" t="s">
-        <v>114</v>
-      </c>
-      <c r="C151">
-        <v>0</v>
-      </c>
-      <c r="D151">
+      <c r="D151" t="str">
         <f>IF(B151="", "", VLOOKUP(B151,Sheet2!A:B,2,FALSE))</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="E151">
         <f>IF(B151="",E150,VLOOKUP(B151,Sheet2!A:B,2,FALSE)+E150)</f>
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F151">
-        <f t="shared" si="8"/>
-        <v>11</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="G151" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I151" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve">i2c_sending            byte ? </v>
+        <f>IF(B151="",IF(A151="","","; " &amp;A151),A151&amp;REPT(" ",MAX(F:F)-F151+1)&amp;B151&amp;" ? "&amp;IF(H151&lt;&gt;"","; "&amp;H151,""))</f>
+        <v/>
       </c>
       <c r="J151" t="str">
         <f>IF(B151&lt;&gt;"", "        public "&amp;VLOOKUP(B151,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A151)&amp;" = "&amp;C151&amp;";"&amp;IF(H151="",""," // "&amp;H151), IF(A151&lt;&gt;"","        // "&amp;A151,""))</f>
-        <v xml:space="preserve">        public byte I2C_Sending = 0;</v>
+        <v/>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>109</v>
-      </c>
-      <c r="B152" t="s">
-        <v>114</v>
-      </c>
-      <c r="C152">
-        <v>0</v>
-      </c>
-      <c r="D152">
+        <v>137</v>
+      </c>
+      <c r="D152" t="str">
         <f>IF(B152="", "", VLOOKUP(B152,Sheet2!A:B,2,FALSE))</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="E152">
         <f>IF(B152="",E151,VLOOKUP(B152,Sheet2!A:B,2,FALSE)+E151)</f>
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F152">
-        <f t="shared" si="8"/>
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="G152" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="H152" t="s">
-        <v>123</v>
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="I152" t="str">
-        <f t="shared" si="10"/>
-        <v>i2c_data               byte ? ; data that is being transmitted</v>
+        <f>IF(B152="",IF(A152="","","; " &amp;A152),A152&amp;REPT(" ",MAX(F:F)-F152+1)&amp;B152&amp;" ? "&amp;IF(H152&lt;&gt;"","; "&amp;H152,""))</f>
+        <v>; L2C</v>
       </c>
       <c r="J152" t="str">
         <f>IF(B152&lt;&gt;"", "        public "&amp;VLOOKUP(B152,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A152)&amp;" = "&amp;C152&amp;";"&amp;IF(H152="",""," // "&amp;H152), IF(A152&lt;&gt;"","        // "&amp;A152,""))</f>
-        <v xml:space="preserve">        public byte I2C_Data = 0; // data that is being transmitted</v>
+        <v xml:space="preserve">        // L2C</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B153" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C153">
         <v>0</v>
       </c>
       <c r="D153">
         <f>IF(B153="", "", VLOOKUP(B153,Sheet2!A:B,2,FALSE))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E153">
         <f>IF(B153="",E152,VLOOKUP(B153,Sheet2!A:B,2,FALSE)+E152)</f>
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F153">
-        <f t="shared" si="8"/>
-        <v>7</v>
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
       <c r="G153" t="str">
-        <f t="shared" si="9"/>
-        <v/>
+        <f t="shared" si="6"/>
+        <v>ERROR</v>
       </c>
       <c r="H153" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I153" t="str">
-        <f t="shared" si="10"/>
-        <v>i2c_pos                byte ? ; position in that data</v>
+        <f>IF(B153="",IF(A153="","","; " &amp;A153),A153&amp;REPT(" ",MAX(F:F)-F153+1)&amp;B153&amp;" ? "&amp;IF(H153&lt;&gt;"","; "&amp;H153,""))</f>
+        <v>i2c_address            word ? ; 7 bit address of destination</v>
       </c>
       <c r="J153" t="str">
         <f>IF(B153&lt;&gt;"", "        public "&amp;VLOOKUP(B153,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A153)&amp;" = "&amp;C153&amp;";"&amp;IF(H153="",""," // "&amp;H153), IF(A153&lt;&gt;"","        // "&amp;A153,""))</f>
+        <v xml:space="preserve">        public ushort I2C_Address = 0; // 7 bit address of destination</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>107</v>
+      </c>
+      <c r="B154" t="s">
+        <v>114</v>
+      </c>
+      <c r="C154">
+        <v>0</v>
+      </c>
+      <c r="D154">
+        <f>IF(B154="", "", VLOOKUP(B154,Sheet2!A:B,2,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="E154">
+        <f>IF(B154="",E153,VLOOKUP(B154,Sheet2!A:B,2,FALSE)+E153)</f>
+        <v>316</v>
+      </c>
+      <c r="F154">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="G154" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H154" t="s">
+        <v>122</v>
+      </c>
+      <c r="I154" t="str">
+        <f>IF(B154="",IF(A154="","","; " &amp;A154),A154&amp;REPT(" ",MAX(F:F)-F154+1)&amp;B154&amp;" ? "&amp;IF(H154&lt;&gt;"","; "&amp;H154,""))</f>
+        <v>i2c_state              byte ? ; enum of where we are in the message</v>
+      </c>
+      <c r="J154" t="str">
+        <f>IF(B154&lt;&gt;"", "        public "&amp;VLOOKUP(B154,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A154)&amp;" = "&amp;C154&amp;";"&amp;IF(H154="",""," // "&amp;H154), IF(A154&lt;&gt;"","        // "&amp;A154,""))</f>
+        <v xml:space="preserve">        public byte I2C_State = 0; // enum of where we are in the message</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>108</v>
+      </c>
+      <c r="B155" t="s">
+        <v>114</v>
+      </c>
+      <c r="C155">
+        <v>0</v>
+      </c>
+      <c r="D155">
+        <f>IF(B155="", "", VLOOKUP(B155,Sheet2!A:B,2,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="E155">
+        <f>IF(B155="",E154,VLOOKUP(B155,Sheet2!A:B,2,FALSE)+E154)</f>
+        <v>317</v>
+      </c>
+      <c r="F155">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="G155" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I155" t="str">
+        <f>IF(B155="",IF(A155="","","; " &amp;A155),A155&amp;REPT(" ",MAX(F:F)-F155+1)&amp;B155&amp;" ? "&amp;IF(H155&lt;&gt;"","; "&amp;H155,""))</f>
+        <v xml:space="preserve">i2c_sending            byte ? </v>
+      </c>
+      <c r="J155" t="str">
+        <f>IF(B155&lt;&gt;"", "        public "&amp;VLOOKUP(B155,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A155)&amp;" = "&amp;C155&amp;";"&amp;IF(H155="",""," // "&amp;H155), IF(A155&lt;&gt;"","        // "&amp;A155,""))</f>
+        <v xml:space="preserve">        public byte I2C_Sending = 0;</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>109</v>
+      </c>
+      <c r="B156" t="s">
+        <v>114</v>
+      </c>
+      <c r="C156">
+        <v>0</v>
+      </c>
+      <c r="D156">
+        <f>IF(B156="", "", VLOOKUP(B156,Sheet2!A:B,2,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="E156">
+        <f>IF(B156="",E155,VLOOKUP(B156,Sheet2!A:B,2,FALSE)+E155)</f>
+        <v>318</v>
+      </c>
+      <c r="F156">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="G156" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H156" t="s">
+        <v>123</v>
+      </c>
+      <c r="I156" t="str">
+        <f>IF(B156="",IF(A156="","","; " &amp;A156),A156&amp;REPT(" ",MAX(F:F)-F156+1)&amp;B156&amp;" ? "&amp;IF(H156&lt;&gt;"","; "&amp;H156,""))</f>
+        <v>i2c_data               byte ? ; data that is being transmitted</v>
+      </c>
+      <c r="J156" t="str">
+        <f>IF(B156&lt;&gt;"", "        public "&amp;VLOOKUP(B156,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A156)&amp;" = "&amp;C156&amp;";"&amp;IF(H156="",""," // "&amp;H156), IF(A156&lt;&gt;"","        // "&amp;A156,""))</f>
+        <v xml:space="preserve">        public byte I2C_Data = 0; // data that is being transmitted</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>110</v>
+      </c>
+      <c r="B157" t="s">
+        <v>114</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+      <c r="D157">
+        <f>IF(B157="", "", VLOOKUP(B157,Sheet2!A:B,2,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="E157">
+        <f>IF(B157="",E156,VLOOKUP(B157,Sheet2!A:B,2,FALSE)+E156)</f>
+        <v>319</v>
+      </c>
+      <c r="F157">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="G157" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H157" t="s">
+        <v>124</v>
+      </c>
+      <c r="I157" t="str">
+        <f>IF(B157="",IF(A157="","","; " &amp;A157),A157&amp;REPT(" ",MAX(F:F)-F157+1)&amp;B157&amp;" ? "&amp;IF(H157&lt;&gt;"","; "&amp;H157,""))</f>
+        <v>i2c_pos                byte ? ; position in that data</v>
+      </c>
+      <c r="J157" t="str">
+        <f>IF(B157&lt;&gt;"", "        public "&amp;VLOOKUP(B157,Sheet2!A:C,3,FALSE)&amp;" "&amp;PROPER(A157)&amp;" = "&amp;C157&amp;";"&amp;IF(H157="",""," // "&amp;H157), IF(A157&lt;&gt;"","        // "&amp;A157,""))</f>
         <v xml:space="preserve">        public byte I2C_Pos = 0; // position in that data</v>
       </c>
     </row>

</xml_diff>